<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@434575140893d5dbb0b476a478f1a023bd112399 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -642,7 +642,7 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>The operating system must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
+          <t>Red Hat Enterprise Linux 9 must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
@@ -695,7 +695,15 @@
         </is>
       </c>
       <c r="L3" s="2" t="n"/>
-      <c r="M3" s="2" t="inlineStr"/>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to use TCP syncookies.
+Add or edit the following line in a system configuration file in the "/etc/sysctl.d/" directory:
+ net.ipv4.tcp_syncookies = 1
+ Load settings from all system configuration files with the following command:
+ $ sudo sysctl --system</t>
+        </is>
+      </c>
       <c r="N3" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -3945,7 +3953,7 @@
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
+          <t>Red Hat Enterprise Linux 9must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
         </is>
       </c>
       <c r="G50" s="2" t="inlineStr">
@@ -4999,7 +5007,7 @@
       </c>
       <c r="F65" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for network access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for network access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G65" s="2" t="inlineStr">
@@ -6042,7 +6050,7 @@
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for local access to privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for local access to privileged accounts.</t>
         </is>
       </c>
       <c r="G80" s="2" t="inlineStr">
@@ -6088,7 +6096,14 @@
         </is>
       </c>
       <c r="L80" s="2" t="n"/>
-      <c r="M80" s="2" t="inlineStr"/>
+      <c r="M80" s="2" t="inlineStr">
+        <is>
+          <t>To configure the system add or modify the following line in "/etc/ssh/sshd_config".
+PubkeyAuthentication yes
+Restart the SSH daemon for the settings to take effect:
+$ sudo systemctl restart sshd.service</t>
+        </is>
+      </c>
       <c r="N80" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -9410,7 +9425,7 @@
       </c>
       <c r="F129" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for local access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for local access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G129" s="2" t="inlineStr">
@@ -10979,7 +10994,7 @@
       </c>
       <c r="F151" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for network access to privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for network access to privileged accounts.</t>
         </is>
       </c>
       <c r="G151" s="2" t="inlineStr">
@@ -12813,7 +12828,7 @@
       </c>
       <c r="F181" s="2" t="inlineStr">
         <is>
-          <t>The operating system must isolate security functions from nonsecurity functions.</t>
+          <t>Red Hat Enterprise Linux 9 must isolate security functions from nonsecurity functions.</t>
         </is>
       </c>
       <c r="G181" s="2" t="inlineStr">
@@ -12857,7 +12872,16 @@
         </is>
       </c>
       <c r="L181" s="2" t="n"/>
-      <c r="M181" s="2" t="inlineStr"/>
+      <c r="M181" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To ensure that "vsyscall=none" is added as a kernel command line
+argument to newly installed kernels, add "vsyscall=none" to the
+default Grub2 command line for Linux operating systems.  Modify the line within
+"/etc/default/grub" as shown below:
+ GRUB_CMDLINE_LINUX="... vsyscall=none ..." 
+Run the following command to update command line for already installed kernels: # grubby --update-kernel=ALL --args="vsyscall=none" </t>
+        </is>
+      </c>
       <c r="N181" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@53aed0d04952cc5f33f6c0970b48f9ffc7c3d198 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4, AU-4 (1)</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, SC-5, SC-5 (2)</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8), AC-6 (9), AU-12 (3), AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 b, AU-7 b, AU-8 b, AU-8 b, CM-5 (1)</t>
+          <t>AU-7 a,CM-5 (1),AU-7 b,AU-12 (3),AC-6 (9),AU-8 b,AC-6 (8)</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b, AC-17 (1), AC-17 (9), CM-6 b, CM-6 b</t>
+          <t>AC-17 (9),CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11), IA-2 (12)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1155,7 +1155,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b), CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1307,7 +1307,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b, AC-7 a</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-2, IA-8, AU-3 (1)</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1596,7 +1596,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10), CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b), IA-5 (1) (a), IA-5 (1) (a), IA-5 (1) (a), IA-5 (1) (a), CM-6 b, IA-5 (1) (a)</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e, SC-10, AC-12, MA-4 (7)</t>
+          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3, AU-3, AU-3, AU-3, AU-3 (1), AU-6 (4), AU-7 (1), AU-7 a, AU-14 (1), AU-3, CM-5 (1), MA-4 (1) (a), CM-6 b, AU-12 a, AU-7 a</t>
+          <t>MA-4 (1) (a),AU-7 a,CM-5 (1),AU-12 a,AU-7 (1),AU-6 (4),AU-3,CM-6 b,AU-14 (1),AU-3 (1)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8, SC-8 (1), SC-8 (2), SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AU-3, AU-3 (1), AU-12 a, AC-2 (4), MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2838,7 +2838,7 @@
     <row r="34" ht="130" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a, AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -3110,7 +3110,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9, SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3178,7 +3178,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3, CM-6 b</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3305,7 +3305,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1), AU-4 (1)</t>
+          <t>AU-4 (1)</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3377,7 +3377,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1), SC-28, SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -3439,7 +3439,13 @@
         </is>
       </c>
       <c r="L42" s="2" t="n"/>
-      <c r="M42" s="2" t="inlineStr"/>
+      <c r="M42" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to prevent unauthorized modification of all information at rest by using disk encryption.
+Encrypting a partition in an already installed system is more difficult, because existing partitions will need to be resized and changed.
+To encrypt an entire partition, dedicate a partition for encryption in the partition layout.</t>
+        </is>
+      </c>
       <c r="N42" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -3523,7 +3529,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>IA-11, IA-11, IA-11</t>
+          <t>IA-11</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3593,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a, AC-8 b, AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3804,7 +3810,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, CM-6 b</t>
+          <t>CM-6 b</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -3932,7 +3938,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5), CM-6 b</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4140,7 +4146,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>SC-13, MA-4 (6), MA-4 (6)</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4277,7 +4283,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2), SC-8</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4348,7 +4354,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a), AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4835,7 +4841,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a, AU-5 (1)</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -4986,7 +4992,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2), CM-6 b, CM-6 b</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5126,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5252,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a, AU-12 (3), AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 b, AU-7 b, AU-8 b, AU-8 b, CM-5 (1), AU-12 c, AU-12 c, CM-6 b, AU-12 a</t>
+          <t>CM-5 (1),AU-7 a,AU-12 c,AU-12 (3),AU-7 b,AU-12 a,AU-8 b,CM-6 b</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5402,7 +5408,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-4 (1), AU-4 (1)</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5793,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AU-3, AU-3 (1), AU-12 a, AC-2 (4), MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -5958,7 +5964,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9, AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6029,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1), IA-2 (2), IA-2 (3), IA-2 (4)</t>
+          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6116,7 +6122,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6449,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6595,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AC-6 (9), AU-12 c, CM-5 (1), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AC-2 (4),AC-6 (9),CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6662,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2, IA-2 (2), IA-2 (3), IA-2 (5), IA-2 (4)</t>
+          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6742,7 +6748,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11), IA-2 (12)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -6818,7 +6824,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7192,7 +7198,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1), AC-18 (1), SC-8 (1), SC-8</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7268,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a), AU-8 (1) (b), AU-8 b</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7416,7 +7422,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9</t>
+          <t>AU-9</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -7505,7 +7511,7 @@
       </c>
       <c r="F100" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow the use of a temporary password for system logons with an immediate change to a permanent password.</t>
+          <t>Red Hat Enterprise Linux 9 must allow the use of a temporary password for system logons with an immediate change to a permanent password.</t>
         </is>
       </c>
       <c r="G100" s="2" t="inlineStr">
@@ -7514,10 +7520,17 @@
 Temporary passwords are typically used to allow access when new accounts are created or passwords are changed. It is common practice for administrators to create temporary passwords for user accounts which allow the users to log on, yet force them to change the password once they have successfully authenticated.</t>
         </is>
       </c>
-      <c r="H100" s="2" t="inlineStr"/>
+      <c r="H100" s="2" t="inlineStr">
+        <is>
+          <t>Without providing this capability, an account may be created without a password.
+Non-repudiation cannot be guaranteed once an account is created if a user is not forced to change the temporary password upon initial logon.
+Temporary passwords are typically used to allow access when new accounts are created or passwords are changed.
+It is common practice for administrators to create temporary passwords for user accounts that allow the users to log on, yet force them to change the password once they have successfully authenticated.</t>
+        </is>
+      </c>
       <c r="I100" s="2" t="inlineStr">
         <is>
-          <t>Applicable - Configurable</t>
+          <t>Applicable - Inherently Met</t>
         </is>
       </c>
       <c r="J100" s="2" t="inlineStr">
@@ -7525,7 +7538,12 @@
           <t>Verify the operating system allows the use of a temporary password for system logons with an immediate change to a permanent password. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K100" s="2" t="n"/>
+      <c r="K100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 supports this requirement and cannot be configured to be out of compliance.
+Red Hat Enterprise Linux 9 inherently meets this requirement.</t>
+        </is>
+      </c>
       <c r="L100" s="2" t="n"/>
       <c r="M100" s="2" t="n"/>
       <c r="N100" s="2" t="inlineStr">
@@ -7534,13 +7552,26 @@
         </is>
       </c>
       <c r="O100" s="2" t="n"/>
-      <c r="P100" s="2" t="n"/>
-      <c r="Q100" s="2" t="n"/>
+      <c r="P100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 offers the following commands to facilitate the use of a temporary password.
+chage -d 0 [username]
+(forces the user to change their password at next logon)
+passwd -e [username]
+(expires the passwd for a given user forcing a change at next logon.)</t>
+        </is>
+      </c>
+      <c r="Q100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 has the capability to perform temporary passwords based on organization policy.
+Configuration is not appropriate to define at an enterprise level.</t>
+        </is>
+      </c>
     </row>
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>IA-11, AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -7610,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -7701,7 +7732,7 @@
       </c>
       <c r="F103" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement replay-resistant authentication mechanisms for network access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 system must implement replay-resistant authentication mechanisms for network access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G103" s="2" t="inlineStr">
@@ -7715,7 +7746,7 @@
       <c r="H103" s="2" t="inlineStr"/>
       <c r="I103" s="2" t="inlineStr">
         <is>
-          <t>Applicable - Configurable</t>
+          <t>Applicable - Inherently Met</t>
         </is>
       </c>
       <c r="J103" s="2" t="inlineStr">
@@ -7723,17 +7754,36 @@
           <t>Verify the operating system implements replay-resistant authentication mechanisms for network access to non-privileged accounts. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K103" s="2" t="n"/>
+      <c r="K103" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 supports this requirement and cannot be configured to be out of compliance.
+Red Hat Enterprise Linux 9 inherently meets this requirement.</t>
+        </is>
+      </c>
       <c r="L103" s="2" t="n"/>
-      <c r="M103" s="2" t="n"/>
+      <c r="M103" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 inherently meets this requirement.
+No fix is required.</t>
+        </is>
+      </c>
       <c r="N103" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
         </is>
       </c>
       <c r="O103" s="2" t="n"/>
-      <c r="P103" s="2" t="n"/>
-      <c r="Q103" s="2" t="n"/>
+      <c r="P103" s="2" t="inlineStr">
+        <is>
+          <t>The release notes of OpenSSH 7.6 states "OpenSSH is a 100% complete SSH protocol 2.0 implementation and includes sftp client and server support."
+https://www.openssh.com/txt/release-7.6</t>
+        </is>
+      </c>
+      <c r="Q103" s="2" t="inlineStr">
+        <is>
+          <t>The OpenSSH package in Red Hat Enterprise Linux 9 is version 8.7, which is newer than 7.6 which only supports SSH protocol 2.0 which is restraint to replay attacks.</t>
+        </is>
+      </c>
     </row>
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
@@ -8177,7 +8227,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a, AU-5 b</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -8719,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9009,7 +9059,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b, CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9079,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9149,7 +9199,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a, AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9334,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c), CM-7 a, CM-6 b</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9896,7 +9946,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1), AC-11 b</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10117,7 +10167,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5), SI-6 b, SI-6 d</t>
+          <t>CM-3 (5),SI-6 d,SI-6 b</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10310,7 +10360,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (2), AC-2 (2)</t>
+          <t>AC-2 (2)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -10759,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-14 (1)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-14 (1),AU-3 (1)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11320,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11452,7 +11502,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>SC-8, AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -12435,7 +12485,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>SI-16, CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -12807,7 +12857,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -13629,7 +13679,7 @@
       </c>
       <c r="F192" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect the confidentiality and integrity of all information at rest.</t>
+          <t>Red Hat Enterprise Linux 9 must protect the confidentiality and integrity of all information at rest.</t>
         </is>
       </c>
       <c r="G192" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@2d18ba5a9ff660e66d0609c1fa719a520c5729ac 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),CM-6 b,SC-5</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-5 (1),AU-7 b,AU-12 (3),AC-6 (9),AU-8 b,AC-6 (8)</t>
+          <t>AC-6 (8),AC-6 (9),AU-12 (3),AU-7 a,AU-7 b,CM-5 (1),AU-8 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>CM-7 b,CM-6 b,AC-17 (9),AC-17 (1)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
+          <t>AC-12,MA-4 (7),MA-4 e,SC-10</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-7 a,CM-5 (1),AU-12 a,AU-7 (1),AU-6 (4),AU-3,CM-6 b,AU-14 (1),AU-3 (1)</t>
+          <t>AU-7 (1),AU-14 (1),AU-12 a,AU-6 (4),AU-3,AU-7 a,AU-3 (1),CM-5 (1),MA-4 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -3110,7 +3110,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3178,7 +3178,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3599,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 b</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a,AC-8 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4283,7 +4283,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4841,7 +4841,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -4992,7 +4992,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5132,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5258,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-7 a,AU-12 c,AU-12 (3),AU-7 b,AU-12 a,AU-8 b,CM-6 b</t>
+          <t>AU-12 c,AU-12 a,AU-7 a,AU-12 (3),AU-7 b,CM-5 (1),AU-8 b,CM-6 b</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5408,7 +5408,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5799,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -5964,7 +5964,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6035,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6455,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6601,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),CM-5 (1),AU-12 c</t>
+          <t>AC-2 (4),AC-6 (9),AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6668,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (4),IA-2,IA-2 (2)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6824,7 +6824,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7198,7 +7198,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7274,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7571,7 +7571,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -7641,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8227,7 +8227,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -8769,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9059,7 +9059,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9384,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10167,7 +10167,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d,SI-6 b</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10809,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-14 (1),AU-3 (1)</t>
+          <t>AU-12 c,AU-14 (1),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11370,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11502,7 +11502,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -12485,7 +12485,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@b4ede572458fc0a3e3ca8f984e777ee7c2bf2ef6 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8),AC-6 (9),AU-12 (3),AU-7 a,AU-7 b,CM-5 (1),AU-8 b</t>
+          <t>AU-12 (3),AU-7 b,AC-6 (8),AU-7 a,CM-5 (1),AC-6 (9),AU-8 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (9),AC-17 (1)</t>
+          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-2,IA-8,AU-3 (1)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 (7),MA-4 e,SC-10</t>
+          <t>AC-12,MA-4 (7),SC-10,MA-4 e</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-7 (1),AU-14 (1),AU-12 a,AU-6 (4),AU-3,AU-7 a,AU-3 (1),CM-5 (1),MA-4 (1) (a),CM-6 b</t>
+          <t>CM-6 b,AU-12 a,AU-7 a,CM-5 (1),AU-3,MA-4 (1) (a),AU-3 (1),AU-14 (1),AU-7 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2838,7 +2838,7 @@
     <row r="34" ht="130" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -3599,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a,AC-8 b</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 b,AC-8 a</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4283,7 +4283,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4992,7 +4992,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5132,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5258,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-7 a,AU-12 (3),AU-7 b,CM-5 (1),AU-8 b,CM-6 b</t>
+          <t>AU-12 (3),CM-6 b,AU-7 b,AU-12 a,AU-7 a,CM-5 (1),AU-12 c,AU-8 b</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5799,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6035,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (2),IA-2 (1),IA-2 (3),IA-2 (4)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6455,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6601,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c,CM-5 (1)</t>
+          <t>AC-6 (9),AC-2 (4),AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6668,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (4),IA-2,IA-2 (2)</t>
+          <t>IA-2,IA-2 (5),IA-2 (2),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6748,7 +6748,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7274,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7641,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8227,7 +8227,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -8769,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9199,7 +9199,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9384,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9946,7 +9946,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10167,7 +10167,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>CM-3 (5),SI-6 b,SI-6 d</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10809,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-14 (1),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c,AU-14 (1)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11370,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11502,7 +11502,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@75bb2908a7ea008345937532ce505a73de90940f 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),CM-6 b,SC-5</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-7 b,AC-6 (8),AU-7 a,CM-5 (1),AC-6 (9),AU-8 b</t>
+          <t>AU-7 a,AC-6 (9),AU-7 b,AU-12 (3),AU-8 b,AC-6 (8),CM-5 (1)</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-7 b,CM-6 b,AC-17 (9),AC-17 (1)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1155,7 +1155,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-8,AU-3 (1)</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 (7),SC-10,MA-4 e</t>
+          <t>AC-12,SC-10,MA-4 e,MA-4 (7)</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a,AU-7 a,CM-5 (1),AU-3,MA-4 (1) (a),AU-3 (1),AU-14 (1),AU-7 (1),AU-6 (4)</t>
+          <t>AU-7 a,AU-12 a,CM-6 b,AU-7 (1),AU-3 (1),AU-6 (4),MA-4 (1) (a),CM-5 (1),AU-14 (1),AU-3</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2838,7 +2838,7 @@
     <row r="34" ht="130" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -3377,7 +3377,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -3599,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 b,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4354,7 +4354,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4841,7 +4841,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5132,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5258,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),CM-6 b,AU-7 b,AU-12 a,AU-7 a,CM-5 (1),AU-12 c,AU-8 b</t>
+          <t>AU-7 a,AU-12 c,AU-12 a,CM-6 b,AU-7 b,AU-12 (3),AU-8 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5799,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6035,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (1),IA-2 (3),IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (1),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6122,7 +6122,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6455,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6601,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c,CM-5 (1)</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4),CM-5 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6668,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (5),IA-2 (2),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2,IA-2 (5),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7274,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7641,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8227,7 +8227,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -8769,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9199,7 +9199,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9384,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10809,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c,AU-14 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-3</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11370,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12857,7 +12857,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@fe68fcd788b85eed7559e6174d71a676223ab02b 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AC-6 (9),AU-7 b,AU-12 (3),AU-8 b,AC-6 (8),CM-5 (1)</t>
+          <t>AU-8 b,AU-12 (3),AU-7 b,AU-7 a,AC-6 (9),AC-6 (8),CM-5 (1)</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1155,7 +1155,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1596,7 +1596,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10,MA-4 e,MA-4 (7)</t>
+          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-12 a,CM-6 b,AU-7 (1),AU-3 (1),AU-6 (4),MA-4 (1) (a),CM-5 (1),AU-14 (1),AU-3</t>
+          <t>MA-4 (1) (a),AU-7 (1),AU-7 a,AU-12 a,AU-3,AU-3 (1),AU-6 (4),AU-14 (1),CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AC-2 (4),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -3599,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 b</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a,AC-8 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4283,7 +4283,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4354,7 +4354,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4992,7 +4992,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5132,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5258,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-12 c,AU-12 a,CM-6 b,AU-7 b,AU-12 (3),AU-8 b,CM-5 (1)</t>
+          <t>AU-8 b,AU-12 (3),AU-7 b,AU-7 a,AU-12 a,CM-6 b,AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5799,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AC-2 (4),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6035,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (1),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6122,7 +6122,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6455,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6601,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-6 (9),AC-2 (4),CM-5 (1)</t>
+          <t>AC-2 (4),CM-5 (1),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6668,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2,IA-2 (5),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (5),IA-2 (4),IA-2 (2),IA-2 (3),IA-2</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6748,7 +6748,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7274,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7571,7 +7571,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -7641,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8769,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9059,7 +9059,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9199,7 +9199,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9384,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9946,7 +9946,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10167,7 +10167,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 b,SI-6 d</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10809,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-14 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11370,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11502,7 +11502,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@30e59c20ece2702b3bff665dc0cb4d5919a46eec 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -554,7 +554,11 @@
           <t>SRG-OS-000341-GPOS-00132,SRG-OS-000342-GPOS-00133</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr"/>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88173-0</t>
+        </is>
+      </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
           <t>The operating system must allocate audit record storage capacity to store at least one weeks worth of audit records, when audit records are not immediately sent to a central audit record storage facility.</t>
@@ -562,7 +566,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allocate audit record storage capacity to store at least one weeks worth of audit records, when audit records are not immediately sent to a central audit record storage facility.</t>
+          <t>Red Hat Enterprise Linux 9 must allocate audit record storage capacity to store at least one weeks worth of audit records, when audit records are not immediately sent to a central audit record storage facility.</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
@@ -621,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -634,7 +638,11 @@
           <t>SRG-OS-000480-GPOS-00227,SRG-OS-000420-GPOS-00186,SRG-OS-000142-GPOS-00071</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr"/>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84006-6</t>
+        </is>
+      </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
           <t>The operating system must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
@@ -716,7 +724,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-12 (3),AU-7 b,AU-7 a,AC-6 (9),AC-6 (8),CM-5 (1)</t>
+          <t>AU-7 b,AU-7 a,AC-6 (8),CM-5 (1),AU-12 (3),AC-6 (9),AU-8 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -729,7 +737,11 @@
           <t>SRG-OS-000326-GPOS-00126,SRG-OS-000327-GPOS-00127,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000359-GPOS-00146,SRG-OS-000365-GPOS-00152</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr"/>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86402-5</t>
+        </is>
+      </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide a report generation capability that supports on-demand audit review and analysis.</t>
@@ -737,7 +749,7 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide a report generation capability that supports on-demand audit review and analysis.</t>
+          <t>Red Hat Enterprise Linux 9 must provide a report generation capability that supports on-demand audit review and analysis.</t>
         </is>
       </c>
       <c r="G4" s="2" t="inlineStr">
@@ -792,7 +804,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (9),AC-17 (1)</t>
+          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -805,7 +817,11 @@
           <t>SRG-OS-000096-GPOS-00050,SRG-OS-000297-GPOS-00115,SRG-OS-000298-GPOS-00116,SRG-OS-000480-GPOS-00227,SRG-OS-000480-GPOS-00232</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr"/>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84021-5</t>
+        </is>
+      </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability to immediately disconnect or disable remote access to the operating system.</t>
@@ -813,7 +829,7 @@
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide the capability to immediately disconnect or disable remote access to the operating system.</t>
+          <t>Red Hat Enterprise Linux 9 must provide the capability to immediately disconnect or disable remote access to the operating system.</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
@@ -973,7 +989,7 @@
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require devices to re-authenticate when changing authenticators.</t>
+          <t>Red Hat Enterprise Linux 9 must require devices to re-authenticate when changing authenticators.</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr">
@@ -1021,7 +1037,11 @@
           <t>SRG-OS-000375-GPOS-00160,SRG-OS-000376-GPOS-00161</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr"/>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83595-9</t>
+        </is>
+      </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
           <t>The operating system must accept Personal Identity Verification (PIV) credentials.</t>
@@ -1029,7 +1049,7 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>The operating system must accept Personal Identity Verification (PIV) credentials.</t>
+          <t>Red Hat Enterprise Linux 9 must accept Personal Identity Verification (PIV) credentials.</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
@@ -1155,7 +1175,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1168,7 +1188,11 @@
           <t>SRG-OS-000370-GPOS-00155,SRG-OS-000368-GPOS-00154</t>
         </is>
       </c>
-      <c r="D10" s="2" t="inlineStr"/>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84224-5</t>
+        </is>
+      </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent program execution in accordance with local policies regarding software program usage and restrictions and/or rules authorizing the terms and conditions of software program usage.</t>
@@ -1176,7 +1200,7 @@
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent program execution in accordance with local policies regarding software program usage and restrictions and/or rules authorizing the terms and conditions of software program usage.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent program execution in accordance with local policies regarding software program usage and restrictions and/or rules authorizing the terms and conditions of software program usage.</t>
         </is>
       </c>
       <c r="G10" s="2" t="inlineStr">
@@ -1240,7 +1264,11 @@
           <t>SRG-OS-000118-GPOS-00060</t>
         </is>
       </c>
-      <c r="D11" s="2" t="inlineStr"/>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83627-0</t>
+        </is>
+      </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
           <t>The operating system must disable account identifiers (individuals, groups, roles, and devices) after 35 days of inactivity.</t>
@@ -1320,7 +1348,11 @@
           <t>SRG-OS-000329-GPOS-00128,SRG-OS-000021-GPOS-00005</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr"/>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83587-6</t>
+        </is>
+      </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce the limit of three consecutive invalid logon attempts by a user during a 15-minute time period.</t>
@@ -1328,7 +1360,7 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce the limit of three consecutive invalid logon attempts by a user during a 15-minute time period.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce the limit of three consecutive invalid logon attempts by a user during a 15-minute time period.</t>
         </is>
       </c>
       <c r="G12" s="2" t="inlineStr">
@@ -1400,7 +1432,11 @@
           <t>SRG-OS-000076-GPOS-00044</t>
         </is>
       </c>
-      <c r="D13" s="2" t="inlineStr"/>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83606-4</t>
+        </is>
+      </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
           <t>Operating systems must enforce a 60-day maximum password lifetime restriction.</t>
@@ -1487,7 +1523,7 @@
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow operating system admins to pass information to any other operating system admin or user.</t>
+          <t>Red Hat Enterprise Linux 9 must allow operating system admins to pass information to any other operating system admin or user.</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr">
@@ -1522,7 +1558,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>IA-2,IA-8,AU-3 (1)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1535,7 +1571,11 @@
           <t>SRG-OS-000104-GPOS-00051,SRG-OS-000121-GPOS-00062,SRG-OS-000042-GPOS-00020</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr"/>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88493-2</t>
+        </is>
+      </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records containing the full-text recording of privileged commands.</t>
@@ -1543,7 +1583,7 @@
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records containing the full-text recording of privileged commands.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records containing the full-text recording of privileged commands.</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
@@ -1596,7 +1636,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1609,7 +1649,11 @@
           <t>SRG-OS-000324-GPOS-00125,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr"/>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90308-8</t>
+        </is>
+      </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.</t>
@@ -1617,7 +1661,7 @@
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.</t>
         </is>
       </c>
       <c r="G16" s="2" t="inlineStr">
@@ -1668,7 +1712,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1681,7 +1725,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000064-GPOS-00033,SRG-OS-000466-GPOS-00210,SRG-OS-000458-GPOS-00203</t>
         </is>
       </c>
-      <c r="D17" s="2" t="inlineStr"/>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83830-0</t>
+        </is>
+      </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to modify privileges occur.</t>
@@ -1689,7 +1737,7 @@
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to modify privileges occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to modify privileges occur.</t>
         </is>
       </c>
       <c r="G17" s="2" t="inlineStr">
@@ -1760,7 +1808,7 @@
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>In the event of a system failure, the operating system must preserve any information necessary to determine cause of failure and any information necessary to return to operations with least disruption to mission processes.</t>
+          <t>In the event of a system failure, Red Hat Enterprise Linux 9 must preserve any information necessary to determine cause of failure and any information necessary to return to operations with least disruption to mission processes.</t>
         </is>
       </c>
       <c r="G18" s="2" t="inlineStr">
@@ -1795,7 +1843,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1808,7 +1856,11 @@
           <t>SRG-OS-000072-GPOS-00040,SRG-OS-000071-GPOS-00039,SRG-OS-000070-GPOS-00038,SRG-OS-000266-GPOS-00101,SRG-OS-000078-GPOS-00046,SRG-OS-000480-GPOS-00225,SRG-OS-000069-GPOS-00037</t>
         </is>
       </c>
-      <c r="D19" s="2" t="inlineStr"/>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86356-3</t>
+        </is>
+      </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce password complexity by requiring that at least one lower-case character be used.</t>
@@ -1886,7 +1938,11 @@
           <t>SRG-OS-000478-GPOS-00223</t>
         </is>
       </c>
-      <c r="D20" s="2" t="inlineStr"/>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86547-7</t>
+        </is>
+      </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement NIST FIPS-validated cryptography for the following: to provision digital signatures, to generate cryptographic hashes, and to protect unclassified information requiring confidentiality and cryptographic protection in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
@@ -1894,7 +1950,7 @@
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement NIST FIPS-validated cryptography for the following: to provision digital signatures, to generate cryptographic hashes, and to protect unclassified information requiring confidentiality and cryptographic protection in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
+          <t>Red Hat Enterprise Linux 9 must implement NIST FIPS-validated cryptography for the following: to provision digital signatures, to generate cryptographic hashes, and to protect unclassified information requiring confidentiality and cryptographic protection in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
         </is>
       </c>
       <c r="G20" s="2" t="inlineStr">
@@ -1943,7 +1999,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
+          <t>AC-12,MA-4 e,SC-10,MA-4 (7)</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -1956,7 +2012,11 @@
           <t>SRG-OS-000126-GPOS-00066,SRG-OS-000163-GPOS-00072,SRG-OS-000279-GPOS-00109,SRG-OS-000395-GPOS-00175</t>
         </is>
       </c>
-      <c r="D21" s="2" t="inlineStr"/>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90811-1</t>
+        </is>
+      </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
           <t>The operating system must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inactivity; and for user sessions (non-privileged session), the session must be terminated after 15 minutes of inactivity, except to fulfill documented and validated mission requirements.</t>
@@ -1964,7 +2024,7 @@
       </c>
       <c r="F21" s="2" t="inlineStr">
         <is>
-          <t>The operating system must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inacti</t>
+          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inacti</t>
         </is>
       </c>
       <c r="G21" s="2" t="inlineStr">
@@ -2014,7 +2074,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-7 (1),AU-7 a,AU-12 a,AU-3,AU-3 (1),AU-6 (4),AU-14 (1),CM-6 b,CM-5 (1)</t>
+          <t>AU-7 a,AU-12 a,CM-5 (1),AU-7 (1),CM-6 b,AU-3,AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2027,7 +2087,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000038-GPOS-00016,SRG-OS-000039-GPOS-00017,SRG-OS-000040-GPOS-00018,SRG-OS-000041-GPOS-00019,SRG-OS-000042-GPOS-00021,SRG-OS-000051-GPOS-00024,SRG-OS-000054-GPOS-00025,SRG-OS-000122-GPOS-00063,SRG-OS-000254-GPOS-00095,SRG-OS-000255-GPOS-00096,SRG-OS-000365-GPOS-00152,SRG-OS-000392-GPOS-00172,SRG-OS-000480-GPOS-00227,SRG-OS-000062-GPOS-00031,SRG-OS-000349-GPOS-00137</t>
         </is>
       </c>
-      <c r="D22" s="2" t="inlineStr"/>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90829-3</t>
+        </is>
+      </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish the outcome of the events.</t>
@@ -2115,7 +2179,7 @@
       </c>
       <c r="F23" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow operating system admins to change security attributes on users, the operating system, or the operating systems components.</t>
+          <t>Red Hat Enterprise Linux 9 must allow operating system admins to change security attributes on users, the operating system, or the operating systems components.</t>
         </is>
       </c>
       <c r="G23" s="2" t="inlineStr">
@@ -2163,7 +2227,11 @@
           <t>SRG-OS-000278-GPOS-00108</t>
         </is>
       </c>
-      <c r="D24" s="2" t="inlineStr"/>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87757-1</t>
+        </is>
+      </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
           <t>The operating system must use cryptographic mechanisms to protect the integrity of audit tools.</t>
@@ -2171,7 +2239,7 @@
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use cryptographic mechanisms to protect the integrity of audit tools.</t>
+          <t>Red Hat Enterprise Linux 9 must use cryptographic mechanisms to protect the integrity of audit tools.</t>
         </is>
       </c>
       <c r="G24" s="2" t="inlineStr">
@@ -2243,7 +2311,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2256,7 +2324,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000064-GPOS-00033,SRG-OS-000458-GPOS-00203,SRG-OS-000461-GPOS-00205</t>
         </is>
       </c>
-      <c r="D25" s="2" t="inlineStr"/>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83786-4</t>
+        </is>
+      </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to access categories of information (e.g., classification levels) occur.</t>
@@ -2264,7 +2336,7 @@
       </c>
       <c r="F25" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to access categories of information (e.g., classification levels) occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to access categories of information (e.g., classification levels) occur.</t>
         </is>
       </c>
       <c r="G25" s="2" t="inlineStr">
@@ -2325,7 +2397,11 @@
           <t>SRG-OS-000068-GPOS-00036</t>
         </is>
       </c>
-      <c r="D26" s="2" t="inlineStr"/>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89737-1</t>
+        </is>
+      </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
           <t>The operating system must map the authenticated identity to the user or group account for PKI-based authentication.</t>
@@ -2472,7 +2548,7 @@
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>The operating system must automatically terminate a user session after inactivity time-outs have expired or at shutdown.</t>
+          <t>Red Hat Enterprise Linux 9 must automatically terminate a user session after inactivity time-outs have expired or at shutdown.</t>
         </is>
       </c>
       <c r="G28" s="2" t="inlineStr">
@@ -2522,7 +2598,11 @@
           <t>SRG-OS-000423-GPOS-00187,SRG-OS-000424-GPOS-00188,SRG-OS-000425-GPOS-00189,SRG-OS-000426-GPOS-00190</t>
         </is>
       </c>
-      <c r="D29" s="2" t="inlineStr"/>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90823-6</t>
+        </is>
+      </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect the confidentiality and integrity of transmitted information.</t>
@@ -2530,7 +2610,7 @@
       </c>
       <c r="F29" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect the confidentiality and integrity of transmitted information.</t>
+          <t>Red Hat Enterprise Linux 9 must protect the confidentiality and integrity of transmitted information.</t>
         </is>
       </c>
       <c r="G29" s="2" t="inlineStr">
@@ -2634,7 +2714,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AC-2 (4),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2647,7 +2727,11 @@
           <t>SRG-OS-000004-GPOS-00004,SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000304-GPOS-00121,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000470-GPOS-00214,SRG-OS-000471-GPOS-00215,SRG-OS-000239-GPOS-00089,SRG-OS-000240-GPOS-00090,SRG-OS-000241-GPOS-00091,SRG-OS-000303-GPOS-00120,SRG-OS-000304-GPOS-00121,SRG-OS-000466-GPOS-00210,SRG-OS-000476-GPOS-00221</t>
         </is>
       </c>
-      <c r="D31" s="2" t="inlineStr"/>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90176-9</t>
+        </is>
+      </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
           <t>The operating system must audit all account removal actions.</t>
@@ -2655,7 +2739,7 @@
       </c>
       <c r="F31" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account removal actions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account removal actions.</t>
         </is>
       </c>
       <c r="G31" s="2" t="inlineStr">
@@ -2732,7 +2816,7 @@
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>The operating system must produce audit records containing information to establish what type of events occurred.</t>
+          <t>Red Hat Enterprise Linux 9 must produce audit records containing information to establish what type of events occurred.</t>
         </is>
       </c>
       <c r="G32" s="2" t="inlineStr">
@@ -2781,7 +2865,11 @@
           <t>SRG-OS-000480-GPOS-00226</t>
         </is>
       </c>
-      <c r="D33" s="2" t="inlineStr"/>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83635-3</t>
+        </is>
+      </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce a delay of at least 4 seconds between logon prompts following a failed logon attempt.</t>
@@ -2789,7 +2877,7 @@
       </c>
       <c r="F33" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce a delay of at least 4 seconds between logon prompts following a failed logon attempt.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce a delay of at least 4 seconds between logon prompts following a failed logon attempt.</t>
         </is>
       </c>
       <c r="G33" s="2" t="inlineStr">
@@ -2851,7 +2939,11 @@
           <t>SRG-OS-000030-GPOS-00011,SRG-OS-000028-GPOS-00009</t>
         </is>
       </c>
-      <c r="D34" s="2" t="inlineStr"/>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83599-1</t>
+        </is>
+      </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability for users to directly initiate a session lock for all connection types.</t>
@@ -2925,7 +3017,11 @@
           <t>SRG-OS-000077-GPOS-00045</t>
         </is>
       </c>
-      <c r="D35" s="2" t="inlineStr"/>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86354-8</t>
+        </is>
+      </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
           <t>The operating system must prohibit password reuse for a minimum of five generations.</t>
@@ -2933,7 +3029,7 @@
       </c>
       <c r="F35" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prohibit password reuse for a minimum of five generations.</t>
+          <t>Red Hat Enterprise Linux 9 must prohibit password reuse for a minimum of five generations.</t>
         </is>
       </c>
       <c r="G35" s="2" t="inlineStr">
@@ -2996,7 +3092,11 @@
           <t>SRG-OS-000051-GPOS-00024</t>
         </is>
       </c>
-      <c r="D36" s="2" t="inlineStr"/>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83704-7</t>
+        </is>
+      </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
@@ -3004,7 +3104,7 @@
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
+          <t>Red Hat Enterprise Linux 9 must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
         </is>
       </c>
       <c r="G36" s="2" t="inlineStr">
@@ -3110,7 +3210,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3123,7 +3223,11 @@
           <t>SRG-OS-000057-GPOS-00027,SRG-OS-000058-GPOS-00028,SRG-OS-000059-GPOS-00029,SRG-OS-000206-GPOS-00084</t>
         </is>
       </c>
-      <c r="D38" s="2" t="inlineStr"/>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90516-6</t>
+        </is>
+      </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
           <t>The operating system must reveal error messages only to authorized users.</t>
@@ -3131,7 +3235,7 @@
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>The operating system must reveal error messages only to authorized users.</t>
+          <t>Red Hat Enterprise Linux 9 must reveal error messages only to authorized users.</t>
         </is>
       </c>
       <c r="G38" s="2" t="inlineStr">
@@ -3178,7 +3282,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3191,7 +3295,11 @@
           <t>SRG-OS-000255-GPOS-00096,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D39" s="2" t="inlineStr"/>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83696-5</t>
+        </is>
+      </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish the identity of any individual or process associated with the event.</t>
@@ -3199,7 +3307,7 @@
       </c>
       <c r="F39" s="2" t="inlineStr">
         <is>
-          <t>The operating system must produce audit records containing information to establish the identity of any individual or process associated with the event.</t>
+          <t>Red Hat Enterprise Linux 9 must produce audit records containing information to establish the identity of any individual or process associated with the event.</t>
         </is>
       </c>
       <c r="G39" s="2" t="inlineStr">
@@ -3269,7 +3377,7 @@
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>The operating system must not alter original content or time ordering of audit records when it provides an audit reduction capability.</t>
+          <t>Red Hat Enterprise Linux 9 must not alter original content or time ordering of audit records when it provides an audit reduction capability.</t>
         </is>
       </c>
       <c r="G40" s="2" t="inlineStr">
@@ -3326,7 +3434,7 @@
       </c>
       <c r="F41" s="2" t="inlineStr">
         <is>
-          <t>The operating system must off-load audit records onto a different system or media from the system being audited.</t>
+          <t>Red Hat Enterprise Linux 9 must off-load audit records onto a different system or media from the system being audited.</t>
         </is>
       </c>
       <c r="G41" s="2" t="inlineStr">
@@ -3377,7 +3485,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -3390,7 +3498,11 @@
           <t>SRG-OS-000405-GPOS-00184,SRG-OS-000185-GPOS-00079,SRG-OS-000404-GPOS-00183</t>
         </is>
       </c>
-      <c r="D42" s="2" t="inlineStr"/>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90849-1</t>
+        </is>
+      </c>
       <c r="E42" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement cryptographic mechanisms to prevent unauthorized modification of all information at rest on all operating system components.</t>
@@ -3398,7 +3510,7 @@
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to prevent unauthorized modification of all information at rest on all operating system components.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to prevent unauthorized modification of all information at rest on all operating system components.</t>
         </is>
       </c>
       <c r="G42" s="2" t="inlineStr">
@@ -3471,7 +3583,11 @@
           <t>SRG-OS-000027-GPOS-00008</t>
         </is>
       </c>
-      <c r="D43" s="2" t="inlineStr"/>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83641-1</t>
+        </is>
+      </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit the number of concurrent sessions to ten for all accounts and/or account types.</t>
@@ -3479,7 +3595,7 @@
       </c>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>The operating system must limit the number of concurrent sessions to ten for all accounts and/or account types.</t>
+          <t>Red Hat Enterprise Linux 9 must limit the number of concurrent sessions to ten for all accounts and/or account types.</t>
         </is>
       </c>
       <c r="G43" s="2" t="inlineStr">
@@ -3542,7 +3658,11 @@
           <t>SRG-OS-000373-GPOS-00156,SRG-OS-000373-GPOS-00157,SRG-OS-000373-GPOS-00158</t>
         </is>
       </c>
-      <c r="D44" s="2" t="inlineStr"/>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83544-7</t>
+        </is>
+      </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
           <t>The operating system must require users to re-authenticate when changing authenticators.</t>
@@ -3550,7 +3670,7 @@
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require users to re-authenticate when changing authenticators.</t>
+          <t>Red Hat Enterprise Linux 9 must require users to re-authenticate when changing authenticators.</t>
         </is>
       </c>
       <c r="G44" s="2" t="inlineStr">
@@ -3612,7 +3732,11 @@
           <t>SRG-OS-000023-GPOS-00006,SRG-OS-000024-GPOS-00007,SRG-OS-000228-GPOS-00088</t>
         </is>
       </c>
-      <c r="D45" s="2" t="inlineStr"/>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90807-9</t>
+        </is>
+      </c>
       <c r="E45" s="2" t="inlineStr">
         <is>
           <t>Any publically accessible connection to the operating system must display the Standard Mandatory DoD Notice and Consent Banner before granting access to the system.</t>
@@ -3620,7 +3744,7 @@
       </c>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>Any publically accessible connection to the operating system must display the Standard Mandatory DoD Notice and Consent Banner before granting access to the system.</t>
+          <t>Any publically accessible connection to Red Hat Enterprise Linux 9 must display the Standard Mandatory DoD Notice and Consent Banner before granting access to the system.</t>
         </is>
       </c>
       <c r="G45" s="2" t="inlineStr">
@@ -3718,7 +3842,7 @@
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to access security objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to access security objects occur.</t>
         </is>
       </c>
       <c r="G46" s="2" t="inlineStr">
@@ -3774,7 +3898,7 @@
       </c>
       <c r="F47" s="2" t="inlineStr">
         <is>
-          <t>The operating system must notify system administrators and ISSOs of account enabling actions.</t>
+          <t>Red Hat Enterprise Linux 9 must notify system administrators and ISSOs of account enabling actions.</t>
         </is>
       </c>
       <c r="G47" s="2" t="inlineStr">
@@ -3823,7 +3947,11 @@
           <t>SRG-OS-000480-GPOS-00228,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D48" s="2" t="inlineStr"/>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83644-5</t>
+        </is>
+      </c>
       <c r="E48" s="2" t="inlineStr">
         <is>
           <t>The operating system must define default permissions for all authenticated users in such a way that the user can only read and modify their own files.</t>
@@ -3831,7 +3959,7 @@
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>The operating system must define default permissions for all authenticated users in such a way that the user can only read and modify their own files.</t>
+          <t>Red Hat Enterprise Linux 9 must define default permissions for all authenticated users in such a way that the user can only read and modify their own files.</t>
         </is>
       </c>
       <c r="G48" s="2" t="inlineStr">
@@ -3903,7 +4031,7 @@
       </c>
       <c r="F49" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to prevent unauthorized disclosure of all information at rest on all operating system components.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to prevent unauthorized disclosure of all information at rest on all operating system components.</t>
         </is>
       </c>
       <c r="G49" s="2" t="inlineStr">
@@ -3951,7 +4079,11 @@
           <t>SRG-OS-000109-GPOS-00056,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D50" s="2" t="inlineStr"/>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90800-4</t>
+        </is>
+      </c>
       <c r="E50" s="2" t="inlineStr">
         <is>
           <t>The operating system must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
@@ -4033,7 +4165,7 @@
       </c>
       <c r="F51" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to prevent unauthorized disclosure of information and/or detect changes to information during transmission unless otherwise protected by alternative physical safeguards, such as, at a minimum, a</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to prevent unauthorized disclosure of information and/or detect changes to information during transmission unless otherwise protected by alternative physical safeguards, such as, at a minimum, a</t>
         </is>
       </c>
       <c r="G51" s="2" t="inlineStr">
@@ -4083,7 +4215,11 @@
           <t>SRG-OS-000120-GPOS-00061</t>
         </is>
       </c>
-      <c r="D52" s="2" t="inlineStr"/>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84221-1</t>
+        </is>
+      </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
           <t>The operating system must use mechanisms meeting the requirements of applicable federal laws, Executive orders, directives, policies, regulations, standards, and guidance for authentication to a cryptographic module.</t>
@@ -4159,7 +4295,11 @@
           <t>SRG-OS-000396-GPOS-00176,SRG-OS-000393-GPOS-00173,SRG-OS-000394-GPOS-00174</t>
         </is>
       </c>
-      <c r="D53" s="2" t="inlineStr"/>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83450-7</t>
+        </is>
+      </c>
       <c r="E53" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement cryptographic mechanisms to protect the integrity of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
@@ -4167,7 +4307,7 @@
       </c>
       <c r="F53" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to protect the integrity of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to protect the integrity of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
         </is>
       </c>
       <c r="G53" s="2" t="inlineStr">
@@ -4296,7 +4436,11 @@
           <t>SRG-OS-000250-GPOS-00093,SRG-OS-000423-GPOS-00187</t>
         </is>
       </c>
-      <c r="D55" s="2" t="inlineStr"/>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86860-4</t>
+        </is>
+      </c>
       <c r="E55" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement cryptography to protect the integrity of remote access sessions.</t>
@@ -4304,7 +4448,7 @@
       </c>
       <c r="F55" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptography to protect the integrity of remote access sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptography to protect the integrity of remote access sessions.</t>
         </is>
       </c>
       <c r="G55" s="2" t="inlineStr">
@@ -4354,7 +4498,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4367,7 +4511,11 @@
           <t>SRG-OS-000392-GPOS-00172,SRG-OS-000470-GPOS-00214,SRG-OS-000473-GPOS-00218</t>
         </is>
       </c>
-      <c r="D56" s="2" t="inlineStr"/>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83783-1</t>
+        </is>
+      </c>
       <c r="E56" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful logon attempts occur.</t>
@@ -4375,7 +4523,7 @@
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful logon attempts occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful logon attempts occur.</t>
         </is>
       </c>
       <c r="G56" s="2" t="inlineStr">
@@ -4434,7 +4582,11 @@
           <t>SRG-OS-000433-GPOS-00192</t>
         </is>
       </c>
-      <c r="D57" s="2" t="inlineStr"/>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83970-4</t>
+        </is>
+      </c>
       <c r="E57" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement non-executable data to protect its memory from unauthorized code execution.</t>
@@ -4442,7 +4594,7 @@
       </c>
       <c r="F57" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement non-executable data to protect its memory from unauthorized code execution.</t>
+          <t>Red Hat Enterprise Linux 9 must implement non-executable data to protect its memory from unauthorized code execution.</t>
         </is>
       </c>
       <c r="G57" s="2" t="inlineStr">
@@ -4521,7 +4673,11 @@
           <t>SRG-OS-000029-GPOS-00010</t>
         </is>
       </c>
-      <c r="D58" s="2" t="inlineStr"/>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89876-7</t>
+        </is>
+      </c>
       <c r="E58" s="2" t="inlineStr">
         <is>
           <t>The operating system must initiate a session lock after a 15-minute period of inactivity for all connection types.</t>
@@ -4529,7 +4685,7 @@
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>The operating system must initiate a session lock after a 15-minute period of inactivity for all connection types.</t>
+          <t>Red Hat Enterprise Linux 9 must initiate a session lock after a 15-minute period of inactivity for all connection types.</t>
         </is>
       </c>
       <c r="G58" s="2" t="inlineStr">
@@ -4599,7 +4755,7 @@
       </c>
       <c r="F59" s="2" t="inlineStr">
         <is>
-          <t>The operating system must uniquely identify peripherals before establishing a connection.</t>
+          <t>Red Hat Enterprise Linux 9 must uniquely identify peripherals before establishing a connection.</t>
         </is>
       </c>
       <c r="G59" s="2" t="inlineStr">
@@ -4750,7 +4906,7 @@
       </c>
       <c r="F61" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide the capability for assigned IMOs/ISSOs or designated SAs to change the auditing to be performed on all operating system components, based on all selectable event criteria in near real time.</t>
+          <t>Red Hat Enterprise Linux 9 must provide the capability for assigned IMOs/ISSOs or designated SAs to change the auditing to be performed on all operating system components, based on all selectable event criteria in near real time.</t>
         </is>
       </c>
       <c r="G61" s="2" t="inlineStr">
@@ -4806,7 +4962,7 @@
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
       <c r="G62" s="2" t="inlineStr">
@@ -4841,7 +4997,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -4854,7 +5010,11 @@
           <t>SRG-OS-000046-GPOS-00022,SRG-OS-000343-GPOS-00134</t>
         </is>
       </c>
-      <c r="D63" s="2" t="inlineStr"/>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83698-1</t>
+        </is>
+      </c>
       <c r="E63" s="2" t="inlineStr">
         <is>
           <t>The operating system must immediately notify the SA and ISSO (at a minimum) when allocated audit record storage volume reaches 75% of the repository maximum audit record storage capacity.</t>
@@ -4862,7 +5022,7 @@
       </c>
       <c r="F63" s="2" t="inlineStr">
         <is>
-          <t>The operating system must immediately notify the SA and ISSO (at a minimum) when allocated audit record storage volume reaches 75% of the repository maximum audit record storage capacity.</t>
+          <t>Red Hat Enterprise Linux 9 must immediately notify the SA and ISSO (at a minimum) when allocated audit record storage volume reaches 75% of the repository maximum audit record storage capacity.</t>
         </is>
       </c>
       <c r="G63" s="2" t="inlineStr">
@@ -4942,7 +5102,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>To prevent the compromise of authentication information, such as passwords during the authentication process, the feedback from the operating system must not provide any information allowing an unauthorized user to compromise the authentication mechanism.
+          <t>To prevent the compromise of authentication information, such as passwords during the authentication process, the feedback from Red Hat Enterprise Linux 9 must not provide any information allowing an unauthorized user to compromise the authentication mechanism.
 Obfuscation of user-provided information that is typed into the system is a method used when addressing this risk.
 For example, displaying asterisks when a user types in a password is an example of obscuring feedback of authentication information.</t>
         </is>
@@ -5005,7 +5165,11 @@
           <t>SRG-OS-000106-GPOS-00053,SRG-OS-000480-GPOS-00229,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D65" s="2" t="inlineStr"/>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90799-8</t>
+        </is>
+      </c>
       <c r="E65" s="2" t="inlineStr">
         <is>
           <t>The operating system must use multifactor authentication for network access to non-privileged accounts.</t>
@@ -5096,7 +5260,7 @@
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce password complexity by requiring that at least one special character be used.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce password complexity by requiring that at least one special character be used.</t>
         </is>
       </c>
       <c r="G66" s="2" t="inlineStr">
@@ -5132,7 +5296,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5145,7 +5309,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000458-GPOS-00203,SRG-OS-000462-GPOS-00206,SRG-OS-000463-GPOS-00207,SRG-OS-000471-GPOS-00215,SRG-OS-000474-GPOS-00219,SRG-OS-000466-GPOS-00210,SRG-OS-000064-GPOS-00033</t>
         </is>
       </c>
-      <c r="D67" s="2" t="inlineStr"/>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83821-9</t>
+        </is>
+      </c>
       <c r="E67" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to modify security objects occur.</t>
@@ -5153,7 +5321,7 @@
       </c>
       <c r="F67" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to modify security objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to modify security objects occur.</t>
         </is>
       </c>
       <c r="G67" s="2" t="inlineStr">
@@ -5224,7 +5392,7 @@
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>The operating system must limit the ability of non-privileged users to grant other users direct access to the contents of their home directories/folders.</t>
+          <t>Red Hat Enterprise Linux 9 must limit the ability of non-privileged users to grant other users direct access to the contents of their home directories/folders.</t>
         </is>
       </c>
       <c r="G68" s="2" t="inlineStr">
@@ -5258,7 +5426,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-12 (3),AU-7 b,AU-7 a,AU-12 a,CM-6 b,AU-12 c,CM-5 (1)</t>
+          <t>AU-7 b,AU-7 a,AU-12 a,CM-5 (1),CM-6 b,AU-12 (3),AU-12 c,AU-8 b</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5271,7 +5439,11 @@
           <t>SRG-OS-000122-GPOS-00063,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000359-GPOS-00146,SRG-OS-000365-GPOS-00152,SRG-OS-000474-GPOS-00219,SRG-OS-000475-GPOS-00220,SRG-OS-000480-GPOS-00227,SRG-OS-000062-GPOS-00031</t>
         </is>
       </c>
-      <c r="D69" s="2" t="inlineStr"/>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83649-4</t>
+        </is>
+      </c>
       <c r="E69" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish when (date and time) the events occurred.</t>
@@ -5342,7 +5514,11 @@
           <t>SRG-OS-000138-GPOS-00069</t>
         </is>
       </c>
-      <c r="D70" s="2" t="inlineStr"/>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83895-3</t>
+        </is>
+      </c>
       <c r="E70" s="2" t="inlineStr">
         <is>
           <t>Operating systems must prevent unauthorized and unintended information transfer via shared system resources.</t>
@@ -5421,7 +5597,11 @@
           <t>SRG-OS-000039-GPOS-00017,SRG-OS-000342-GPOS-00133,SRG-OS-000479-GPOS-00224</t>
         </is>
       </c>
-      <c r="D71" s="2" t="inlineStr"/>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83686-6</t>
+        </is>
+      </c>
       <c r="E71" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish where the events occurred.</t>
@@ -5571,7 +5751,7 @@
       </c>
       <c r="F73" s="2" t="inlineStr">
         <is>
-          <t>The operating system must not alter original content or time ordering of audit records when it provides a report generation capability.</t>
+          <t>Red Hat Enterprise Linux 9 must not alter original content or time ordering of audit records when it provides a report generation capability.</t>
         </is>
       </c>
       <c r="G73" s="2" t="inlineStr">
@@ -5620,7 +5800,11 @@
           <t>SRG-OS-000062-GPOS-00031</t>
         </is>
       </c>
-      <c r="D74" s="2" t="inlineStr"/>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84206-2</t>
+        </is>
+      </c>
       <c r="E74" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
@@ -5628,7 +5812,7 @@
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
+          <t>Red Hat Enterprise Linux 9 must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
         </is>
       </c>
       <c r="G74" s="2" t="inlineStr">
@@ -5765,7 +5949,7 @@
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement NSA-approved cryptography to protect classified information in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
+          <t>Red Hat Enterprise Linux 9 must implement NSA-approved cryptography to protect classified information in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
         </is>
       </c>
       <c r="G76" s="2" t="inlineStr">
@@ -5799,7 +5983,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AC-2 (4),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -5812,7 +5996,11 @@
           <t>SRG-OS-000004-GPOS-00004,SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000304-GPOS-00121,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000470-GPOS-00214,SRG-OS-000471-GPOS-00215,SRG-OS-000239-GPOS-00089,SRG-OS-000240-GPOS-00090,SRG-OS-000241-GPOS-00091,SRG-OS-000303-GPOS-00120,SRG-OS-000304-GPOS-00121,SRG-OS-000466-GPOS-00210,SRG-OS-000476-GPOS-00221,SRG-OS-000274-GPOS-00104,SRG-OS-000275-GPOS-00105,SRG-OS-000276-GPOS-00106,SRG-OS-000277-GPOS-00107</t>
         </is>
       </c>
-      <c r="D77" s="2" t="inlineStr"/>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83714-6</t>
+        </is>
+      </c>
       <c r="E77" s="2" t="inlineStr">
         <is>
           <t>The operating system must notify system administrators and ISSOs when accounts are removed.</t>
@@ -5899,7 +6087,11 @@
           <t>SRG-OS-000125-GPOS-00065</t>
         </is>
       </c>
-      <c r="D78" s="2" t="inlineStr"/>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86722-6</t>
+        </is>
+      </c>
       <c r="E78" s="2" t="inlineStr">
         <is>
           <t>The operating system must employ strong authenticators in the establishment of nonlocal maintenance and diagnostic sessions.</t>
@@ -5964,7 +6156,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -5977,7 +6169,11 @@
           <t>SRG-OS-000256-GPOS-00097,SRG-OS-000257-GPOS-00098,SRG-OS-000258-GPOS-00099,SRG-OS-000278-GPOS-00108</t>
         </is>
       </c>
-      <c r="D79" s="2" t="inlineStr"/>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90840-0</t>
+        </is>
+      </c>
       <c r="E79" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect audit tools from unauthorized deletion.</t>
@@ -5985,7 +6181,7 @@
       </c>
       <c r="F79" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit tools from unauthorized deletion.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit tools from unauthorized deletion.</t>
         </is>
       </c>
       <c r="G79" s="2" t="inlineStr">
@@ -6035,7 +6231,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (1),IA-2 (2),IA-2 (3),IA-2 (4)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6122,7 +6318,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6135,7 +6331,11 @@
           <t>SRG-OS-000480-GPOS-00227,SRG-OS-000366-GPOS-00153</t>
         </is>
       </c>
-      <c r="D81" s="2" t="inlineStr"/>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83954-8</t>
+        </is>
+      </c>
       <c r="E81" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent the installation of patches, service packs, device drivers, or operating system components without verification they have been digitally signed using a certificate that is recognized and approved by the organization.</t>
@@ -6143,7 +6343,7 @@
       </c>
       <c r="F81" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent the installation of patches, service packs, device drivers, or operating system components without verification they have been digitally signed using a certificate that is recognized and approved by the organization.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent the installation of patches, service packs, device drivers, or operating system components without verification they have been digitally signed using a certificate that is recognized and approved by the organization.</t>
         </is>
       </c>
       <c r="G81" s="2" t="inlineStr">
@@ -6228,7 +6428,7 @@
       </c>
       <c r="F82" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to access privileges occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to access privileges occur.</t>
         </is>
       </c>
       <c r="G82" s="2" t="inlineStr">
@@ -6341,7 +6541,7 @@
       </c>
       <c r="F84" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect against or limit the effects of Denial of Service (DoS) attacks by ensuring the operating system is implementing rate-limiting measures on impacted network interfaces.</t>
+          <t>Red Hat Enterprise Linux 9 must protect against or limit the effects of Denial of Service (DoS) attacks by ensuring the operating system is implementing rate-limiting measures on impacted network interfaces.</t>
         </is>
       </c>
       <c r="G84" s="2" t="inlineStr">
@@ -6420,7 +6620,7 @@
       </c>
       <c r="F85" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent all software from executing at higher privilege levels than users executing the software.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent all software from executing at higher privilege levels than users executing the software.</t>
         </is>
       </c>
       <c r="G85" s="2" t="inlineStr">
@@ -6455,7 +6655,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6468,7 +6668,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000064-GPOS-00033,SRG-OS-000466-GPOS-00210,SRG-OS-000458-GPOS-00203,SRG-OS-000474-GPOS-00219</t>
         </is>
       </c>
-      <c r="D86" s="2" t="inlineStr"/>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83812-8</t>
+        </is>
+      </c>
       <c r="E86" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful accesses to objects occur.</t>
@@ -6476,7 +6680,7 @@
       </c>
       <c r="F86" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful accesses to objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful accesses to objects occur.</t>
         </is>
       </c>
       <c r="G86" s="2" t="inlineStr">
@@ -6539,7 +6743,11 @@
           <t>SRG-OS-000073-GPOS-00041</t>
         </is>
       </c>
-      <c r="D87" s="2" t="inlineStr"/>
+      <c r="D87" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88865-1</t>
+        </is>
+      </c>
       <c r="E87" s="2" t="inlineStr">
         <is>
           <t>The operating system must store only encrypted representations of passwords.</t>
@@ -6547,7 +6755,7 @@
       </c>
       <c r="F87" s="2" t="inlineStr">
         <is>
-          <t>The operating system must store only encrypted representations of passwords.</t>
+          <t>Red Hat Enterprise Linux 9 must store only encrypted representations of passwords.</t>
         </is>
       </c>
       <c r="G87" s="2" t="inlineStr">
@@ -6601,7 +6809,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),CM-5 (1),AC-6 (9),AU-12 c</t>
+          <t>AU-12 c,CM-5 (1),AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6622,7 +6830,7 @@
       </c>
       <c r="F88" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records showing starting and ending time for user access to the system.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records showing starting and ending time for user access to the system.</t>
         </is>
       </c>
       <c r="G88" s="2" t="inlineStr">
@@ -6668,7 +6876,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (4),IA-2 (2),IA-2 (3),IA-2</t>
+          <t>IA-2,IA-2 (2),IA-2 (3),IA-2 (5),IA-2 (4)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6681,7 +6889,11 @@
           <t>SRG-OS-000104-GPOS-00051,SRG-OS-000106-GPOS-00053,SRG-OS-000107-GPOS-00054,SRG-OS-000109-GPOS-00056,SRG-OS-000108-GPOS-00055,SRG-OS-000108-GPOS-00057,SRG-OS-000108-GPOS-00058</t>
         </is>
       </c>
-      <c r="D89" s="2" t="inlineStr"/>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89122-6</t>
+        </is>
+      </c>
       <c r="E89" s="2" t="inlineStr">
         <is>
           <t>The operating system must uniquely identify and must authenticate organizational users (or processes acting on behalf of organizational users).</t>
@@ -6761,7 +6973,11 @@
           <t>SRG-OS-000375-GPOS-00160,SRG-OS-000377-GPOS-00162</t>
         </is>
       </c>
-      <c r="D90" s="2" t="inlineStr"/>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87088-1</t>
+        </is>
+      </c>
       <c r="E90" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
@@ -6769,7 +6985,7 @@
       </c>
       <c r="F90" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
+          <t>Red Hat Enterprise Linux 9 must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
         </is>
       </c>
       <c r="G90" s="2" t="inlineStr">
@@ -6824,7 +7040,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -6837,7 +7053,11 @@
           <t>SRG-OS-000256-GPOS-00097,SRG-OS-000257-GPOS-00098,SRG-OS-000278-GPOS-00108</t>
         </is>
       </c>
-      <c r="D91" s="2" t="inlineStr"/>
+      <c r="D91" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90842-6</t>
+        </is>
+      </c>
       <c r="E91" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect audit tools from unauthorized modification.</t>
@@ -6845,7 +7065,7 @@
       </c>
       <c r="F91" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit tools from unauthorized modification.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit tools from unauthorized modification.</t>
         </is>
       </c>
       <c r="G91" s="2" t="inlineStr">
@@ -7008,7 +7228,7 @@
       </c>
       <c r="F93" s="2" t="inlineStr">
         <is>
-          <t>The operating system must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
+          <t>Red Hat Enterprise Linux 9 must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
         </is>
       </c>
       <c r="G93" s="2" t="inlineStr">
@@ -7056,7 +7276,11 @@
           <t>SRG-OS-000075-GPOS-00043</t>
         </is>
       </c>
-      <c r="D94" s="2" t="inlineStr"/>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83610-6</t>
+        </is>
+      </c>
       <c r="E94" s="2" t="inlineStr">
         <is>
           <t>Operating systems must enforce 24 hours/1 day as the minimum password lifetime.</t>
@@ -7133,7 +7357,11 @@
           <t>SRG-OS-000072-GPOS-00040</t>
         </is>
       </c>
-      <c r="D95" s="2" t="inlineStr"/>
+      <c r="D95" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83564-5</t>
+        </is>
+      </c>
       <c r="E95" s="2" t="inlineStr">
         <is>
           <t>The operating system must require the change of at least 50% of the total number of characters when passwords are changed.</t>
@@ -7141,7 +7369,7 @@
       </c>
       <c r="F95" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require the change of at least 50% of the total number of characters when passwords are changed.</t>
+          <t>Red Hat Enterprise Linux 9 must require the change of at least 50% of the total number of characters when passwords are changed.</t>
         </is>
       </c>
       <c r="G95" s="2" t="inlineStr">
@@ -7198,7 +7426,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>SC-8 (1),AC-18 (1),SC-8</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7211,7 +7439,11 @@
           <t>SRG-OS-000299-GPOS-00117,SRG-OS-000300-GPOS-00118,SRG-OS-000424-GPOS-00188,SRG-OS-000481-GPOS-000481</t>
         </is>
       </c>
-      <c r="D96" s="2" t="inlineStr"/>
+      <c r="D96" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84066-0</t>
+        </is>
+      </c>
       <c r="E96" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect wireless access to and from the system using encryption.</t>
@@ -7219,7 +7451,7 @@
       </c>
       <c r="F96" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect wireless access to and from the system using encryption.</t>
+          <t>Red Hat Enterprise Linux 9 must protect wireless access to and from the system using encryption.</t>
         </is>
       </c>
       <c r="G96" s="2" t="inlineStr">
@@ -7287,7 +7519,11 @@
           <t>SRG-OS-000355-GPOS-00143,SRG-OS-000356-GPOS-00144,SRG-OS-000359-GPOS-00146</t>
         </is>
       </c>
-      <c r="D97" s="2" t="inlineStr"/>
+      <c r="D97" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88648-1</t>
+        </is>
+      </c>
       <c r="E97" s="2" t="inlineStr">
         <is>
           <t>The operating system must synchronize internal information system clocks to the authoritative time source when the time difference is greater than one second.</t>
@@ -7295,7 +7531,7 @@
       </c>
       <c r="F97" s="2" t="inlineStr">
         <is>
-          <t>The operating system must synchronize internal information system clocks to the authoritative time source when the time difference is greater than one second.</t>
+          <t>Red Hat Enterprise Linux 9 must synchronize internal information system clocks to the authoritative time source when the time difference is greater than one second.</t>
         </is>
       </c>
       <c r="G97" s="2" t="inlineStr">
@@ -7360,7 +7596,11 @@
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D98" s="2" t="inlineStr"/>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89858-5</t>
+        </is>
+      </c>
       <c r="E98" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
@@ -7368,7 +7608,7 @@
       </c>
       <c r="F98" s="2" t="inlineStr">
         <is>
-          <t>The operating system must limit privileges to change software resident within software libraries.</t>
+          <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
       <c r="G98" s="2" t="inlineStr">
@@ -7435,7 +7675,11 @@
           <t>SRG-OS-000057-GPOS-00027,SRG-OS-000058-GPOS-00028,SRG-OS-000059-GPOS-00029</t>
         </is>
       </c>
-      <c r="D99" s="2" t="inlineStr"/>
+      <c r="D99" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83716-1</t>
+        </is>
+      </c>
       <c r="E99" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect audit information from unauthorized read access.</t>
@@ -7443,7 +7687,7 @@
       </c>
       <c r="F99" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit information from unauthorized read access.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit information from unauthorized read access.</t>
         </is>
       </c>
       <c r="G99" s="2" t="inlineStr">
@@ -7584,7 +7828,11 @@
           <t>SRG-OS-000373-GPOS-00156,SRG-OS-000312-GPOS-00123</t>
         </is>
       </c>
-      <c r="D101" s="2" t="inlineStr"/>
+      <c r="D101" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90085-2</t>
+        </is>
+      </c>
       <c r="E101" s="2" t="inlineStr">
         <is>
           <t>The operating system must require users to re-authenticate for privilege escalation.</t>
@@ -7592,7 +7840,7 @@
       </c>
       <c r="F101" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require users to re-authenticate for privilege escalation.</t>
+          <t>Red Hat Enterprise Linux 9 must require users to re-authenticate for privilege escalation.</t>
         </is>
       </c>
       <c r="G101" s="2" t="inlineStr">
@@ -7641,7 +7889,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -7654,7 +7902,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000471-GPOS-00216,SRG-OS-000477-GPOS-00222</t>
         </is>
       </c>
-      <c r="D102" s="2" t="inlineStr"/>
+      <c r="D102" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83802-9</t>
+        </is>
+      </c>
       <c r="E102" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records for all kernel module load, unload, and restart actions, and also for all program initiations.</t>
@@ -7662,7 +7914,7 @@
       </c>
       <c r="F102" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for all kernel module load, unload, and restart actions, and also for all program initiations.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for all kernel module load, unload, and restart actions, and also for all program initiations.</t>
         </is>
       </c>
       <c r="G102" s="2" t="inlineStr">
@@ -7809,7 +8061,7 @@
       </c>
       <c r="F104" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account enabling actions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account enabling actions.</t>
         </is>
       </c>
       <c r="G104" s="2" t="inlineStr">
@@ -7857,7 +8109,11 @@
           <t>SRG-OS-000327-GPOS-00127</t>
         </is>
       </c>
-      <c r="D105" s="2" t="inlineStr"/>
+      <c r="D105" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83759-1</t>
+        </is>
+      </c>
       <c r="E105" s="2" t="inlineStr">
         <is>
           <t>The operating system must audit the execution of privileged functions.</t>
@@ -7865,7 +8121,7 @@
       </c>
       <c r="F105" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit the execution of privileged functions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit the execution of privileged functions.</t>
         </is>
       </c>
       <c r="G105" s="2" t="inlineStr">
@@ -7945,7 +8201,7 @@
       </c>
       <c r="F106" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for all direct access to the information system.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for all direct access to the information system.</t>
         </is>
       </c>
       <c r="G106" s="2" t="inlineStr">
@@ -8001,7 +8257,7 @@
       </c>
       <c r="F107" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide a report generation capability that supports on-demand reporting requirements.</t>
+          <t>Red Hat Enterprise Linux 9 must provide a report generation capability that supports on-demand reporting requirements.</t>
         </is>
       </c>
       <c r="G107" s="2" t="inlineStr">
@@ -8057,7 +8313,7 @@
       </c>
       <c r="F108" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit information from unauthorized deletion.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit information from unauthorized deletion.</t>
         </is>
       </c>
       <c r="G108" s="2" t="inlineStr">
@@ -8191,7 +8447,7 @@
       </c>
       <c r="F110" s="2" t="inlineStr">
         <is>
-          <t>The operating system must maintain the confidentiality and integrity of information during reception.</t>
+          <t>Red Hat Enterprise Linux 9 must maintain the confidentiality and integrity of information during reception.</t>
         </is>
       </c>
       <c r="G110" s="2" t="inlineStr">
@@ -8240,7 +8496,11 @@
           <t>SRG-OS-000046-GPOS-00022,SRG-OS-000047-GPOS-00023</t>
         </is>
       </c>
-      <c r="D111" s="2" t="inlineStr"/>
+      <c r="D111" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83709-6</t>
+        </is>
+      </c>
       <c r="E111" s="2" t="inlineStr">
         <is>
           <t>The operating system must shut down by default upon audit failure (unless availability is an overriding concern).</t>
@@ -8248,7 +8508,7 @@
       </c>
       <c r="F111" s="2" t="inlineStr">
         <is>
-          <t>The operating system must shut down by default upon audit failure (unless availability is an overriding concern).</t>
+          <t>Red Hat Enterprise Linux 9 must shut down by default upon audit failure (unless availability is an overriding concern).</t>
         </is>
       </c>
       <c r="G111" s="2" t="inlineStr">
@@ -8325,7 +8585,7 @@
       </c>
       <c r="F112" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when concurrent logons to the same account occur from different sources.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when concurrent logons to the same account occur from different sources.</t>
         </is>
       </c>
       <c r="G112" s="2" t="inlineStr">
@@ -8381,7 +8641,7 @@
       </c>
       <c r="F113" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow operating system admins to grant their privileges to other operating system admins.</t>
+          <t>Red Hat Enterprise Linux 9 must allow operating system admins to grant their privileges to other operating system admins.</t>
         </is>
       </c>
       <c r="G113" s="2" t="inlineStr">
@@ -8437,7 +8697,7 @@
       </c>
       <c r="F114" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide a report generation capability that supports after-the-fact investigations of security incidents.</t>
+          <t>Red Hat Enterprise Linux 9 must provide a report generation capability that supports after-the-fact investigations of security incidents.</t>
         </is>
       </c>
       <c r="G114" s="2" t="inlineStr">
@@ -8576,7 +8836,7 @@
       </c>
       <c r="F116" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">The operating system must notify system administrators and ISSOs when accounts are disabled. </t>
+          <t xml:space="preserve">Red Hat Enterprise Linux 9 must notify system administrators and ISSOs when accounts are disabled. </t>
         </is>
       </c>
       <c r="G116" s="2" t="inlineStr">
@@ -8629,7 +8889,11 @@
           <t>SRG-OS-000437-GPOS-00194</t>
         </is>
       </c>
-      <c r="D117" s="2" t="inlineStr"/>
+      <c r="D117" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83458-0</t>
+        </is>
+      </c>
       <c r="E117" s="2" t="inlineStr">
         <is>
           <t>The operating system must remove all software components after updated versions have been installed.</t>
@@ -8769,7 +9033,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -8782,7 +9046,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000458-GPOS-00203,SRG-OS-000462-GPOS-00206,SRG-OS-000463-GPOS-00207,SRG-OS-000468-GPOS-00212,SRG-OS-000471-GPOS-00215,SRG-OS-000474-GPOS-00219,SRG-OS-000064-GPOS-00033</t>
         </is>
       </c>
-      <c r="D119" s="2" t="inlineStr"/>
+      <c r="D119" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83817-7</t>
+        </is>
+      </c>
       <c r="E119" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security objects occur.</t>
@@ -8790,7 +9058,7 @@
       </c>
       <c r="F119" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete security objects occur.</t>
         </is>
       </c>
       <c r="G119" s="2" t="inlineStr">
@@ -8936,7 +9204,7 @@
       </c>
       <c r="F121" s="2" t="inlineStr">
         <is>
-          <t>The operating system must behave in a predictable and documented manner that reflects organizational and system objectives when invalid inputs are received.</t>
+          <t>Red Hat Enterprise Linux 9 must behave in a predictable and documented manner that reflects organizational and system objectives when invalid inputs are received.</t>
         </is>
       </c>
       <c r="G121" s="2" t="inlineStr">
@@ -9005,7 +9273,11 @@
           <t>SRG-OS-000378-GPOS-00163</t>
         </is>
       </c>
-      <c r="D122" s="2" t="inlineStr"/>
+      <c r="D122" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84203-9</t>
+        </is>
+      </c>
       <c r="E122" s="2" t="inlineStr">
         <is>
           <t>The operating system must authenticate peripherals before establishing a connection.</t>
@@ -9013,7 +9285,7 @@
       </c>
       <c r="F122" s="2" t="inlineStr">
         <is>
-          <t>The operating system must authenticate peripherals before establishing a connection.</t>
+          <t>Red Hat Enterprise Linux 9 must authenticate peripherals before establishing a connection.</t>
         </is>
       </c>
       <c r="G122" s="2" t="inlineStr">
@@ -9059,7 +9331,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9072,7 +9344,11 @@
           <t>SRG-OS-000096-GPOS-00050,SRG-OS-000095-GPOS-00049</t>
         </is>
       </c>
-      <c r="D123" s="2" t="inlineStr"/>
+      <c r="D123" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87543-5</t>
+        </is>
+      </c>
       <c r="E123" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured to prohibit or restrict the use of functions, ports, protocols, and/or services, as defined in the PPSM CAL and vulnerability assessments.</t>
@@ -9080,7 +9356,7 @@
       </c>
       <c r="F123" s="2" t="inlineStr">
         <is>
-          <t>The operating system must be configured to prohibit or restrict the use of functions, ports, protocols, and/or services, as defined in the PPSM CAL and vulnerability assessments.</t>
+          <t>Red Hat Enterprise Linux 9 must be configured to prohibit or restrict the use of functions, ports, protocols, and/or services, as defined in the PPSM CAL and vulnerability assessments.</t>
         </is>
       </c>
       <c r="G123" s="2" t="inlineStr">
@@ -9129,7 +9405,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9142,7 +9418,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000466-GPOS-00210,SRG-OS-000467-GPOS-00211,SRG-OS-000468-GPOS-00212</t>
         </is>
       </c>
-      <c r="D124" s="2" t="inlineStr"/>
+      <c r="D124" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83754-2</t>
+        </is>
+      </c>
       <c r="E124" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security levels occur.</t>
@@ -9150,7 +9430,7 @@
       </c>
       <c r="F124" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security levels occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete security levels occur.</t>
         </is>
       </c>
       <c r="G124" s="2" t="inlineStr">
@@ -9199,7 +9479,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9212,7 +9492,11 @@
           <t>SRG-OS-000095-GPOS-00049,SRG-OS-000300-GPOS-00118</t>
         </is>
       </c>
-      <c r="D125" s="2" t="inlineStr"/>
+      <c r="D125" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84067-8</t>
+        </is>
+      </c>
       <c r="E125" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect wireless access to the system using authentication of users and/or devices.</t>
@@ -9220,7 +9504,7 @@
       </c>
       <c r="F125" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect wireless access to the system using authentication of users and/or devices.</t>
+          <t>Red Hat Enterprise Linux 9 must protect wireless access to the system using authentication of users and/or devices.</t>
         </is>
       </c>
       <c r="G125" s="2" t="inlineStr">
@@ -9293,7 +9577,7 @@
       </c>
       <c r="F126" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account disabling actions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account disabling actions.</t>
         </is>
       </c>
       <c r="G126" s="2" t="inlineStr">
@@ -9349,7 +9633,7 @@
       </c>
       <c r="F127" s="2" t="inlineStr">
         <is>
-          <t>The operating system must record time stamps for audit records that meet a minimum granularity of one second for a minimum degree of precision.</t>
+          <t>Red Hat Enterprise Linux 9 must record time stamps for audit records that meet a minimum granularity of one second for a minimum degree of precision.</t>
         </is>
       </c>
       <c r="G127" s="2" t="inlineStr">
@@ -9384,7 +9668,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9397,7 +9681,11 @@
           <t>SRG-OS-000074-GPOS-00042,SRG-OS-000095-GPOS-00049,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D128" s="2" t="inlineStr"/>
+      <c r="D128" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84159-3</t>
+        </is>
+      </c>
       <c r="E128" s="2" t="inlineStr">
         <is>
           <t>The operating system must transmit only encrypted representations of passwords.</t>
@@ -9611,7 +9899,11 @@
           <t>SRG-OS-000071-GPOS-00039</t>
         </is>
       </c>
-      <c r="D131" s="2" t="inlineStr"/>
+      <c r="D131" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83566-0</t>
+        </is>
+      </c>
       <c r="E131" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce password complexity by requiring that at least one numeric character be used.</t>
@@ -9701,7 +9993,7 @@
       </c>
       <c r="F132" s="2" t="inlineStr">
         <is>
-          <t>The operating system must authenticate all endpoint devices before establishing a local, remote, and/or network connection using bidirectional authentication that is cryptographically based.</t>
+          <t>Red Hat Enterprise Linux 9 must authenticate all endpoint devices before establishing a local, remote, and/or network connection using bidirectional authentication that is cryptographically based.</t>
         </is>
       </c>
       <c r="G132" s="2" t="inlineStr">
@@ -9816,7 +10108,11 @@
           <t>SRG-OS-000046-GPOS-00022</t>
         </is>
       </c>
-      <c r="D134" s="2" t="inlineStr"/>
+      <c r="D134" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90826-9</t>
+        </is>
+      </c>
       <c r="E134" s="2" t="inlineStr">
         <is>
           <t>The operating system must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
@@ -9824,7 +10120,7 @@
       </c>
       <c r="F134" s="2" t="inlineStr">
         <is>
-          <t>The operating system must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
+          <t>Red Hat Enterprise Linux 9 must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
       <c r="G134" s="2" t="inlineStr">
@@ -9888,7 +10184,11 @@
           <t>SRG-OS-000080-GPOS-00048</t>
         </is>
       </c>
-      <c r="D135" s="2" t="inlineStr"/>
+      <c r="D135" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83592-6</t>
+        </is>
+      </c>
       <c r="E135" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce approved authorizations for logical access to information and system resources in accordance with applicable access control policies.</t>
@@ -9896,7 +10196,7 @@
       </c>
       <c r="F135" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce approved authorizations for logical access to information and system resources in accordance with applicable access control policies.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce approved authorizations for logical access to information and system resources in accordance with applicable access control policies.</t>
         </is>
       </c>
       <c r="G135" s="2" t="inlineStr">
@@ -9946,7 +10246,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -9959,7 +10259,11 @@
           <t>SRG-OS-000031-GPOS-00012,SRG-OS-000028-GPOS-00009</t>
         </is>
       </c>
-      <c r="D136" s="2" t="inlineStr"/>
+      <c r="D136" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90586-9</t>
+        </is>
+      </c>
       <c r="E136" s="2" t="inlineStr">
         <is>
           <t>The operating system must retain a users session lock until that user reestablishes access using established identification and authentication procedures.</t>
@@ -10054,7 +10358,7 @@
       </c>
       <c r="F137" s="2" t="inlineStr">
         <is>
-          <t>The operating system must notify system administrators and ISSOs when accounts are created.</t>
+          <t>Red Hat Enterprise Linux 9 must notify system administrators and ISSOs when accounts are created.</t>
         </is>
       </c>
       <c r="G137" s="2" t="inlineStr">
@@ -10167,7 +10471,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d,SI-6 b</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10180,7 +10484,11 @@
           <t>SRG-OS-000363-GPOS-00150,SRG-OS-000446-GPOS-00200,SRG-OS-000447-GPOS-00201</t>
         </is>
       </c>
-      <c r="D139" s="2" t="inlineStr"/>
+      <c r="D139" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83437-4</t>
+        </is>
+      </c>
       <c r="E139" s="2" t="inlineStr">
         <is>
           <t>The operating system must perform verification of the correct operation of security functions: upon system start-up and/or restart; upon command by a user with privileged access; and/or every 30 days.</t>
@@ -10188,7 +10496,7 @@
       </c>
       <c r="F139" s="2" t="inlineStr">
         <is>
-          <t>The operating system must perform verification of the correct operation of security functions: upon system start-up and/or restart; upon command by a user with privileged access; and/or every 30 days.</t>
+          <t>Red Hat Enterprise Linux 9 must perform verification of the correct operation of security functions: upon system start-up and/or restart; upon command by a user with privileged access; and/or every 30 days.</t>
         </is>
       </c>
       <c r="G139" s="2" t="inlineStr">
@@ -10268,7 +10576,7 @@
       </c>
       <c r="F140" s="2" t="inlineStr">
         <is>
-          <t>The operating system must be configured to disable non-essential capabilities.</t>
+          <t>Red Hat Enterprise Linux 9 must be configured to disable non-essential capabilities.</t>
         </is>
       </c>
       <c r="G140" s="2" t="inlineStr">
@@ -10325,7 +10633,7 @@
       </c>
       <c r="F141" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide an audit reduction capability that supports on-demand audit review and analysis.</t>
+          <t>Red Hat Enterprise Linux 9 must provide an audit reduction capability that supports on-demand audit review and analysis.</t>
         </is>
       </c>
       <c r="G141" s="2" t="inlineStr">
@@ -10373,7 +10681,11 @@
           <t>SRG-OS-000123-GPOS-00064,SRG-OS-000002-GPOS-00002</t>
         </is>
       </c>
-      <c r="D142" s="2" t="inlineStr"/>
+      <c r="D142" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90560-4</t>
+        </is>
+      </c>
       <c r="E142" s="2" t="inlineStr">
         <is>
           <t>The operating system must automatically remove or disable temporary user accounts after 72 hours.</t>
@@ -10692,7 +11004,7 @@
       </c>
       <c r="F146" s="2" t="inlineStr">
         <is>
-          <t>The operating system must control remote access methods.</t>
+          <t>Red Hat Enterprise Linux 9 must control remote access methods.</t>
         </is>
       </c>
       <c r="G146" s="2" t="inlineStr">
@@ -10741,7 +11053,11 @@
           <t>SRG-OS-000032-GPOS-00013</t>
         </is>
       </c>
-      <c r="D147" s="2" t="inlineStr"/>
+      <c r="D147" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86923-0</t>
+        </is>
+      </c>
       <c r="E147" s="2" t="inlineStr">
         <is>
           <t>The operating system must monitor remote access methods.</t>
@@ -10809,7 +11125,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-14 (1),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-14 (1)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -10822,7 +11138,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000473-GPOS-00218,SRG-OS-000254-GPOS-00095</t>
         </is>
       </c>
-      <c r="D148" s="2" t="inlineStr"/>
+      <c r="D148" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83651-0</t>
+        </is>
+      </c>
       <c r="E148" s="2" t="inlineStr">
         <is>
           <t>The operating system must initiate session audits at system start-up.</t>
@@ -10830,7 +11150,7 @@
       </c>
       <c r="F148" s="2" t="inlineStr">
         <is>
-          <t>The operating system must initiate session audits at system start-up.</t>
+          <t>Red Hat Enterprise Linux 9 must initiate session audits at system start-up.</t>
         </is>
       </c>
       <c r="G148" s="2" t="inlineStr">
@@ -10957,7 +11277,11 @@
           <t>SRG-OS-000063-GPOS-00032</t>
         </is>
       </c>
-      <c r="D150" s="2" t="inlineStr"/>
+      <c r="D150" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89284-4</t>
+        </is>
+      </c>
       <c r="E150" s="2" t="inlineStr">
         <is>
           <t>The operating system must allow only the ISSM (or individuals or roles appointed by the ISSM) to select which auditable events are to be audited.</t>
@@ -11220,7 +11544,7 @@
       </c>
       <c r="F154" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require users to re-authenticate when changing roles.</t>
+          <t>Red Hat Enterprise Linux 9 must require users to re-authenticate when changing roles.</t>
         </is>
       </c>
       <c r="G154" s="2" t="inlineStr">
@@ -11276,7 +11600,7 @@
       </c>
       <c r="F155" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to protect the confidentiality of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to protect the confidentiality of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
         </is>
       </c>
       <c r="G155" s="2" t="inlineStr">
@@ -11334,7 +11658,7 @@
       </c>
       <c r="F156" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit information from unauthorized modification.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit information from unauthorized modification.</t>
         </is>
       </c>
       <c r="G156" s="2" t="inlineStr">
@@ -11370,7 +11694,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11383,7 +11707,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000468-GPOS-00212,SRG-OS-000471-GPOS-00215,SRG-OS-000463-GPOS-00207,SRG-OS-000465-GPOS-00209</t>
         </is>
       </c>
-      <c r="D157" s="2" t="inlineStr"/>
+      <c r="D157" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83748-4</t>
+        </is>
+      </c>
       <c r="E157" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to modify categories of information (e.g., classification levels) occur.</t>
@@ -11391,7 +11719,7 @@
       </c>
       <c r="F157" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to modify categories of information (e.g., classification levels) occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to modify categories of information (e.g., classification levels) occur.</t>
         </is>
       </c>
       <c r="G157" s="2" t="inlineStr">
@@ -11467,7 +11795,7 @@
       </c>
       <c r="F158" s="2" t="inlineStr">
         <is>
-          <t>The operating system must electronically verify Personal Identity Verification (PIV) credentials.</t>
+          <t>Red Hat Enterprise Linux 9 must electronically verify Personal Identity Verification (PIV) credentials.</t>
         </is>
       </c>
       <c r="G158" s="2" t="inlineStr">
@@ -11515,7 +11843,11 @@
           <t>SRG-OS-000423-GPOS-00187,SRG-OS-000033-GPOS-00014</t>
         </is>
       </c>
-      <c r="D159" s="2" t="inlineStr"/>
+      <c r="D159" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87522-9</t>
+        </is>
+      </c>
       <c r="E159" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
@@ -11523,7 +11855,7 @@
       </c>
       <c r="F159" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
         </is>
       </c>
       <c r="G159" s="2" t="inlineStr">
@@ -11663,7 +11995,11 @@
           <t>SRG-OS-000445-GPOS-00199</t>
         </is>
       </c>
-      <c r="D161" s="2" t="inlineStr"/>
+      <c r="D161" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84074-4</t>
+        </is>
+      </c>
       <c r="E161" s="2" t="inlineStr">
         <is>
           <t>The operating system must verify correct operation of all security functions.</t>
@@ -11752,7 +12088,7 @@
       </c>
       <c r="F162" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect the confidentiality and integrity of communications with wireless peripherals.</t>
+          <t>Red Hat Enterprise Linux 9 must protect the confidentiality and integrity of communications with wireless peripherals.</t>
         </is>
       </c>
       <c r="G162" s="2" t="inlineStr">
@@ -11809,7 +12145,7 @@
       </c>
       <c r="F163" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all activities performed during nonlocal maintenance and diagnostic sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all activities performed during nonlocal maintenance and diagnostic sessions.</t>
         </is>
       </c>
       <c r="G163" s="2" t="inlineStr">
@@ -11867,7 +12203,7 @@
       </c>
       <c r="F164" s="2" t="inlineStr">
         <is>
-          <t>The operating system must terminate all sessions and network connections related to nonlocal maintenance when nonlocal maintenance is completed.</t>
+          <t>Red Hat Enterprise Linux 9 must terminate all sessions and network connections related to nonlocal maintenance when nonlocal maintenance is completed.</t>
         </is>
       </c>
       <c r="G164" s="2" t="inlineStr">
@@ -11980,7 +12316,7 @@
       </c>
       <c r="F166" s="2" t="inlineStr">
         <is>
-          <t>The operating system must maintain the confidentiality and integrity of information during preparation for transmission.</t>
+          <t>Red Hat Enterprise Linux 9 must maintain the confidentiality and integrity of information during preparation for transmission.</t>
         </is>
       </c>
       <c r="G166" s="2" t="inlineStr">
@@ -12037,7 +12373,7 @@
       </c>
       <c r="F167" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce password complexity by requiring that at least one upper-case character be used.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce password complexity by requiring that at least one upper-case character be used.</t>
         </is>
       </c>
       <c r="G167" s="2" t="inlineStr">
@@ -12093,7 +12429,7 @@
       </c>
       <c r="F168" s="2" t="inlineStr">
         <is>
-          <t>The operating system must automatically lock an account until the locked account is released by an administrator when three unsuccessful logon attempts in 15 minutes occur.</t>
+          <t>Red Hat Enterprise Linux 9 must automatically lock an account until the locked account is released by an administrator when three unsuccessful logon attempts in 15 minutes occur.</t>
         </is>
       </c>
       <c r="G168" s="2" t="inlineStr">
@@ -12148,7 +12484,7 @@
       </c>
       <c r="F169" s="2" t="inlineStr">
         <is>
-          <t>The operating system must record time stamps for audit records that can be mapped to Coordinated Universal Time (UTC) or Greenwich Mean Time (GMT).</t>
+          <t>Red Hat Enterprise Linux 9 must record time stamps for audit records that can be mapped to Coordinated Universal Time (UTC) or Greenwich Mean Time (GMT).</t>
         </is>
       </c>
       <c r="G169" s="2" t="inlineStr">
@@ -12196,7 +12532,11 @@
           <t>SRG-OS-000480-GPOS-00225</t>
         </is>
       </c>
-      <c r="D170" s="2" t="inlineStr"/>
+      <c r="D170" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88413-0</t>
+        </is>
+      </c>
       <c r="E170" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent the use of dictionary words for passwords.</t>
@@ -12204,7 +12544,7 @@
       </c>
       <c r="F170" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent the use of dictionary words for passwords.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent the use of dictionary words for passwords.</t>
         </is>
       </c>
       <c r="G170" s="2" t="inlineStr">
@@ -12277,7 +12617,7 @@
       </c>
       <c r="F171" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit tools from unauthorized access.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit tools from unauthorized access.</t>
         </is>
       </c>
       <c r="G171" s="2" t="inlineStr">
@@ -12392,7 +12732,7 @@
       </c>
       <c r="F173" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for privileged activities or other system-level access.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for privileged activities or other system-level access.</t>
         </is>
       </c>
       <c r="G173" s="2" t="inlineStr">
@@ -12448,7 +12788,7 @@
       </c>
       <c r="F174" s="2" t="inlineStr">
         <is>
-          <t>The operating system must shut down the information system, restart the information system, and/or notify the system administrator when anomalies in the operation of any security functions are discovered.</t>
+          <t>Red Hat Enterprise Linux 9 must shut down the information system, restart the information system, and/or notify the system administrator when anomalies in the operation of any security functions are discovered.</t>
         </is>
       </c>
       <c r="G174" s="2" t="inlineStr">
@@ -12485,7 +12825,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -12498,7 +12838,11 @@
           <t>SRG-OS-000433-GPOS-00193,SRG-OS-000095-GPOS-00049</t>
         </is>
       </c>
-      <c r="D175" s="2" t="inlineStr"/>
+      <c r="D175" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83843-3</t>
+        </is>
+      </c>
       <c r="E175" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement address space layout randomization to protect its memory from unauthorized code execution.</t>
@@ -12506,7 +12850,7 @@
       </c>
       <c r="F175" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement address space layout randomization to protect its memory from unauthorized code execution.</t>
+          <t>Red Hat Enterprise Linux 9 must implement address space layout randomization to protect its memory from unauthorized code execution.</t>
         </is>
       </c>
       <c r="G175" s="2" t="inlineStr">
@@ -12585,7 +12929,7 @@
       </c>
       <c r="F176" s="2" t="inlineStr">
         <is>
-          <t>The operating system must, for networked systems, compare internal information system clocks at least every 24 hours with a server which is synchronized to one of the redundant United States Naval Observatory (USNO) time servers, or a time server designat</t>
+          <t>Red Hat Enterprise Linux 9 must, for networked systems, compare internal information system clocks at least every 24 hours with a server which is synchronized to one of the redundant United States Naval Observatory (USNO) time servers, or a time server designat</t>
         </is>
       </c>
       <c r="G176" s="2" t="inlineStr">
@@ -12634,7 +12978,11 @@
           <t>SRG-OS-000383-GPOS-00166</t>
         </is>
       </c>
-      <c r="D177" s="2" t="inlineStr"/>
+      <c r="D177" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87996-5</t>
+        </is>
+      </c>
       <c r="E177" s="2" t="inlineStr">
         <is>
           <t>The operating system must prohibit the use of cached authenticators after one day.</t>
@@ -12642,7 +12990,7 @@
       </c>
       <c r="F177" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prohibit the use of cached authenticators after one day.</t>
+          <t>Red Hat Enterprise Linux 9 must prohibit the use of cached authenticators after one day.</t>
         </is>
       </c>
       <c r="G177" s="2" t="inlineStr">
@@ -12710,7 +13058,7 @@
       </c>
       <c r="F178" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account modifications.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account modifications.</t>
         </is>
       </c>
       <c r="G178" s="2" t="inlineStr">
@@ -12822,7 +13170,7 @@
       </c>
       <c r="F180" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for all account creations, modifications, disabling, and termination events.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for all account creations, modifications, disabling, and termination events.</t>
         </is>
       </c>
       <c r="G180" s="2" t="inlineStr">
@@ -12870,7 +13218,11 @@
           <t>SRG-OS-000480-GPOS-00227,SRG-OS-000134-GPOS-00068</t>
         </is>
       </c>
-      <c r="D181" s="2" t="inlineStr"/>
+      <c r="D181" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83842-5</t>
+        </is>
+      </c>
       <c r="E181" s="2" t="inlineStr">
         <is>
           <t>The operating system must isolate security functions from nonsecurity functions.</t>
@@ -13113,7 +13465,11 @@
           <t>SRG-OS-000480-GPOS-00229</t>
         </is>
       </c>
-      <c r="D184" s="2" t="inlineStr"/>
+      <c r="D184" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90816-0</t>
+        </is>
+      </c>
       <c r="E184" s="2" t="inlineStr">
         <is>
           <t>The operating system must not allow an unattended or automatic logon to the system.</t>
@@ -13187,7 +13543,11 @@
           <t>SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D185" s="2" t="inlineStr"/>
+      <c r="D185" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84232-8</t>
+        </is>
+      </c>
       <c r="E185" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
@@ -13195,7 +13555,7 @@
       </c>
       <c r="F185" s="2" t="inlineStr">
         <is>
-          <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
+          <t>Red Hat Enterprise Linux 9 must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
       <c r="G185" s="2" t="inlineStr">
@@ -13360,7 +13720,7 @@
       </c>
       <c r="F187" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce a minimum 15-character password length.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce a minimum 15-character password length.</t>
         </is>
       </c>
       <c r="G187" s="2" t="inlineStr">
@@ -13487,7 +13847,7 @@
       </c>
       <c r="F189" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit the enforcement actions used to restrict access associated with changes to the system.</t>
+          <t>Red Hat Enterprise Linux 9 must audit the enforcement actions used to restrict access associated with changes to the system.</t>
         </is>
       </c>
       <c r="G189" s="2" t="inlineStr">
@@ -13543,7 +13903,7 @@
       </c>
       <c r="F190" s="2" t="inlineStr">
         <is>
-          <t>The operating system must notify designated personnel if baseline configurations are changed in an unauthorized manner.</t>
+          <t>Red Hat Enterprise Linux 9 must notify designated personnel if baseline configurations are changed in an unauthorized manner.</t>
         </is>
       </c>
       <c r="G190" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@6ee48f01e75473283b8e7995f338d94976aa4ef7 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -724,7 +724,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-7 a,AC-6 (8),CM-5 (1),AU-12 (3),AC-6 (9),AU-8 b</t>
+          <t>AC-6 (9),CM-5 (1),AU-12 (3),AU-7 a,AC-6 (8),AU-8 b,AU-7 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1175,7 +1175,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1335,7 +1335,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1558,7 +1558,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-8,AU-3 (1)</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1712,7 +1712,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1843,7 +1843,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1999,7 +1999,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 e,SC-10,MA-4 (7)</t>
+          <t>MA-4 e,AC-12,SC-10,MA-4 (7)</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2074,7 +2074,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-12 a,CM-5 (1),AU-7 (1),CM-6 b,AU-3,AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-6 (4)</t>
+          <t>AU-3 (1),CM-6 b,AU-3,AU-7 (1),CM-5 (1),AU-12 a,AU-7 a,MA-4 (1) (a),AU-6 (4),AU-14 (1)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2311,7 +2311,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2585,7 +2585,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2714,7 +2714,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2926,7 +2926,7 @@
     <row r="34" ht="130" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -3210,7 +3210,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3282,7 +3282,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -4498,7 +4498,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -5296,7 +5296,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5426,7 +5426,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-7 a,AU-12 a,CM-5 (1),CM-6 b,AU-12 (3),AU-12 c,AU-8 b</t>
+          <t>CM-6 b,CM-5 (1),AU-12 (3),AU-12 a,AU-12 c,AU-7 a,AU-8 b,AU-7 b</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5983,7 +5983,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6156,7 +6156,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6231,7 +6231,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (3),IA-2 (4)</t>
+          <t>IA-2 (1),IA-2 (3),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6318,7 +6318,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6655,7 +6655,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6809,7 +6809,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1),AC-2 (4),AC-6 (9)</t>
+          <t>AC-2 (4),AC-6 (9),CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6876,7 +6876,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (2),IA-2 (3),IA-2 (5),IA-2 (4)</t>
+          <t>IA-2 (2),IA-2,IA-2 (4),IA-2 (5),IA-2 (3)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7040,7 +7040,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7426,7 +7426,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),AC-18 (1),SC-8</t>
+          <t>SC-8,AC-18 (1),SC-8 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7506,7 +7506,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7815,7 +7815,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -7889,7 +7889,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -9033,7 +9033,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9331,7 +9331,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9405,7 +9405,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9479,7 +9479,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9668,7 +9668,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10471,7 +10471,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d,SI-6 b</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11125,7 +11125,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-14 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-14 (1)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11694,7 +11694,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@e732c1ecc2c95634f4fbfa0e13dffc08a5de7b9b 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),CM-5 (1),AU-12 (3),AU-7 a,AC-6 (8),AU-8 b,AU-7 b</t>
+          <t>AC-6 (9),AC-6 (8),AU-12 (3),AU-7 a,CM-5 (1),AU-7 b,AU-8 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>AC-17 (1),AC-17 (9),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1175,7 +1175,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1335,7 +1335,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1558,7 +1558,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1636,7 +1636,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1712,7 +1712,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1843,7 +1843,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1999,7 +1999,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,AC-12,SC-10,MA-4 (7)</t>
+          <t>AC-12,MA-4 (7),SC-10,MA-4 e</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2074,7 +2074,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),CM-6 b,AU-3,AU-7 (1),CM-5 (1),AU-12 a,AU-7 a,MA-4 (1) (a),AU-6 (4),AU-14 (1)</t>
+          <t>AU-12 a,AU-14 (1),AU-3,AU-7 (1),AU-7 a,MA-4 (1) (a),AU-6 (4),CM-6 b,CM-5 (1),AU-3 (1)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2311,7 +2311,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2585,7 +2585,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2714,7 +2714,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -3210,7 +3210,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3282,7 +3282,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3719,7 +3719,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a,AC-8 b</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 b,AC-8 a</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4282,7 +4282,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4423,7 +4423,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4997,7 +4997,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5152,7 +5152,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5296,7 +5296,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5426,7 +5426,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1),AU-12 (3),AU-12 a,AU-12 c,AU-7 a,AU-8 b,AU-7 b</t>
+          <t>AU-12 a,AU-12 (3),AU-12 c,AU-7 a,CM-6 b,CM-5 (1),AU-7 b,AU-8 b</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5584,7 +5584,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5983,7 +5983,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6231,7 +6231,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (3),IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (1),IA-2 (4)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6318,7 +6318,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6655,7 +6655,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6809,7 +6809,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),CM-5 (1),AU-12 c</t>
+          <t>CM-5 (1),AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6876,7 +6876,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2,IA-2 (4),IA-2 (5),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2,IA-2 (3),IA-2 (5),IA-2 (4)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6960,7 +6960,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7426,7 +7426,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7889,7 +7889,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8483,7 +8483,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9033,7 +9033,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9405,7 +9405,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9668,7 +9668,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10246,7 +10246,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10471,7 +10471,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11125,7 +11125,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-14 (1)</t>
+          <t>AU-12 a,AU-14 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11694,7 +11694,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11830,7 +11830,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -13205,7 +13205,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@9f8d6335b3c0c9dabcefd6f74d9e51f2920dac25 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-6 (8),AU-12 (3),AU-7 a,CM-5 (1),AU-7 b,AU-8 b</t>
+          <t>AU-7 a,AC-6 (8),AU-7 b,AU-12 (3),CM-5 (1),AC-6 (9),AU-8 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),AC-17 (9),CM-7 b,CM-6 b</t>
+          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1175,7 +1175,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1712,7 +1712,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1843,7 +1843,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -2074,7 +2074,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-14 (1),AU-3,AU-7 (1),AU-7 a,MA-4 (1) (a),AU-6 (4),CM-6 b,CM-5 (1),AU-3 (1)</t>
+          <t>AU-7 a,AU-3 (1),CM-6 b,AU-6 (4),CM-5 (1),AU-7 (1),MA-4 (1) (a),AU-14 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2311,7 +2311,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2585,7 +2585,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2714,7 +2714,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -3210,7 +3210,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3485,7 +3485,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -3719,7 +3719,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 b,AC-8 a</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a,AC-8 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4066,7 +4066,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4282,7 +4282,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4423,7 +4423,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4498,7 +4498,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4997,7 +4997,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5296,7 +5296,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5426,7 +5426,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 (3),AU-12 c,AU-7 a,CM-6 b,CM-5 (1),AU-7 b,AU-8 b</t>
+          <t>AU-12 c,AU-7 a,CM-6 b,AU-12 (3),AU-7 b,CM-5 (1),AU-8 b,AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5983,7 +5983,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6231,7 +6231,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2 (1),IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (1),IA-2 (3),IA-2 (4)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6655,7 +6655,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6809,7 +6809,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AU-12 c,CM-5 (1),AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6876,7 +6876,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2,IA-2 (3),IA-2 (5),IA-2 (4)</t>
+          <t>IA-2 (5),IA-2 (3),IA-2 (4),IA-2,IA-2 (2)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7426,7 +7426,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7506,7 +7506,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7889,7 +7889,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8483,7 +8483,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9033,7 +9033,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9331,7 +9331,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9405,7 +9405,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9479,7 +9479,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9668,7 +9668,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -11125,7 +11125,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-14 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11694,7 +11694,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11830,7 +11830,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -12825,7 +12825,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@d584dbfa36a12c71e89dc73fd2aaa5ab3e6bf4f9 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-12 (3),AU-7 a,CM-5 (1),AC-6 (9),AC-6 (8),AU-7 b</t>
+          <t>AU-7 a,AU-12 (3),AU-8 b,AC-6 (8),CM-5 (1),AC-6 (9),AU-7 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-12 (3),AU-7 a,CM-5 (1),CM-6 b,AU-12 a,AU-7 b,AU-12 c</t>
+          <t>CM-6 b,AU-7 a,AU-12 (3),AU-8 b,AU-12 c,CM-5 (1),AU-7 b,AU-12 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>CM-6 b,AC-17 (1),AC-17 (9),CM-7 b</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -3286,7 +3286,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3455,7 +3455,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3527,7 +3527,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>IA-8,AU-3 (1),IA-2</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6869,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-14 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9263,7 +9263,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9849,7 +9849,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),CM-5 (1),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),CM-5 (1),AC-6 (9)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>MA-4 c,SC-8,AC-17 (2),SC-13</t>
+          <t>SC-8,MA-4 c,SC-13,AC-17 (2)</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 (7),SC-10,MA-4 e</t>
+          <t>MA-4 (7),SC-10,AC-12,MA-4 e</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10822,7 +10822,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10901,7 +10901,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-6 (4),AU-3 (1),AU-7 a,CM-5 (1),CM-6 b,AU-12 a,AU-3,AU-7 (1),MA-4 (1) (a)</t>
+          <t>CM-6 b,AU-7 a,AU-6 (4),AU-14 (1),MA-4 (1) (a),AU-3,AU-7 (1),AU-3 (1),CM-5 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11304,7 +11304,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11380,7 +11380,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -11456,7 +11456,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11525,7 +11525,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11594,7 +11594,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11664,7 +11664,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11733,7 +11733,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11802,7 +11802,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11872,7 +11872,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11941,7 +11941,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12010,7 +12010,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12080,7 +12080,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12149,7 +12149,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12218,7 +12218,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12287,7 +12287,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13125,7 +13125,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13507,7 +13507,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -14333,7 +14333,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14412,7 +14412,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14484,7 +14484,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14556,7 +14556,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14630,7 +14630,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14704,7 +14704,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14778,7 +14778,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15299,7 +15299,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15733,7 +15733,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16642,7 +16642,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16744,7 +16744,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16854,7 +16854,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -16965,7 +16965,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17453,7 +17453,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (5),IA-2 (3),IA-2</t>
+          <t>IA-2 (5),IA-2 (2),IA-2 (4),IA-2,IA-2 (3)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17538,7 +17538,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (5),IA-2 (3),IA-2</t>
+          <t>IA-2 (5),IA-2 (2),IA-2 (4),IA-2,IA-2 (3)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17623,7 +17623,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17873,7 +17873,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17949,7 +17949,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18034,7 +18034,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18191,7 +18191,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18354,7 +18354,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19026,7 +19026,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19097,7 +19097,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19259,7 +19259,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-2,CM-6 b</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -20333,7 +20333,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20408,7 +20408,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20496,7 +20496,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20573,7 +20573,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -21171,7 +21171,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21258,7 +21258,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (1),IA-2 (3),IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (1),IA-2 (4)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21427,7 +21427,7 @@
     <row r="272" ht="130" customHeight="1">
       <c r="A272" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B272" s="2" t="inlineStr">
@@ -21645,7 +21645,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -23544,7 +23544,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24366,7 +24366,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -26934,7 +26934,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27008,7 +27008,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27168,7 +27168,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27245,7 +27245,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28810,7 +28810,7 @@
     <row r="366" ht="130" customHeight="1">
       <c r="A366" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B366" s="2" t="inlineStr">
@@ -29350,7 +29350,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29421,7 +29421,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29493,7 +29493,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30253,7 +30253,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -30701,7 +30701,7 @@
     <row r="390" ht="130" customHeight="1">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
@@ -31267,7 +31267,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -31508,7 +31508,7 @@
     <row r="400" ht="130" customHeight="1">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
@@ -31599,7 +31599,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31693,7 +31693,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@f51f214bcb5daa09384e0c47b17c32fb0b021447 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-12 (3),AU-8 b,AC-6 (8),CM-5 (1),AC-6 (9),AU-7 b</t>
+          <t>AU-7 a,AC-6 (8),AU-12 (3),CM-5 (1),AU-8 b,AU-7 b,AC-6 (9)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-7 a,AU-12 (3),AU-8 b,AU-12 c,CM-5 (1),AU-7 b,AU-12 a</t>
+          <t>CM-5 (1),AU-7 a,AU-12 (3),AU-12 a,AU-8 b,AU-7 b,AU-12 c,CM-6 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),AC-17 (9),CM-7 b</t>
+          <t>AC-17 (1),AC-17 (9),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1257,7 +1257,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1334,7 +1334,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1484,7 +1484,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1560,7 +1560,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-8,AU-3 (1),IA-2</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6869,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-14 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9096,7 +9096,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9177,7 +9177,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9263,7 +9263,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9341,7 +9341,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9849,7 +9849,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),CM-5 (1),AC-6 (9)</t>
+          <t>AC-6 (9),CM-5 (1),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-8,MA-4 c,SC-13,AC-17 (2)</t>
+          <t>MA-4 c,SC-13,SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),SC-10,AC-12,MA-4 e</t>
+          <t>AC-12,MA-4 (7),SC-10,MA-4 e</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10822,7 +10822,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10901,7 +10901,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10977,7 +10977,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-7 a,AU-6 (4),AU-14 (1),MA-4 (1) (a),AU-3,AU-7 (1),AU-3 (1),CM-5 (1),AU-12 a</t>
+          <t>AU-3,AU-7 a,CM-5 (1),AU-12 a,AU-3 (1),AU-14 (1),MA-4 (1) (a),AU-7 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11456,7 +11456,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11525,7 +11525,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11594,7 +11594,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11664,7 +11664,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11733,7 +11733,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11802,7 +11802,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11872,7 +11872,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11941,7 +11941,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12010,7 +12010,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12080,7 +12080,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12149,7 +12149,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12218,7 +12218,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12287,7 +12287,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13125,7 +13125,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13357,7 +13357,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13507,7 +13507,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13721,7 +13721,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -14262,7 +14262,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14333,7 +14333,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -15299,7 +15299,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15733,7 +15733,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16248,7 +16248,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -17453,7 +17453,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2 (4),IA-2,IA-2 (3)</t>
+          <t>IA-2 (5),IA-2 (3),IA-2 (4),IA-2 (2),IA-2</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17538,7 +17538,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2 (4),IA-2,IA-2 (3)</t>
+          <t>IA-2 (5),IA-2 (3),IA-2 (4),IA-2 (2),IA-2</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17623,7 +17623,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17790,7 +17790,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -17873,7 +17873,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17949,7 +17949,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18034,7 +18034,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18191,7 +18191,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18270,7 +18270,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18354,7 +18354,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -18429,7 +18429,7 @@
     <row r="233" ht="130" customHeight="1">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B233" s="2" t="inlineStr">
@@ -19026,7 +19026,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19097,7 +19097,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19259,7 +19259,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -21171,7 +21171,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21258,7 +21258,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2 (1),IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21427,7 +21427,7 @@
     <row r="272" ht="130" customHeight="1">
       <c r="A272" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B272" s="2" t="inlineStr">
@@ -21645,7 +21645,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -21726,7 +21726,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21814,7 +21814,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22052,7 +22052,7 @@
     <row r="280" ht="130" customHeight="1">
       <c r="A280" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B280" s="2" t="inlineStr">
@@ -23375,7 +23375,7 @@
     <row r="297" ht="130" customHeight="1">
       <c r="A297" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B297" s="2" t="inlineStr">
@@ -23544,7 +23544,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24366,7 +24366,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25783,7 +25783,7 @@
     <row r="327" ht="130" customHeight="1">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B327" s="2" t="inlineStr">
@@ -26859,7 +26859,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -27168,7 +27168,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27245,7 +27245,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28090,7 +28090,7 @@
     <row r="357" ht="130" customHeight="1">
       <c r="A357" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B357" s="2" t="inlineStr">
@@ -28339,7 +28339,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28430,7 +28430,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28810,7 +28810,7 @@
     <row r="366" ht="130" customHeight="1">
       <c r="A366" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B366" s="2" t="inlineStr">
@@ -30253,7 +30253,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -30701,7 +30701,7 @@
     <row r="390" ht="130" customHeight="1">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
@@ -31267,7 +31267,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -31508,7 +31508,7 @@
     <row r="400" ht="130" customHeight="1">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
@@ -31599,7 +31599,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31693,7 +31693,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -35253,7 +35253,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35326,7 +35326,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -41137,7 +41137,7 @@
     <row r="523" ht="130" customHeight="1">
       <c r="A523" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B523" s="2" t="inlineStr">
@@ -41224,7 +41224,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -42456,7 +42456,7 @@
     <row r="540" ht="130" customHeight="1">
       <c r="A540" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B540" s="2" t="inlineStr">
@@ -43103,7 +43103,7 @@
     <row r="549" ht="130" customHeight="1">
       <c r="A549" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B549" s="2" t="inlineStr">
@@ -43535,12 +43535,18 @@
         <is>
           <t>To check how many characters are required in a password, run the following command:
  $ grep minlen /etc/security/pwquality.conf 
-Your output should contain  minlen =  
+Your output should contain  minlen = 15 
 If minlen is not found, or not equal to or greater than the required value then this is a finding.</t>
         </is>
       </c>
       <c r="L554" s="2" t="n"/>
-      <c r="M554" s="2" t="inlineStr"/>
+      <c r="M554" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to enforce a minimum 15-character password length.
+Add the following line to "/etc/security/pwquality.conf" (or modify the line to have the required value):
+minlen = 15</t>
+        </is>
+      </c>
       <c r="N554" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -43615,7 +43621,13 @@
         </is>
       </c>
       <c r="L555" s="2" t="n"/>
-      <c r="M555" s="2" t="inlineStr"/>
+      <c r="M555" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to enforce a minimum 15-character password length for new user accounts.
+Add, or modify the following line in the "/etc/login.defs" file:
+PASS_MIN_LEN 15</t>
+        </is>
+      </c>
       <c r="N555" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@8e3f9b14c7fb366fb7b45878ba15b4606c5b8fea 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-5 (1),AU-8 b,AC-6 (8),AC-6 (9),AU-7 b,AU-12 (3)</t>
+          <t>AC-6 (8),AU-7 a,AU-7 b,CM-5 (1),AU-8 b,AU-12 (3),AC-6 (9)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-5 (1),AU-8 b,AU-12 c,CM-6 b,AU-7 b,AU-12 (3),AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-7 a,AU-7 b,CM-5 (1),AU-8 b,AU-12 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (9),CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1714,7 +1714,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2084,7 +2084,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2158,7 +2158,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3286,7 +3286,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3455,7 +3455,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3527,7 +3527,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6869,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AC-2 (4),AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-14 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-14 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9096,7 +9096,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9177,7 +9177,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9341,7 +9341,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9849,7 +9849,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (9),AC-2 (4),AU-12 c</t>
+          <t>CM-5 (1),AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),MA-4 c,SC-13</t>
+          <t>SC-13,AC-17 (2),SC-8,MA-4 c</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>SC-10,MA-4 (7),MA-4 e,AC-12</t>
+          <t>MA-4 (7),MA-4 e,SC-10,AC-12</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10977,7 +10977,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-5 (1),AU-12 a,AU-3,CM-6 b,AU-14 (1),MA-4 (1) (a),AU-6 (4),AU-7 (1),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-6 (4),AU-7 (1),AU-12 a,AU-3 (1),AU-7 a,AU-3,CM-5 (1),AU-14 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -13125,7 +13125,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13278,7 +13278,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13357,7 +13357,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13432,7 +13432,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13581,7 +13581,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13659,7 +13659,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13742,7 +13742,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14122,7 +14122,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14193,7 +14193,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -15593,7 +15593,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16108,7 +16108,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16188,7 +16188,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16502,7 +16502,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16604,7 +16604,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16714,7 +16714,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16825,7 +16825,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -16934,7 +16934,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17376,7 +17376,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17454,7 +17454,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2,IA-2 (5),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2,IA-2 (5),IA-2 (4)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17539,7 +17539,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2,IA-2 (5),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2,IA-2 (5),IA-2 (4)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17624,7 +17624,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17791,7 +17791,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -17874,7 +17874,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17950,7 +17950,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18035,7 +18035,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -19260,7 +19260,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19420,7 +19420,7 @@
     <row r="246" ht="130" customHeight="1">
       <c r="A246" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B246" s="2" t="inlineStr">
@@ -20334,7 +20334,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20409,7 +20409,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20497,7 +20497,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20574,7 +20574,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -21172,7 +21172,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21259,7 +21259,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2 (1),IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (1),IA-2 (4)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21646,7 +21646,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -22276,7 +22276,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -23456,7 +23456,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23545,7 +23545,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24367,7 +24367,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25941,7 +25941,7 @@
     <row r="329" ht="130" customHeight="1">
       <c r="A329" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B329" s="2" t="inlineStr">
@@ -26860,7 +26860,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -27083,7 +27083,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
@@ -27169,7 +27169,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27246,7 +27246,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28091,7 +28091,7 @@
     <row r="357" ht="130" customHeight="1">
       <c r="A357" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B357" s="2" t="inlineStr">
@@ -28340,7 +28340,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 b,SI-6 d</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28431,7 +28431,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -30254,7 +30254,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -30563,7 +30563,7 @@
     <row r="388" ht="130" customHeight="1">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
@@ -30702,7 +30702,7 @@
     <row r="390" ht="130" customHeight="1">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
@@ -31184,7 +31184,7 @@
     <row r="396" ht="130" customHeight="1">
       <c r="A396" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B396" s="2" t="inlineStr">
@@ -31268,7 +31268,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -31509,7 +31509,7 @@
     <row r="400" ht="130" customHeight="1">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
@@ -31600,7 +31600,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31694,7 +31694,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -35104,7 +35104,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
@@ -35254,7 +35254,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35327,7 +35327,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -41138,7 +41138,7 @@
     <row r="523" ht="130" customHeight="1">
       <c r="A523" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B523" s="2" t="inlineStr">
@@ -41225,7 +41225,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -42457,7 +42457,7 @@
     <row r="540" ht="130" customHeight="1">
       <c r="A540" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B540" s="2" t="inlineStr">
@@ -43104,7 +43104,7 @@
     <row r="549" ht="130" customHeight="1">
       <c r="A549" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B549" s="2" t="inlineStr">
@@ -43712,7 +43712,7 @@
     <row r="557" ht="130" customHeight="1">
       <c r="A557" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B557" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@1ce120b5203c36034ee6236a67033a9b117b9cc4 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8),AU-12 (3),CM-5 (1),AC-6 (9),AU-7 b,AU-8 b,AU-7 a</t>
+          <t>CM-5 (1),AC-6 (8),AU-8 b,AU-7 b,AU-7 a,AU-12 (3),AC-6 (9)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -893,7 +893,7 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>SRG-OS-000326-GPOS-00126,SRG-OS-000327-GPOS-00127,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000359-GPOS-00146,SRG-OS-000365-GPOS-00152</t>
+          <t>SRG-OS-000326-GPOS-00126,SRG-OS-000327-GPOS-00127,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000365-GPOS-00152</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),CM-5 (1),CM-6 b,AU-7 b,AU-12 c,AU-8 b,AU-12 a,AU-7 a</t>
+          <t>CM-6 b,AU-12 c,CM-5 (1),AU-8 b,AU-7 b,AU-7 a,AU-12 (3),AU-12 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1015,7 +1015,7 @@
       <c r="K7" s="2" t="inlineStr">
         <is>
           <t>Run the following command to determine if the  audit  package is installed:  $ rpm -q audit 
-If the package is not installed then this is a finding.</t>
+If the audit package is not installed then this is a finding.</t>
         </is>
       </c>
       <c r="L7" s="2" t="n"/>
@@ -1496,7 +1496,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1572,7 +1572,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1726,7 +1726,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2096,7 +2096,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2170,7 +2170,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3298,7 +3298,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3382,7 +3382,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3467,7 +3467,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3539,7 +3539,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3997,7 +3997,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4072,7 +4072,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4147,7 +4147,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4297,7 +4297,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4447,7 +4447,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4597,7 +4597,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4897,7 +4897,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4977,7 +4977,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5140,7 +5140,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5220,7 +5220,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5300,7 +5300,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5454,7 +5454,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5528,7 +5528,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6115,7 +6115,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6188,7 +6188,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6262,7 +6262,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6336,7 +6336,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6410,7 +6410,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6468,7 +6468,14 @@
         </is>
       </c>
       <c r="L79" s="2" t="n"/>
-      <c r="M79" s="2" t="inlineStr"/>
+      <c r="M79" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to generate audit records for all account creations, modifications, disabling, and termination events that affect  /var/log/lastlog .
+Add or update the following file system rule to  /etc/audit/rules.d/audit.rules :
+-w /var/log/lastlog -p wa -k logins
+The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
       <c r="N79" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -6481,7 +6488,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6561,7 +6568,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6641,7 +6648,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6721,7 +6728,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6801,7 +6808,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6881,7 +6888,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6961,7 +6968,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7041,7 +7048,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7121,7 +7128,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7201,7 +7208,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7281,7 +7288,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7361,7 +7368,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7437,7 +7444,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7514,7 +7521,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7594,7 +7601,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7674,7 +7681,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7754,7 +7761,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7834,7 +7841,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7914,7 +7921,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7994,7 +8001,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8074,7 +8081,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8154,7 +8161,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8234,7 +8241,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8307,7 +8314,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8388,7 +8395,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8469,7 +8476,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8540,7 +8547,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8615,7 +8622,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8697,7 +8704,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8779,7 +8786,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8861,7 +8868,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8943,7 +8950,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9025,7 +9032,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-14 (1),AU-12 c,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9095,7 +9102,16 @@
         </is>
       </c>
       <c r="L112" s="2" t="n"/>
-      <c r="M112" s="2" t="inlineStr"/>
+      <c r="M112" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To ensure that  audit=1  is added as a kernel command line
+argument to newly installed kernels, add  audit=1  to the
+default Grub2 command line for Linux operating systems.  Modify the line within
+ /etc/default/grub  as shown below:
+ GRUB_CMDLINE_LINUX="... audit=1 ..." 
+Run the following command to update command line for already installed kernels: # grubby --update-kernel=ALL --args="audit=1" </t>
+        </is>
+      </c>
       <c r="N112" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -9108,7 +9124,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9189,7 +9205,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9275,7 +9291,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9353,7 +9369,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9719,7 +9735,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9790,7 +9806,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10234,7 +10250,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),CM-5 (1),AU-12 c</t>
+          <t>CM-5 (1),AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10677,7 +10693,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-13,AC-17 (2),MA-4 c</t>
+          <t>SC-8,AC-17 (2),MA-4 c,SC-13</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10759,7 +10775,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),MA-4 e,SC-10,AC-12</t>
+          <t>MA-4 (7),MA-4 e,AC-12,SC-10</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11066,7 +11082,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b,AU-3,AU-6 (4),MA-4 (1) (a),AU-14 (1),AU-3 (1),AU-12 a,AU-7 a,AU-7 (1)</t>
+          <t>AU-3,AU-6 (4),AU-7 (1),CM-6 b,AU-14 (1),AU-3 (1),CM-5 (1),MA-4 (1) (a),AU-7 a,AU-12 a</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11316,7 +11332,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11392,7 +11408,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -11468,7 +11484,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11537,7 +11553,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11606,7 +11622,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11676,7 +11692,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11745,7 +11761,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11814,7 +11830,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11884,7 +11900,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11953,7 +11969,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12022,7 +12038,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12092,7 +12108,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12161,7 +12177,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12230,7 +12246,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12299,7 +12315,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13137,7 +13153,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -14134,7 +14150,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14205,7 +14221,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (9),AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14282,7 +14298,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14361,7 +14377,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14433,7 +14449,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14505,7 +14521,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14579,7 +14595,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14653,7 +14669,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14727,7 +14743,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15248,7 +15264,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -16197,7 +16213,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -17023,7 +17039,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17465,7 +17481,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17543,7 +17559,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2,IA-2 (3),IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (5),IA-2,IA-2 (4),IA-2 (2),IA-2 (3)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17628,7 +17644,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2,IA-2 (3),IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (5),IA-2,IA-2 (4),IA-2 (2),IA-2 (3)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17713,7 +17729,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17963,7 +17979,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18039,7 +18055,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18124,7 +18140,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -18360,7 +18376,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -18444,7 +18460,7 @@
     <row r="233" ht="130" customHeight="1">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B233" s="2" t="inlineStr">
@@ -18519,7 +18535,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19116,7 +19132,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19170,11 +19186,18 @@
         <is>
           <t>To verify that auditing is configured for system administrator actions, run the following command:
  $ sudo auditctl -l | grep "watch=/var/run/faillock\|-w /var/run/faillock" 
-If there is not output then this is a finding.</t>
+If there is no output then this is a finding.</t>
         </is>
       </c>
       <c r="L242" s="2" t="n"/>
-      <c r="M242" s="2" t="inlineStr"/>
+      <c r="M242" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to generate audit records for all account creations, modifications, disabling, and termination events that affect  /var/run/faillock .
+Add or update the following file system rule to  /etc/audit/rules.d/audit.rules :
+-w /var/run/faillock -p wa -k logins
+The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
       <c r="N242" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -19187,7 +19210,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19245,7 +19268,14 @@
         </is>
       </c>
       <c r="L243" s="2" t="n"/>
-      <c r="M243" s="2" t="inlineStr"/>
+      <c r="M243" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to generate audit records for all account creations, modifications, disabling, and termination events that affect  /var/log/tallylog .
+Add or update the following file system rule to  /etc/audit/rules.d/audit.rules :
+-w /var/log/tallylog -p wa -k logins
+The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
       <c r="N243" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -19349,7 +19379,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -21348,7 +21378,7 @@
     <row r="271" ht="130" customHeight="1">
       <c r="A271" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (1),IA-2 (4)</t>
         </is>
       </c>
       <c r="B271" s="2" t="inlineStr">
@@ -21517,7 +21547,7 @@
     <row r="273" ht="130" customHeight="1">
       <c r="A273" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B273" s="2" t="inlineStr">
@@ -21735,7 +21765,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21816,7 +21846,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -21904,7 +21934,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -22142,7 +22172,7 @@
     <row r="281" ht="130" customHeight="1">
       <c r="A281" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B281" s="2" t="inlineStr">
@@ -22365,7 +22395,7 @@
     <row r="284" ht="130" customHeight="1">
       <c r="A284" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B284" s="2" t="inlineStr">
@@ -24456,7 +24486,7 @@
     <row r="310" ht="130" customHeight="1">
       <c r="A310" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B310" s="2" t="inlineStr">
@@ -26949,7 +26979,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27172,7 +27202,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27335,7 +27365,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28180,7 +28210,7 @@
     <row r="358" ht="130" customHeight="1">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
@@ -28429,7 +28459,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d,SI-6 b</t>
+          <t>CM-3 (5),SI-6 b,SI-6 d</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28497,7 +28527,7 @@
 The output should return something similar to the following:
  05 4 * * * root  --check 
 NOTE: The usage of special cron times, such as @daily or @weekly, is acceptable.
-If AIDE is not configured to periodicly scan then this is a finding.</t>
+If AIDE is not configured to scan periodically then this is a finding.</t>
         </is>
       </c>
       <c r="L361" s="2" t="n"/>
@@ -28520,7 +28550,7 @@
     <row r="362" ht="130" customHeight="1">
       <c r="A362" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B362" s="2" t="inlineStr">
@@ -28971,7 +29001,16 @@
         </is>
       </c>
       <c r="L367" s="2" t="n"/>
-      <c r="M367" s="2" t="inlineStr"/>
+      <c r="M367" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To ensure that  pti=on  is added as a kernel command line
+argument to newly installed kernels, add  pti=on  to the
+default Grub2 command line for Linux operating systems.  Modify the line within
+ /etc/default/grub  as shown below:
+ GRUB_CMDLINE_LINUX="... pti=on ..." 
+Run the following command to update command line for already installed kernels: # grubby --update-kernel=ALL --args="pti=on" </t>
+        </is>
+      </c>
       <c r="N367" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -29440,7 +29479,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29511,7 +29550,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -29583,7 +29622,7 @@
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
@@ -30343,7 +30382,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -30791,7 +30830,7 @@
     <row r="391" ht="130" customHeight="1">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
@@ -31357,7 +31396,7 @@
     <row r="398" ht="130" customHeight="1">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
@@ -31435,7 +31474,14 @@
         </is>
       </c>
       <c r="L398" s="2" t="n"/>
-      <c r="M398" s="2" t="inlineStr"/>
+      <c r="M398" s="2" t="inlineStr">
+        <is>
+          <t>Add or edit the following line in a system configuration file in the "/etc/sysctl.d/" directory:
+kernel.randomize_va_space = 2
+Load settings from all system configuration files with the following command:
+$ sudo sysctl --system</t>
+        </is>
+      </c>
       <c r="N398" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -31473,7 +31519,7 @@
       </c>
       <c r="F399" s="2" t="inlineStr">
         <is>
-          <t>Red Hat Enterprise Linux 9 must, for networked systems, compare internal information system clocks at least every 24 hours with a server which is synchronized to one of the redundant United States Naval Observatory (USNO) time servers, or a time server designat</t>
+          <t>Red Hat Enterprise Linux 9 must, for networked systems, compare internal information system clocks at least every 24 hours with a server which is synchronized to one of the redundant United States Naval Observatory (USNO) time servers, or a time server designated for the appropriate DoD network (NIPRNet/SIPRNet), and/or the Global Positioning System (GPS).</t>
         </is>
       </c>
       <c r="G399" s="2" t="inlineStr">
@@ -31598,7 +31644,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31689,7 +31735,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31783,7 +31829,7 @@
     <row r="403" ht="130" customHeight="1">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
@@ -35193,7 +35239,7 @@
     <row r="448" ht="130" customHeight="1">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
@@ -35343,7 +35389,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -35416,7 +35462,7 @@
     <row r="451" ht="130" customHeight="1">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
@@ -41227,7 +41273,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -41314,7 +41360,7 @@
     <row r="525" ht="130" customHeight="1">
       <c r="A525" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B525" s="2" t="inlineStr">
@@ -42546,7 +42592,7 @@
     <row r="541" ht="130" customHeight="1">
       <c r="A541" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B541" s="2" t="inlineStr">
@@ -43193,7 +43239,7 @@
     <row r="550" ht="130" customHeight="1">
       <c r="A550" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B550" s="2" t="inlineStr">
@@ -43801,7 +43847,7 @@
     <row r="558" ht="130" customHeight="1">
       <c r="A558" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B558" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@9631ba0a461a015c3adc159bb9067ec946b6df1e 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-7 b,CM-5 (1),AU-12 (3),AU-12 a,AU-7 a,CM-6 b,AU-12 c</t>
+          <t>AU-7 b,AU-7 a,AU-12 a,AU-8 b,CM-6 b,AU-12 (3),AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -957,7 +957,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-3 (1),AU-7 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-14 (1),AU-7 a,CM-6 b,AU-6 (4)</t>
+          <t>AU-7 (1),AU-7 a,AU-12 a,CM-6 b,AU-6 (4),AU-3,MA-4 (1) (a),AU-3 (1),CM-5 (1),AU-14 (1)</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -3772,7 +3772,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3850,7 +3850,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3925,7 +3925,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4000,7 +4000,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4075,7 +4075,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4150,7 +4150,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4225,7 +4225,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4300,7 +4300,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4375,7 +4375,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4450,7 +4450,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4525,7 +4525,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4600,7 +4600,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4675,7 +4675,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4750,7 +4750,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4825,7 +4825,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4905,7 +4905,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4988,7 +4988,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5068,7 +5068,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5148,7 +5148,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5228,7 +5228,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5308,7 +5308,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5382,7 +5382,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5456,7 +5456,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5530,7 +5530,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5604,7 +5604,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5678,7 +5678,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5751,7 +5751,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5824,7 +5824,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5897,7 +5897,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5970,7 +5970,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6043,7 +6043,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6116,7 +6116,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6190,7 +6190,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6264,7 +6264,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6338,7 +6338,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6416,7 +6416,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6496,7 +6496,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6576,7 +6576,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6656,7 +6656,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6736,7 +6736,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6816,7 +6816,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6896,7 +6896,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6976,7 +6976,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7056,7 +7056,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7136,7 +7136,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7216,7 +7216,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7296,7 +7296,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7372,7 +7372,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7449,7 +7449,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7529,7 +7529,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7609,7 +7609,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7689,7 +7689,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7769,7 +7769,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7849,7 +7849,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7929,7 +7929,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8009,7 +8009,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8089,7 +8089,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8169,7 +8169,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8242,7 +8242,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AC-2 (4),AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8323,7 +8323,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AC-2 (4),AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8404,7 +8404,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AC-2 (4),AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8475,7 +8475,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c</t>
+          <t>AC-2 (4),AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8550,7 +8550,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AC-2 (4),AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8632,7 +8632,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AC-2 (4),AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8714,7 +8714,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AC-2 (4),AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8796,7 +8796,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AC-2 (4),AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8878,7 +8878,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AC-2 (4),AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8960,7 +8960,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-14 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-14 (1)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9052,7 +9052,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9133,7 +9133,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9219,7 +9219,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9297,7 +9297,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9663,7 +9663,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9734,7 +9734,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -10262,7 +10262,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>MA-4 c,SC-8,SC-13,AC-17 (2)</t>
+          <t>MA-4 c,SC-8,AC-17 (2),SC-13</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10344,7 +10344,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 (7),MA-4 e,SC-10</t>
+          <t>MA-4 (7),AC-12,MA-4 e,SC-10</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -12013,7 +12013,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12090,7 +12090,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12255,7 +12255,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -13027,7 +13027,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13098,7 +13098,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
+          <t>AC-17 (1),AC-17 (9),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13175,7 +13175,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -14160,7 +14160,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14594,7 +14594,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -15109,7 +15109,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15515,7 +15515,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15617,7 +15617,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15727,7 +15727,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -15947,7 +15947,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16389,7 +16389,7 @@
     <row r="205" ht="130" customHeight="1">
       <c r="A205" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B205" s="2" t="inlineStr">
@@ -16467,7 +16467,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (5),IA-2 (2),IA-2</t>
+          <t>IA-2 (3),IA-2,IA-2 (4),IA-2 (5),IA-2 (2)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16552,7 +16552,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (5),IA-2 (2),IA-2</t>
+          <t>IA-2 (3),IA-2,IA-2 (4),IA-2 (5),IA-2 (2)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16637,7 +16637,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16804,7 +16804,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17284,7 +17284,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17368,7 +17368,7 @@
     <row r="217" ht="130" customHeight="1">
       <c r="A217" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B217" s="2" t="inlineStr">
@@ -17443,7 +17443,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -18287,7 +18287,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-2,CM-6 b</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -18447,7 +18447,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -20199,7 +20199,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B254" s="2" t="inlineStr">
@@ -20286,7 +20286,7 @@
     <row r="255" ht="130" customHeight="1">
       <c r="A255" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (1),IA-2 (2)</t>
         </is>
       </c>
       <c r="B255" s="2" t="inlineStr">
@@ -20754,7 +20754,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -20842,7 +20842,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21907,7 +21907,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-7 b,CM-5 (1),AU-12 (3),AC-6 (8),AU-7 a,AC-6 (9)</t>
+          <t>AU-7 b,AU-7 a,AU-8 b,AC-6 (9),AU-12 (3),AC-6 (8),CM-5 (1)</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -23597,7 +23597,7 @@
     <row r="296" ht="130" customHeight="1">
       <c r="A296" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B296" s="2" t="inlineStr">
@@ -25004,7 +25004,7 @@
     <row r="314" ht="130" customHeight="1">
       <c r="A314" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B314" s="2" t="inlineStr">
@@ -25923,7 +25923,7 @@
     <row r="326" ht="130" customHeight="1">
       <c r="A326" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B326" s="2" t="inlineStr">
@@ -25998,7 +25998,7 @@
     <row r="327" ht="130" customHeight="1">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B327" s="2" t="inlineStr">
@@ -26072,7 +26072,7 @@
     <row r="328" ht="130" customHeight="1">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B328" s="2" t="inlineStr">
@@ -26146,7 +26146,7 @@
     <row r="329" ht="130" customHeight="1">
       <c r="A329" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B329" s="2" t="inlineStr">
@@ -27403,7 +27403,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27874,7 +27874,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -29635,7 +29635,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@31f9e4c68da837757dd0a221bfc3c7e803f2add6 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -710,7 +710,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -782,7 +782,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-7 (1),AU-3,MA-4 (1) (a),AU-7 a,AU-6 (4),CM-6 b,AU-14 (1),CM-5 (1),AU-3 (1),AU-12 a</t>
+          <t>AU-7 (1),AU-7 a,CM-6 b,MA-4 (1) (a),AU-14 (1),AU-6 (4),AU-3,AU-12 a,CM-5 (1),AU-3 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1761,7 +1761,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2131,7 +2131,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2205,7 +2205,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-14 (1),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-14 (1),AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3782,7 +3782,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4161,7 +4161,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
+          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4231,7 +4231,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4311,7 +4311,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
+          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4466,7 +4466,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4552,7 +4552,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4636,7 +4636,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 b,SI-6 d</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4728,7 +4728,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4812,7 +4812,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4887,7 +4887,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4962,7 +4962,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5037,7 +5037,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5112,7 +5112,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5187,7 +5187,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5262,7 +5262,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5337,7 +5337,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5412,7 +5412,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-12 (3),AU-7 a,CM-6 b,CM-5 (1),AU-12 a,AU-12 c,AU-8 b</t>
+          <t>AU-7 a,CM-6 b,AU-12 c,AU-7 b,AU-8 b,AU-12 a,CM-5 (1),AU-12 (3)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5561,7 +5561,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5642,7 +5642,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5723,7 +5723,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5805,7 +5805,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5887,7 +5887,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6051,7 +6051,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6133,7 +6133,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -7171,7 +7171,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7245,7 +7245,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7319,7 +7319,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7393,7 +7393,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7969,7 +7969,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8044,7 +8044,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8119,7 +8119,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8194,7 +8194,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8274,7 +8274,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8348,7 +8348,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8422,7 +8422,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8496,7 +8496,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8570,7 +8570,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8724,7 +8724,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8804,7 +8804,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8884,7 +8884,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9134,7 +9134,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9213,7 +9213,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9297,7 +9297,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9553,7 +9553,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 c,SC-13,SC-8</t>
+          <t>MA-4 c,AC-17 (2),SC-8,SC-13</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9635,7 +9635,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
@@ -9713,7 +9713,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9791,7 +9791,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9869,7 +9869,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9949,7 +9949,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10018,7 +10018,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10087,7 +10087,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -10156,7 +10156,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -10225,7 +10225,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10305,7 +10305,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11605,7 +11605,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11685,7 +11685,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11765,7 +11765,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11845,7 +11845,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12157,7 +12157,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12941,7 +12941,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B160" s="2" t="inlineStr">
@@ -13018,7 +13018,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B161" s="2" t="inlineStr">
@@ -13091,7 +13091,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -13164,7 +13164,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13249,7 +13249,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13324,7 +13324,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13399,7 +13399,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13474,7 +13474,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13549,7 +13549,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13620,7 +13620,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13691,7 +13691,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13763,7 +13763,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13834,7 +13834,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13905,7 +13905,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13977,7 +13977,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14052,7 +14052,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14123,7 +14123,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B176" s="2" t="inlineStr">
@@ -14194,7 +14194,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B177" s="2" t="inlineStr">
@@ -14266,7 +14266,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14341,7 +14341,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14423,7 +14423,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14587,7 +14587,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14669,7 +14669,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14751,7 +14751,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14833,7 +14833,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14915,7 +14915,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14997,7 +14997,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15079,7 +15079,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B188" s="2" t="inlineStr">
@@ -15157,7 +15157,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B189" s="2" t="inlineStr">
@@ -15236,7 +15236,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B190" s="2" t="inlineStr">
@@ -15318,7 +15318,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15400,7 +15400,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15482,7 +15482,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15564,7 +15564,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15646,7 +15646,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15728,7 +15728,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15803,7 +15803,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15876,7 +15876,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15953,7 +15953,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (1),IA-2 (4),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16040,7 +16040,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2,IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (5),IA-2 (4),IA-2 (3),IA-2 (2),IA-2</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16129,7 +16129,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2,IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (5),IA-2 (4),IA-2 (3),IA-2 (2),IA-2</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16274,12 +16274,18 @@
  $ sudo grep -i "FAIL_DELAY" /etc/login.defs 
 All output must show the value of "FAIL_DELAY" set as shown in the below:
  $ sudo grep -i "FAIL_DELAY" /etc/login.defs
-FAIL_DELAY  
+FAIL_DELAY 4 
 If the above command returns no output, or FAIL_DELAY is configured less than the expected value then this is a finding.</t>
         </is>
       </c>
       <c r="L202" s="2" t="n"/>
-      <c r="M202" s="2" t="inlineStr"/>
+      <c r="M202" s="2" t="inlineStr">
+        <is>
+          <t>Configure the Red Hat Enterprise Linux 9 to enforce a delay of at least 4 seconds between logon prompts following a failed console logon attempt.
+Modify the "/etc/login.defs" file to set the "FAIL_DELAY" parameter to 4 or greater:
+FAIL_DELAY 4</t>
+        </is>
+      </c>
       <c r="N202" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -16809,7 +16815,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16886,7 +16892,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16972,7 +16978,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>SC-8 (1),AC-18 (1),SC-8</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17132,7 +17138,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17986,7 +17992,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18166,7 +18172,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18258,7 +18264,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18356,7 +18362,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-8,AU-3 (1)</t>
+          <t>IA-8,AU-3 (1),IA-2</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19330,7 +19336,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b,SC-2</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19490,7 +19496,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20188,7 +20194,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -21012,7 +21018,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21101,7 +21107,7 @@
     <row r="263" ht="130" customHeight="1">
       <c r="A263" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B263" s="2" t="inlineStr">
@@ -21426,7 +21432,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -21508,7 +21514,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-7 b,AU-12 (3),AU-7 a,CM-5 (1),AC-6 (8),AU-8 b</t>
+          <t>AC-6 (8),AU-7 a,AC-6 (9),AU-7 b,AU-8 b,CM-5 (1),AU-12 (3)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -22700,7 +22706,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -23002,7 +23008,7 @@
     <row r="287" ht="130" customHeight="1">
       <c r="A287" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B287" s="2" t="inlineStr">
@@ -23076,7 +23082,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B288" s="2" t="inlineStr">
@@ -30967,7 +30973,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1),AC-17 (9)</t>
+          <t>CM-6 b,AC-17 (9),CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -31045,7 +31051,7 @@
     <row r="393" ht="130" customHeight="1">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
@@ -35361,7 +35367,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
@@ -37058,7 +37064,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),MA-4 e,AC-12,SC-10</t>
+          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
         </is>
       </c>
       <c r="B468" s="2" t="inlineStr">
@@ -37288,7 +37294,7 @@
     <row r="471" ht="130" customHeight="1">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
@@ -39890,7 +39896,7 @@
     <row r="505" ht="130" customHeight="1">
       <c r="A505" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B505" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@83ef3fa4544eeff8e505fa599d9e3e4713ed7876 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -710,7 +710,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -782,7 +782,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-7 (1),AU-7 a,CM-6 b,MA-4 (1) (a),AU-14 (1),AU-6 (4),AU-3,AU-12 a,CM-5 (1),AU-3 (1)</t>
+          <t>CM-5 (1),AU-3,AU-7 (1),AU-3 (1),CM-6 b,AU-6 (4),MA-4 (1) (a),AU-7 a,AU-12 a,AU-14 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1531,7 +1531,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1607,7 +1607,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-14 (1),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AU-14 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3782,7 +3782,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4161,7 +4161,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4231,7 +4231,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4311,7 +4311,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4552,7 +4552,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
+          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4636,7 +4636,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 b,SI-6 d</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4728,7 +4728,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4812,7 +4812,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4887,7 +4887,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4962,7 +4962,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5037,7 +5037,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5112,7 +5112,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5187,7 +5187,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5262,7 +5262,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5337,7 +5337,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5412,7 +5412,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-6 b,AU-12 c,AU-7 b,AU-8 b,AU-12 a,CM-5 (1),AU-12 (3)</t>
+          <t>CM-5 (1),AU-12 (3),CM-6 b,AU-12 c,AU-7 a,AU-7 b,AU-12 a,AU-8 b</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5561,7 +5561,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5642,7 +5642,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5723,7 +5723,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5805,7 +5805,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5887,7 +5887,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6051,7 +6051,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6207,7 +6207,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6290,7 +6290,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6368,7 +6368,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6459,7 +6459,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6541,7 +6541,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -7171,7 +7171,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7245,7 +7245,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7319,7 +7319,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7393,7 +7393,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7558,7 +7558,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7817,7 +7817,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7893,7 +7893,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7969,7 +7969,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8044,7 +8044,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8119,7 +8119,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8194,7 +8194,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8274,7 +8274,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8348,7 +8348,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8422,7 +8422,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8496,7 +8496,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8570,7 +8570,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8724,7 +8724,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8804,7 +8804,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9134,7 +9134,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9213,7 +9213,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9297,7 +9297,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9553,7 +9553,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>MA-4 c,AC-17 (2),SC-8,SC-13</t>
+          <t>MA-4 c,SC-13,SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9713,7 +9713,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9869,7 +9869,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10225,7 +10225,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10305,7 +10305,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11685,7 +11685,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11765,7 +11765,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11845,7 +11845,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12157,7 +12157,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12941,7 +12941,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B160" s="2" t="inlineStr">
@@ -13018,7 +13018,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B161" s="2" t="inlineStr">
@@ -13091,7 +13091,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -13164,7 +13164,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13249,7 +13249,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13324,7 +13324,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13399,7 +13399,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13474,7 +13474,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13977,7 +13977,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14266,7 +14266,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14341,7 +14341,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14423,7 +14423,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14587,7 +14587,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14669,7 +14669,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14751,7 +14751,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14833,7 +14833,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14915,7 +14915,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14997,7 +14997,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15079,7 +15079,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B188" s="2" t="inlineStr">
@@ -15157,7 +15157,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B189" s="2" t="inlineStr">
@@ -15236,7 +15236,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B190" s="2" t="inlineStr">
@@ -15318,7 +15318,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15400,7 +15400,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c</t>
+          <t>AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15482,7 +15482,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15564,7 +15564,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15646,7 +15646,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15728,7 +15728,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15803,7 +15803,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15876,7 +15876,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15953,7 +15953,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (4),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16040,7 +16040,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (4),IA-2 (3),IA-2 (2),IA-2</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (5),IA-2 (2),IA-2</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16129,7 +16129,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (4),IA-2 (3),IA-2 (2),IA-2</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (5),IA-2 (2),IA-2</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16815,7 +16815,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16892,7 +16892,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16978,7 +16978,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),AC-18 (1),SC-8</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17138,7 +17138,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17746,7 +17746,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17992,7 +17992,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -19336,7 +19336,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>CM-6 b,SC-2,SI-16</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -20254,7 +20254,7 @@
           <t>To verify if root user is required to use complex passwords, run the following command:
  $ grep enforce_for_root /etc/security/pwquality.conf 
 The output should return "enforce_for_root" uncommented.
-If enforce_for_root is not uncommented or configured correctly then this is a finding.</t>
+If enforce_for_root is commented or not configured correctly then this is a finding.</t>
         </is>
       </c>
       <c r="L252" s="2" t="n"/>
@@ -21514,7 +21514,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8),AU-7 a,AC-6 (9),AU-7 b,AU-8 b,CM-5 (1),AU-12 (3)</t>
+          <t>CM-5 (1),AC-6 (9),AU-12 (3),AU-7 b,AU-7 a,AU-8 b,AC-6 (8)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -21594,7 +21594,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -22108,7 +22108,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -22860,7 +22860,7 @@
     <row r="285" ht="130" customHeight="1">
       <c r="A285" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B285" s="2" t="inlineStr">
@@ -23844,7 +23844,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23915,7 +23915,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -23987,7 +23987,7 @@
     <row r="300" ht="130" customHeight="1">
       <c r="A300" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B300" s="2" t="inlineStr">
@@ -24145,7 +24145,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
+          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B302" s="2" t="inlineStr">
@@ -24362,7 +24362,7 @@
     <row r="304" ht="130" customHeight="1">
       <c r="A304" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B304" s="2" t="inlineStr">
@@ -27724,7 +27724,7 @@
     <row r="349" ht="130" customHeight="1">
       <c r="A349" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B349" s="2" t="inlineStr">
@@ -27874,7 +27874,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -27954,7 +27954,7 @@
     <row r="352" ht="130" customHeight="1">
       <c r="A352" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B352" s="2" t="inlineStr">
@@ -28027,7 +28027,7 @@
     <row r="353" ht="130" customHeight="1">
       <c r="A353" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B353" s="2" t="inlineStr">
@@ -30579,7 +30579,7 @@
     <row r="387" ht="130" customHeight="1">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
@@ -30973,7 +30973,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (9),CM-7 b,AC-17 (1)</t>
+          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -33550,7 +33550,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -33625,7 +33625,7 @@
     <row r="423" ht="130" customHeight="1">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
@@ -34312,7 +34312,7 @@
     <row r="432" ht="130" customHeight="1">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
@@ -34915,7 +34915,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35367,7 +35367,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
@@ -35667,7 +35667,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35744,7 +35744,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -36126,7 +36126,7 @@
     <row r="455" ht="130" customHeight="1">
       <c r="A455" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B455" s="2" t="inlineStr">
@@ -36773,7 +36773,7 @@
     <row r="464" ht="130" customHeight="1">
       <c r="A464" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B464" s="2" t="inlineStr">
@@ -37064,7 +37064,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
+          <t>MA-4 (7),SC-10,AC-12,MA-4 e</t>
         </is>
       </c>
       <c r="B468" s="2" t="inlineStr">
@@ -37139,7 +37139,7 @@
     <row r="469" ht="130" customHeight="1">
       <c r="A469" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B469" s="2" t="inlineStr">
@@ -37218,7 +37218,7 @@
     <row r="470" ht="130" customHeight="1">
       <c r="A470" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B470" s="2" t="inlineStr">
@@ -37294,7 +37294,7 @@
     <row r="471" ht="130" customHeight="1">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
@@ -38589,7 +38589,7 @@
     <row r="488" ht="130" customHeight="1">
       <c r="A488" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B488" s="2" t="inlineStr">
@@ -40135,7 +40135,7 @@
     <row r="508" ht="130" customHeight="1">
       <c r="A508" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B508" s="2" t="inlineStr">
@@ -40237,7 +40237,7 @@
     <row r="509" ht="130" customHeight="1">
       <c r="A509" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B509" s="2" t="inlineStr">
@@ -40347,7 +40347,7 @@
     <row r="510" ht="130" customHeight="1">
       <c r="A510" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B510" s="2" t="inlineStr">
@@ -40458,7 +40458,7 @@
     <row r="511" ht="130" customHeight="1">
       <c r="A511" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B511" s="2" t="inlineStr">
@@ -40930,7 +40930,7 @@
 attacks.
 Password complexity is one factor of several that determines how long it takes
 to crack a password. The more complex the password, the greater the number of
-possble combinations that need to be tested before the password is compromised.
+possible combinations that need to be tested before the password is compromised.
 Requiring a minimum number of special characters makes password guessing attacks
 more difficult by ensuring a larger search space.</t>
         </is>
@@ -40949,14 +40949,21 @@
         <is>
           <t>To check how many special characters are required in a password, run the following command:
  $ grep ocredit /etc/security/pwquality.conf 
-The "ocredit" parameter (as a negative number) will indicate how many special characters are required.
+The "ocredit" parameter (as a negative number) will indicate how many special
+characters are required.
 The DoD and FISMA require at least one special character in a password.
 This would appear as "ocredit = -1".
-If ocredit is not found or not equal to or less than the required value then this is a finding.</t>
+If value of "ocredit" is a positive number or is commented out then this is a finding.</t>
         </is>
       </c>
       <c r="L516" s="2" t="n"/>
-      <c r="M516" s="2" t="inlineStr"/>
+      <c r="M516" s="2" t="inlineStr">
+        <is>
+          <t>Add or modify the "ocredit" option line in /etc/security/pwquality.conf to have the required
+value, like in the following example:
+ocredit = 1</t>
+        </is>
+      </c>
       <c r="N516" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -41161,7 +41168,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">
@@ -42274,7 +42281,7 @@
     <row r="534" ht="130" customHeight="1">
       <c r="A534" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B534" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@5fd4e3a47a6119de7b730abcdecfb7d9dd772249 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -710,7 +710,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -782,7 +782,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-3,AU-7 (1),AU-3 (1),CM-6 b,AU-6 (4),MA-4 (1) (a),AU-7 a,AU-12 a,AU-14 (1)</t>
+          <t>CM-5 (1),CM-6 b,AU-7 (1),MA-4 (1) (a),AU-12 a,AU-3,AU-6 (4),AU-14 (1),AU-3 (1),AU-7 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AU-14 (1)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-14 (1),AU-3 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3340,7 +3340,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -4161,7 +4161,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4311,7 +4311,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4552,7 +4552,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4636,7 +4636,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4812,7 +4812,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4887,7 +4887,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4962,7 +4962,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5037,7 +5037,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5112,7 +5112,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5187,7 +5187,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5262,7 +5262,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5337,7 +5337,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5412,7 +5412,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 (3),CM-6 b,AU-12 c,AU-7 a,AU-7 b,AU-12 a,AU-8 b</t>
+          <t>AU-8 b,CM-5 (1),CM-6 b,AU-12 (3),AU-7 b,AU-12 c,AU-12 a,AU-7 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5561,7 +5561,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5642,7 +5642,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5723,7 +5723,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5805,7 +5805,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5887,7 +5887,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6051,7 +6051,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6133,7 +6133,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6207,7 +6207,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6290,7 +6290,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6368,7 +6368,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6459,7 +6459,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6541,7 +6541,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -7171,7 +7171,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7245,7 +7245,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7319,7 +7319,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7393,7 +7393,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7817,7 +7817,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7893,7 +7893,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7969,7 +7969,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8044,7 +8044,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8119,7 +8119,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8194,7 +8194,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8274,7 +8274,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8348,7 +8348,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8422,7 +8422,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8496,7 +8496,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8570,7 +8570,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8724,7 +8724,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8804,7 +8804,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9055,7 +9055,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9134,7 +9134,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9713,7 +9713,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9869,7 +9869,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10225,7 +10225,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10305,7 +10305,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11072,7 +11072,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11153,7 +11153,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11239,7 +11239,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11685,7 +11685,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11765,7 +11765,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11845,7 +11845,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12941,7 +12941,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B160" s="2" t="inlineStr">
@@ -13018,7 +13018,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B161" s="2" t="inlineStr">
@@ -13091,7 +13091,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -13164,7 +13164,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13249,7 +13249,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13324,7 +13324,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13399,7 +13399,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13474,7 +13474,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13977,7 +13977,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14266,7 +14266,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14341,7 +14341,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14423,7 +14423,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14587,7 +14587,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14669,7 +14669,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14751,7 +14751,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14833,7 +14833,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14915,7 +14915,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14997,7 +14997,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15079,7 +15079,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="2" t="inlineStr">
@@ -15157,7 +15157,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B189" s="2" t="inlineStr">
@@ -15236,7 +15236,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B190" s="2" t="inlineStr">
@@ -15318,7 +15318,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15400,7 +15400,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15482,7 +15482,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15564,7 +15564,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15646,7 +15646,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15728,7 +15728,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15803,7 +15803,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15876,7 +15876,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c,AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15953,7 +15953,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (1),IA-2 (2)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16040,7 +16040,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (5),IA-2 (2),IA-2</t>
+          <t>IA-2 (3),IA-2,IA-2 (5),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16129,7 +16129,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (5),IA-2 (2),IA-2</t>
+          <t>IA-2 (3),IA-2,IA-2 (5),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16373,7 +16373,7 @@
     <row r="204" ht="130" customHeight="1">
       <c r="A204" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B204" s="2" t="inlineStr">
@@ -16815,7 +16815,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16892,7 +16892,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16978,7 +16978,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17906,7 +17906,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17992,7 +17992,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),CM-6 b,SC-5</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18362,7 +18362,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-8,AU-3 (1),IA-2</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19336,7 +19336,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2,SI-16</t>
+          <t>SC-2,CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19658,7 +19658,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -19865,16 +19865,20 @@
         <is>
           <t>Verify the "umask" setting is configured correctly in the "/etc/bashrc" file by
 running the following command:
- # grep "umask" /etc/bashrc 
+ $ sudo grep "umask" /etc/bashrc 
 All output must show the value of "umask" set as shown below:
- # grep "umask" /etc/bashrc
-umask 
-umask  
-If the above command returns no output, or if the umask is configured incorrectly then this is a finding.</t>
+ umask 077 
+If the above command returns no output, or the umask is configured incorrectly then this is a finding.</t>
         </is>
       </c>
       <c r="L247" s="2" t="n"/>
-      <c r="M247" s="2" t="inlineStr"/>
+      <c r="M247" s="2" t="inlineStr">
+        <is>
+          <t>Configure the Red Hat Enterprise Linux 9 to define default permissions for all authenticated users in such a way that the user can only read and modify their own files.
+Add or edit the lines for the "umask" parameter in the "/etc/bashrc" files to "077":
+umask 077</t>
+        </is>
+      </c>
       <c r="N247" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -19941,15 +19945,20 @@
         <is>
           <t>Verify the "umask" setting is configured correctly in the "/etc/csh.cshrc" file by
 running the following command:
- # grep "umask" /etc/csh.cshrc 
+ $ sudo grep "umask" /etc/csh.cshrc 
 All output must show the value of "umask" set as shown in the below:
- # grep "umask" /etc/csh.cshrc
-umask  
-If the above command returns no output, or if the umask is configured incorrectly then this is a finding.</t>
+ umask 077 
+If the above command returns no output, or the umask is configured incorrectly then this is a finding.</t>
         </is>
       </c>
       <c r="L248" s="2" t="n"/>
-      <c r="M248" s="2" t="inlineStr"/>
+      <c r="M248" s="2" t="inlineStr">
+        <is>
+          <t>Configure the Red Hat Enterprise Linux 9 to define default permissions for all authenticated users in such a way that the user can only read and modify their own files.
+Add or edit the lines for the "umask" parameter in the "/etc/csh.cshrc" files to "077":
+umask 077</t>
+        </is>
+      </c>
       <c r="N248" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -20016,15 +20025,20 @@
         <is>
           <t>Verify the "UMASK" setting is configured correctly in the "/etc/login.defs" file by
 running the following command:
- # grep -i "UMASK" /etc/login.defs 
-All output must show the value of "umask" set as shown in the below:
- # grep -i "UMASK" /etc/login.defs
-umask  
-If the above command returns no output, or if the umask is configured incorrectly then this is a finding.</t>
+ $ sudo grep "UMASK" /etc/login.defs 
+All output must show the value of "UMASK" set as shown in the below:
+ UMASK 077 
+If the above command returns no output, or the umask is configured incorrectly then this is a finding.</t>
         </is>
       </c>
       <c r="L249" s="2" t="n"/>
-      <c r="M249" s="2" t="inlineStr"/>
+      <c r="M249" s="2" t="inlineStr">
+        <is>
+          <t>Configure the Red Hat Enterprise Linux 9 to define default permissions for all authenticated users in such a way that the user can only read and modify their own files.
+Add or edit the lines for the "UMASK" parameter in the "/etc/login.defs" files to "077":
+UMASK 077</t>
+        </is>
+      </c>
       <c r="N249" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -20091,15 +20105,20 @@
         <is>
           <t>Verify the "umask" setting is configured correctly in the "/etc/profile" file by
 running the following command:
- # grep "umask" /etc/profile 
+ $ sudo grep "umask" /etc/profile 
 All output must show the value of "umask" set as shown in the below:
- # grep "umask" /etc/profile
-umask  
-If the above command returns no output, or if the umask is configured incorrectly then this is a finding.</t>
+ umask 077 
+If the above command returns no output, or the umask is configured incorrectly then this is a finding.</t>
         </is>
       </c>
       <c r="L250" s="2" t="n"/>
-      <c r="M250" s="2" t="inlineStr"/>
+      <c r="M250" s="2" t="inlineStr">
+        <is>
+          <t>Configure the Red Hat Enterprise Linux 9 to define default permissions for all authenticated users in such a way that the user can only read and modify their own files.
+Add or edit the lines for the "umask" parameter in the "/etc/profile" files to "077":
+umask 077</t>
+        </is>
+      </c>
       <c r="N250" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -20194,7 +20213,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -20843,7 +20862,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20931,7 +20950,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -21432,7 +21451,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -21514,7 +21533,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (9),AU-12 (3),AU-7 b,AU-7 a,AU-8 b,AC-6 (8)</t>
+          <t>AC-6 (8),AU-8 b,AC-6 (9),CM-5 (1),AU-12 (3),AU-7 b,AU-7 a</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -22181,7 +22200,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22706,7 +22725,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -22860,7 +22879,7 @@
     <row r="285" ht="130" customHeight="1">
       <c r="A285" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B285" s="2" t="inlineStr">
@@ -23008,7 +23027,7 @@
     <row r="287" ht="130" customHeight="1">
       <c r="A287" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B287" s="2" t="inlineStr">
@@ -23082,7 +23101,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B288" s="2" t="inlineStr">
@@ -23844,7 +23863,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23915,7 +23934,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -23987,7 +24006,7 @@
     <row r="300" ht="130" customHeight="1">
       <c r="A300" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B300" s="2" t="inlineStr">
@@ -24145,7 +24164,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B302" s="2" t="inlineStr">
@@ -27874,7 +27893,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -30973,7 +30992,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
+          <t>CM-7 b,CM-6 b,AC-17 (1),AC-17 (9)</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -31051,7 +31070,7 @@
     <row r="393" ht="130" customHeight="1">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
@@ -34493,7 +34512,7 @@
     <row r="434" ht="130" customHeight="1">
       <c r="A434" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B434" s="2" t="inlineStr">
@@ -34580,7 +34599,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
@@ -35367,7 +35386,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
@@ -36126,7 +36145,7 @@
     <row r="455" ht="130" customHeight="1">
       <c r="A455" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B455" s="2" t="inlineStr">
@@ -37064,7 +37083,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),SC-10,AC-12,MA-4 e</t>
+          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
         </is>
       </c>
       <c r="B468" s="2" t="inlineStr">
@@ -37294,7 +37313,7 @@
     <row r="471" ht="130" customHeight="1">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>SC-8,SC-8 (1),AC-17 (2)</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
@@ -37304,7 +37323,7 @@
       </c>
       <c r="C471" s="2" t="inlineStr">
         <is>
-          <t>SRG-OS-000423-GPOS-00187,SRG-OS-000033-GPOS-00014</t>
+          <t>SRG-OS-000423-GPOS-00187,SRG-OS-000033-GPOS-00014,SRG-OS-000424-GPOS-00188</t>
         </is>
       </c>
       <c r="D471" s="2" t="inlineStr">
@@ -37353,14 +37372,21 @@
 properly, output should be  /etc/ssh/ssh_config.d/02-rekey-limit.conf:
 RekeyLimit 
   Check also the
-main configuration file with the following command:  sudo grep
+main configuration file with the following command:  $ sudo grep
 RekeyLimit /etc/ssh/ssh_config  The command should not return any
 output.
 If it is commented out or is not set then this is a finding.</t>
         </is>
       </c>
       <c r="L471" s="2" t="n"/>
-      <c r="M471" s="2" t="inlineStr"/>
+      <c r="M471" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to force a frequent session key renegotiation for SSH connections to the server by adding or modifying the following line in the "/etc/ssh/sshd_config" file:
+RekeyLimit  
+Restart the SSH daemon for the settings to take effect.
+$ sudo systemctl restart sshd.service</t>
+        </is>
+      </c>
       <c r="N471" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -39896,7 +39922,7 @@
     <row r="505" ht="130" customHeight="1">
       <c r="A505" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B505" s="2" t="inlineStr">
@@ -40135,7 +40161,7 @@
     <row r="508" ht="130" customHeight="1">
       <c r="A508" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B508" s="2" t="inlineStr">
@@ -40237,7 +40263,7 @@
     <row r="509" ht="130" customHeight="1">
       <c r="A509" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B509" s="2" t="inlineStr">
@@ -40347,7 +40373,7 @@
     <row r="510" ht="130" customHeight="1">
       <c r="A510" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B510" s="2" t="inlineStr">
@@ -40458,7 +40484,7 @@
     <row r="511" ht="130" customHeight="1">
       <c r="A511" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B511" s="2" t="inlineStr">
@@ -41168,7 +41194,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">
@@ -42336,14 +42362,20 @@
       <c r="K534" s="2" t="inlineStr">
         <is>
           <t>To verify if GnuTLS uses defined DoD-approved TLS Crypto Policy, run:
- $ grep
+ $ sudo grep
 '+VERS-ALL:-VERS-DTLS0.9:-VERS-SSL3.0:-VERS-TLS1.0:-VERS-TLS1.1:-VERS-DTLS1.0'
 /etc/crypto-policies/back-ends/gnutls.config  and verify that a match exists.
 If cryptographic policy for gnutls is not configured or is configured incorrectly then this is a finding.</t>
         </is>
       </c>
       <c r="L534" s="2" t="n"/>
-      <c r="M534" s="2" t="inlineStr"/>
+      <c r="M534" s="2" t="inlineStr">
+        <is>
+          <t>Configure the Red Hat Enterprise Linux 9 GnuTLS library to use only DoD-approved encryption by adding the following line to "/etc/crypto-policies/back-ends/gnutls.config":
++VERS-ALL:-VERS-DTLS0.9:-VERS-SSL3.0:-VERS-TLS1.0:-VERS-TLS1.1:-VERS-DTLS1.0
+A reboot is required for the changes to take effect.</t>
+        </is>
+      </c>
       <c r="N534" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@b1c66aa1e97167a6bc98d92cefad52f95b8f8865 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-7 (1),AU-3,AU-12 a,AU-7 a,CM-6 b,AU-6 (4),MA-4 (1) (a),AU-14 (1),CM-5 (1)</t>
+          <t>AU-3 (1),AU-7 (1),AU-7 a,CM-5 (1),AU-12 a,AU-6 (4),CM-6 b,MA-4 (1) (a),AU-3,AU-14 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-14 (1),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3,AU-14 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -4170,7 +4170,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -4320,7 +4320,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4645,7 +4645,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4821,7 +4821,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4896,7 +4896,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -4971,7 +4971,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5046,7 +5046,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5121,7 +5121,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -5196,7 +5196,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -5271,7 +5271,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -5346,7 +5346,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -5421,7 +5421,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -5496,7 +5496,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-7 a,CM-6 b,AU-12 (3),AU-12 c,AU-7 b,AU-8 b,CM-5 (1)</t>
+          <t>AU-7 a,CM-5 (1),AU-8 b,AU-12 a,AU-12 (3),AU-7 b,CM-6 b,AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5570,7 +5570,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5732,7 +5732,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5814,7 +5814,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5978,7 +5978,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6060,7 +6060,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6142,7 +6142,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6216,7 +6216,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6299,7 +6299,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6377,7 +6377,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6468,7 +6468,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6550,7 +6550,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -7180,7 +7180,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7254,7 +7254,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7328,7 +7328,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -7402,7 +7402,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7482,7 +7482,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -7643,7 +7643,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7826,7 +7826,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -7978,7 +7978,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -8053,7 +8053,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -8128,7 +8128,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -8203,7 +8203,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -8283,7 +8283,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8357,7 +8357,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8431,7 +8431,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8505,7 +8505,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -8579,7 +8579,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -8653,7 +8653,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -8733,7 +8733,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -8813,7 +8813,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -9562,7 +9562,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-13,MA-4 c</t>
+          <t>SC-13,AC-17 (2),MA-4 c,SC-8</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9644,7 +9644,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
@@ -9722,7 +9722,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9800,7 +9800,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9878,7 +9878,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -9958,7 +9958,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10027,7 +10027,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -10096,7 +10096,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -10165,7 +10165,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -10234,7 +10234,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -10314,7 +10314,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11081,7 +11081,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11162,7 +11162,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11248,7 +11248,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11614,7 +11614,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="3" t="inlineStr">
@@ -11694,7 +11694,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
@@ -11774,7 +11774,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B145" s="3" t="inlineStr">
@@ -11854,7 +11854,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
@@ -12166,7 +12166,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12553,7 +12553,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -12629,7 +12629,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12714,7 +12714,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12950,7 +12950,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13027,7 +13027,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13100,7 +13100,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13173,7 +13173,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13258,7 +13258,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13333,7 +13333,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13408,7 +13408,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13483,7 +13483,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13558,7 +13558,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
@@ -13629,7 +13629,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
@@ -13700,7 +13700,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
@@ -13772,7 +13772,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -13843,7 +13843,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
@@ -13914,7 +13914,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
@@ -13986,7 +13986,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14061,7 +14061,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14132,7 +14132,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14203,7 +14203,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14275,7 +14275,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14350,7 +14350,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14432,7 +14432,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14514,7 +14514,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14596,7 +14596,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14678,7 +14678,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14760,7 +14760,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14842,7 +14842,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -14924,7 +14924,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15006,7 +15006,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15088,7 +15088,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15166,7 +15166,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15245,7 +15245,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15327,7 +15327,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15409,7 +15409,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15491,7 +15491,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15573,7 +15573,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15655,7 +15655,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15737,7 +15737,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
@@ -15812,7 +15812,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
@@ -15885,7 +15885,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
@@ -15962,7 +15962,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (4),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16049,7 +16049,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (4),IA-2 (5),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16138,7 +16138,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (4),IA-2 (5),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16382,7 +16382,7 @@
     <row r="204" ht="130" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
@@ -16824,7 +16824,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16901,7 +16901,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16987,7 +16987,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17755,7 +17755,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17915,7 +17915,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
@@ -18001,7 +18001,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),CM-6 b,SC-5</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18371,7 +18371,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19345,7 +19345,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2,SI-16</t>
+          <t>SC-2,CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B241" s="3" t="inlineStr">
@@ -20222,7 +20222,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -20790,7 +20790,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20871,7 +20871,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
@@ -20959,7 +20959,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="3" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B261" s="3" t="inlineStr">
@@ -22136,7 +22136,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B276" s="3" t="inlineStr">
@@ -22209,7 +22209,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22894,7 +22894,7 @@
     <row r="285" ht="130" customHeight="1">
       <c r="A285" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B285" s="3" t="inlineStr">
@@ -23042,7 +23042,7 @@
     <row r="287" ht="130" customHeight="1">
       <c r="A287" s="3" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B287" s="3" t="inlineStr">
@@ -23116,7 +23116,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
@@ -24179,7 +24179,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="3" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B302" s="3" t="inlineStr">
@@ -24396,7 +24396,7 @@
     <row r="304" ht="130" customHeight="1">
       <c r="A304" s="3" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B304" s="3" t="inlineStr">
@@ -27758,7 +27758,7 @@
     <row r="349" ht="130" customHeight="1">
       <c r="A349" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B349" s="3" t="inlineStr">
@@ -27908,7 +27908,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -30369,7 +30369,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="3" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B384" s="3" t="inlineStr">
@@ -30613,7 +30613,7 @@
     <row r="387" ht="130" customHeight="1">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
@@ -31007,7 +31007,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>AC-17 (9),AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -31085,7 +31085,7 @@
     <row r="393" ht="130" customHeight="1">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
@@ -34346,7 +34346,7 @@
     <row r="432" ht="130" customHeight="1">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
@@ -34527,7 +34527,7 @@
     <row r="434" ht="130" customHeight="1">
       <c r="A434" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B434" s="3" t="inlineStr">
@@ -34614,7 +34614,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B435" s="3" t="inlineStr">
@@ -34949,7 +34949,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35401,7 +35401,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="3" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B445" s="3" t="inlineStr">
@@ -37098,7 +37098,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
+          <t>SC-10,MA-4 (7),MA-4 e,AC-12</t>
         </is>
       </c>
       <c r="B468" s="3" t="inlineStr">
@@ -37328,7 +37328,7 @@
     <row r="471" ht="130" customHeight="1">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-8 (1)</t>
+          <t>AC-17 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
@@ -38920,7 +38920,7 @@
     <row r="492" ht="130" customHeight="1">
       <c r="A492" s="3" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B492" s="3" t="inlineStr">
@@ -41215,7 +41215,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">
@@ -42405,7 +42405,7 @@
     <row r="535" ht="130" customHeight="1">
       <c r="A535" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B535" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@2615738bcac8c9d7438b4c4bfbcebcb8bfa3c437 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-7 (1),AU-7 a,CM-5 (1),AU-12 a,AU-6 (4),CM-6 b,MA-4 (1) (a),AU-3,AU-14 (1)</t>
+          <t>AU-14 (1),AU-7 a,AU-3 (1),CM-5 (1),MA-4 (1) (a),AU-12 a,AU-3,AU-7 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3,AU-14 (1)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-14 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -4170,7 +4170,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -4240,7 +4240,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -4561,7 +4561,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4645,7 +4645,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4821,7 +4821,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4896,7 +4896,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -4971,7 +4971,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5046,7 +5046,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5121,7 +5121,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -5196,7 +5196,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -5271,7 +5271,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -5346,7 +5346,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -5421,7 +5421,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -5496,7 +5496,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-5 (1),AU-8 b,AU-12 a,AU-12 (3),AU-7 b,CM-6 b,AU-12 c</t>
+          <t>AU-7 b,AU-7 a,CM-5 (1),AU-12 a,AU-12 c,AU-8 b,AU-12 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5570,7 +5570,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5732,7 +5732,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5814,7 +5814,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5978,7 +5978,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6060,7 +6060,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6216,7 +6216,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6299,7 +6299,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6377,7 +6377,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6468,7 +6468,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6550,7 +6550,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -7180,7 +7180,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7254,7 +7254,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7328,7 +7328,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -7402,7 +7402,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7482,7 +7482,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -7643,7 +7643,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7826,7 +7826,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -7978,7 +7978,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -8053,7 +8053,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -8128,7 +8128,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -8203,7 +8203,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -8283,7 +8283,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8357,7 +8357,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8431,7 +8431,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8505,7 +8505,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -8579,7 +8579,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -8653,7 +8653,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -8733,7 +8733,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -8813,7 +8813,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -8893,7 +8893,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9064,7 +9064,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9143,7 +9143,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9222,7 +9222,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9306,7 +9306,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9562,7 +9562,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>SC-13,AC-17 (2),MA-4 c,SC-8</t>
+          <t>SC-8,MA-4 c,AC-17 (2),SC-13</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9722,7 +9722,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9878,7 +9878,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10234,7 +10234,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -10314,7 +10314,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11694,7 +11694,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
@@ -11774,7 +11774,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B145" s="3" t="inlineStr">
@@ -11854,7 +11854,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
@@ -12553,7 +12553,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -12629,7 +12629,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12714,7 +12714,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12950,7 +12950,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13027,7 +13027,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13100,7 +13100,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13173,7 +13173,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13258,7 +13258,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13333,7 +13333,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13408,7 +13408,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13483,7 +13483,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13986,7 +13986,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14275,7 +14275,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14350,7 +14350,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14432,7 +14432,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14514,7 +14514,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14596,7 +14596,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14678,7 +14678,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14760,7 +14760,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14842,7 +14842,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -14924,7 +14924,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15006,7 +15006,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15088,7 +15088,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15166,7 +15166,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15245,7 +15245,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15327,7 +15327,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15409,7 +15409,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15491,7 +15491,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15573,7 +15573,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15655,7 +15655,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15737,7 +15737,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
@@ -15812,7 +15812,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
@@ -15885,7 +15885,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
@@ -15962,7 +15962,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (1)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16049,7 +16049,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (3),IA-2 (2),IA-2,IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16138,7 +16138,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (3),IA-2 (2),IA-2,IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16382,7 +16382,7 @@
     <row r="204" ht="130" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
@@ -16824,7 +16824,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16901,7 +16901,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16987,7 +16987,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17147,7 +17147,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
@@ -17755,7 +17755,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -18001,7 +18001,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18371,7 +18371,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -20222,7 +20222,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -21622,7 +21622,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="3" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B269" s="3" t="inlineStr">
@@ -22136,7 +22136,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B276" s="3" t="inlineStr">
@@ -24179,7 +24179,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="3" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B302" s="3" t="inlineStr">
@@ -27908,7 +27908,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -27988,7 +27988,7 @@
     <row r="352" ht="130" customHeight="1">
       <c r="A352" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B352" s="3" t="inlineStr">
@@ -28061,7 +28061,7 @@
     <row r="353" ht="130" customHeight="1">
       <c r="A353" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B353" s="3" t="inlineStr">
@@ -28641,7 +28641,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="3" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B361" s="3" t="inlineStr">
@@ -31007,7 +31007,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>AC-17 (9),CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -31085,7 +31085,7 @@
     <row r="393" ht="130" customHeight="1">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
@@ -33584,7 +33584,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="3" t="inlineStr">
@@ -33659,7 +33659,7 @@
     <row r="423" ht="130" customHeight="1">
       <c r="A423" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B423" s="3" t="inlineStr">
@@ -35701,7 +35701,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B449" s="3" t="inlineStr">
@@ -35778,7 +35778,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="3" t="inlineStr">
@@ -36160,7 +36160,7 @@
     <row r="455" ht="130" customHeight="1">
       <c r="A455" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B455" s="3" t="inlineStr">
@@ -36807,7 +36807,7 @@
     <row r="464" ht="130" customHeight="1">
       <c r="A464" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B464" s="3" t="inlineStr">
@@ -37098,7 +37098,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="3" t="inlineStr">
         <is>
-          <t>SC-10,MA-4 (7),MA-4 e,AC-12</t>
+          <t>MA-4 (7),MA-4 e,SC-10,AC-12</t>
         </is>
       </c>
       <c r="B468" s="3" t="inlineStr">
@@ -37173,7 +37173,7 @@
     <row r="469" ht="130" customHeight="1">
       <c r="A469" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B469" s="3" t="inlineStr">
@@ -37252,7 +37252,7 @@
     <row r="470" ht="130" customHeight="1">
       <c r="A470" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B470" s="3" t="inlineStr">
@@ -37328,7 +37328,7 @@
     <row r="471" ht="130" customHeight="1">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8 (1),SC-8</t>
+          <t>SC-8,SC-8 (1),AC-17 (2)</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
@@ -38630,7 +38630,7 @@
     <row r="488" ht="130" customHeight="1">
       <c r="A488" s="3" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B488" s="3" t="inlineStr">
@@ -38920,7 +38920,7 @@
     <row r="492" ht="130" customHeight="1">
       <c r="A492" s="3" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B492" s="3" t="inlineStr">
@@ -39937,7 +39937,7 @@
     <row r="505" ht="130" customHeight="1">
       <c r="A505" s="3" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B505" s="3" t="inlineStr">
@@ -40182,7 +40182,7 @@
     <row r="508" ht="130" customHeight="1">
       <c r="A508" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B508" s="2" t="inlineStr">
@@ -40284,7 +40284,7 @@
     <row r="509" ht="130" customHeight="1">
       <c r="A509" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B509" s="2" t="inlineStr">
@@ -40394,7 +40394,7 @@
     <row r="510" ht="130" customHeight="1">
       <c r="A510" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B510" s="2" t="inlineStr">
@@ -40505,7 +40505,7 @@
     <row r="511" ht="130" customHeight="1">
       <c r="A511" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B511" s="2" t="inlineStr">
@@ -41215,7 +41215,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">
@@ -42405,7 +42405,7 @@
     <row r="535" ht="130" customHeight="1">
       <c r="A535" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B535" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@7f40d1f6c0475e2f2acfc993fd8fdfca81b0c94d 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-7 a,AU-3 (1),CM-5 (1),MA-4 (1) (a),AU-12 a,AU-3,AU-7 (1),AU-6 (4),CM-6 b</t>
+          <t>CM-6 b,AU-3,AU-7 (1),AU-14 (1),AU-6 (4),AU-3 (1),AU-12 a,CM-5 (1),MA-4 (1) (a),AU-7 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1770,7 +1770,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2214,7 +2214,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-14 (1)</t>
+          <t>AU-12 c,AU-3,AU-14 (1),AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -3791,7 +3791,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4170,7 +4170,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -4320,7 +4320,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4645,7 +4645,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4737,7 +4737,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4821,7 +4821,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4896,7 +4896,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -4971,7 +4971,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5046,7 +5046,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5121,7 +5121,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -5196,7 +5196,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -5271,7 +5271,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -5346,7 +5346,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -5421,7 +5421,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -5496,7 +5496,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-7 a,CM-5 (1),AU-12 a,AU-12 c,AU-8 b,AU-12 (3),CM-6 b</t>
+          <t>CM-6 b,AU-12 c,AU-7 b,AU-12 (3),AU-12 a,CM-5 (1),AU-8 b,AU-7 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5570,7 +5570,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5732,7 +5732,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5814,7 +5814,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5978,7 +5978,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6060,7 +6060,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6142,7 +6142,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6216,7 +6216,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6299,7 +6299,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6377,7 +6377,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6468,7 +6468,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6550,7 +6550,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -7180,7 +7180,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7254,7 +7254,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7328,7 +7328,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -7402,7 +7402,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7567,7 +7567,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7978,7 +7978,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -8053,7 +8053,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -8128,7 +8128,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -8203,7 +8203,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -8281,60 +8281,60 @@
       <c r="Q100" s="3" t="n"/>
     </row>
     <row r="101" ht="130" customHeight="1">
-      <c r="A101" s="3" t="inlineStr">
-        <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
-        </is>
-      </c>
-      <c r="B101" s="3" t="inlineStr">
+      <c r="A101" s="2" t="inlineStr">
+        <is>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+        </is>
+      </c>
+      <c r="B101" s="2" t="inlineStr">
         <is>
           <t>CCI-000169,CCI-000172,CCI-000366,CCI-002884</t>
         </is>
       </c>
-      <c r="C101" s="3" t="inlineStr">
+      <c r="C101" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000466-GPOS-00210,SRG-OS-000467-GPOS-00211,SRG-OS-000468-GPOS-00212</t>
         </is>
       </c>
-      <c r="D101" s="3" t="inlineStr">
+      <c r="D101" s="2" t="inlineStr">
         <is>
           <t>CCE-83754-2</t>
         </is>
       </c>
-      <c r="E101" s="3" t="inlineStr">
+      <c r="E101" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
-      <c r="F101" s="3" t="inlineStr">
+      <c r="F101" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
-      <c r="G101" s="3" t="inlineStr">
+      <c r="G101" s="2" t="inlineStr">
         <is>
           <t>Without generating audit records that are specific to the security and mission needs of the organization, it would be difficult to establish, correlate, and investigate the events relating to an incident or identify those responsible for one.
 Audit records can be generated from various components within the information system (e.g., module or policy filter).</t>
         </is>
       </c>
-      <c r="H101" s="3" t="inlineStr">
+      <c r="H101" s="2" t="inlineStr">
         <is>
           <t>Auditing file deletions will create an audit trail for files that are removed
 from the system. The audit trail could aid in system troubleshooting, as well as, detecting
 malicious processes that attempt to delete log files to conceal their presence.</t>
         </is>
       </c>
-      <c r="I101" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J101" s="3" t="inlineStr">
+      <c r="I101" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J101" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system generates audit records when successful/unsuccessful attempts to delete privileges occur. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K101" s="3" t="inlineStr">
+      <c r="K101" s="2" t="inlineStr">
         <is>
           <t>To determine if the system is configured to audit calls to the
  rename  system call, run the following command:
@@ -8343,72 +8343,80 @@
 If no line is returned, then this is a finding.</t>
         </is>
       </c>
-      <c r="L101" s="3" t="n"/>
-      <c r="M101" s="3" t="inlineStr"/>
-      <c r="N101" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O101" s="3" t="n"/>
-      <c r="P101" s="3" t="n"/>
-      <c r="Q101" s="3" t="n"/>
+      <c r="L101" s="2" t="n"/>
+      <c r="M101" s="2" t="inlineStr">
+        <is>
+          <t>Configure the audit system to generate an audit event for any successful/unsuccessful use of the "rename" command by adding or updating the following rules in the "/etc/audit/rules.d/audit.rules" file:
+ -a always,exit -F arch=b32 -S rename -F auid&gt;=1000 -F auid!=unset -k delete
+ -a always,exit -F arch=b64 -S rename -F auid&gt;=1000 -F auid!=unset -k delete
+ It's allowed to group this system call within the same line as "rename", "unlink", "rmdir", "renameat", and "unlinkat".
+ The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
+      <c r="N101" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O101" s="2" t="n"/>
+      <c r="P101" s="2" t="n"/>
+      <c r="Q101" s="2" t="n"/>
     </row>
     <row r="102" ht="130" customHeight="1">
-      <c r="A102" s="3" t="inlineStr">
-        <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
-        </is>
-      </c>
-      <c r="B102" s="3" t="inlineStr">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+        </is>
+      </c>
+      <c r="B102" s="2" t="inlineStr">
         <is>
           <t>CCI-000169,CCI-000172,CCI-000366,CCI-002884</t>
         </is>
       </c>
-      <c r="C102" s="3" t="inlineStr">
+      <c r="C102" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000466-GPOS-00210,SRG-OS-000467-GPOS-00211,SRG-OS-000468-GPOS-00212</t>
         </is>
       </c>
-      <c r="D102" s="3" t="inlineStr">
+      <c r="D102" s="2" t="inlineStr">
         <is>
           <t>CCE-83756-7</t>
         </is>
       </c>
-      <c r="E102" s="3" t="inlineStr">
+      <c r="E102" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
-      <c r="F102" s="3" t="inlineStr">
+      <c r="F102" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
-      <c r="G102" s="3" t="inlineStr">
+      <c r="G102" s="2" t="inlineStr">
         <is>
           <t>Without generating audit records that are specific to the security and mission needs of the organization, it would be difficult to establish, correlate, and investigate the events relating to an incident or identify those responsible for one.
 Audit records can be generated from various components within the information system (e.g., module or policy filter).</t>
         </is>
       </c>
-      <c r="H102" s="3" t="inlineStr">
+      <c r="H102" s="2" t="inlineStr">
         <is>
           <t>Auditing file deletions will create an audit trail for files that are removed
 from the system. The audit trail could aid in system troubleshooting, as well as, detecting
 malicious processes that attempt to delete log files to conceal their presence.</t>
         </is>
       </c>
-      <c r="I102" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J102" s="3" t="inlineStr">
+      <c r="I102" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J102" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system generates audit records when successful/unsuccessful attempts to delete privileges occur. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K102" s="3" t="inlineStr">
+      <c r="K102" s="2" t="inlineStr">
         <is>
           <t>To determine if the system is configured to audit calls to the
  renameat  system call, run the following command:
@@ -8417,72 +8425,80 @@
 If no line is returned, then this is a finding.</t>
         </is>
       </c>
-      <c r="L102" s="3" t="n"/>
-      <c r="M102" s="3" t="inlineStr"/>
-      <c r="N102" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O102" s="3" t="n"/>
-      <c r="P102" s="3" t="n"/>
-      <c r="Q102" s="3" t="n"/>
+      <c r="L102" s="2" t="n"/>
+      <c r="M102" s="2" t="inlineStr">
+        <is>
+          <t>Configure the audit system to generate an audit event for any successful/unsuccessful use of the "renameat" command by adding or updating the following rules in the "/etc/audit/rules.d/audit.rules" file:
+-a always,exit -F arch=b32 -S renameat -F auid&gt;=1000 -F auid!=unset -k delete
+-a always,exit -F arch=b64 -S renameat -F auid&gt;=1000 -F auid!=unset -k delete
+It's allowed to group this system call within the same line as "rename", "unlink", "rmdir", "renameat", and "unlinkat".
+The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
+      <c r="N102" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O102" s="2" t="n"/>
+      <c r="P102" s="2" t="n"/>
+      <c r="Q102" s="2" t="n"/>
     </row>
     <row r="103" ht="130" customHeight="1">
-      <c r="A103" s="3" t="inlineStr">
-        <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
-        </is>
-      </c>
-      <c r="B103" s="3" t="inlineStr">
+      <c r="A103" s="2" t="inlineStr">
+        <is>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+        </is>
+      </c>
+      <c r="B103" s="2" t="inlineStr">
         <is>
           <t>CCI-000169,CCI-000172,CCI-000366,CCI-002884</t>
         </is>
       </c>
-      <c r="C103" s="3" t="inlineStr">
+      <c r="C103" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000466-GPOS-00210,SRG-OS-000467-GPOS-00211,SRG-OS-000468-GPOS-00212</t>
         </is>
       </c>
-      <c r="D103" s="3" t="inlineStr">
+      <c r="D103" s="2" t="inlineStr">
         <is>
           <t>CCE-83758-3</t>
         </is>
       </c>
-      <c r="E103" s="3" t="inlineStr">
+      <c r="E103" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
-      <c r="F103" s="3" t="inlineStr">
+      <c r="F103" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
-      <c r="G103" s="3" t="inlineStr">
+      <c r="G103" s="2" t="inlineStr">
         <is>
           <t>Without generating audit records that are specific to the security and mission needs of the organization, it would be difficult to establish, correlate, and investigate the events relating to an incident or identify those responsible for one.
 Audit records can be generated from various components within the information system (e.g., module or policy filter).</t>
         </is>
       </c>
-      <c r="H103" s="3" t="inlineStr">
+      <c r="H103" s="2" t="inlineStr">
         <is>
           <t>Auditing file deletions will create an audit trail for files that are removed
 from the system. The audit trail could aid in system troubleshooting, as well as, detecting
 malicious processes that attempt to delete log files to conceal their presence.</t>
         </is>
       </c>
-      <c r="I103" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J103" s="3" t="inlineStr">
+      <c r="I103" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J103" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system generates audit records when successful/unsuccessful attempts to delete privileges occur. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K103" s="3" t="inlineStr">
+      <c r="K103" s="2" t="inlineStr">
         <is>
           <t>To determine if the system is configured to audit calls to the
  rmdir  system call, run the following command:
@@ -8491,72 +8507,80 @@
 If no line is returned, then this is a finding.</t>
         </is>
       </c>
-      <c r="L103" s="3" t="n"/>
-      <c r="M103" s="3" t="inlineStr"/>
-      <c r="N103" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O103" s="3" t="n"/>
-      <c r="P103" s="3" t="n"/>
-      <c r="Q103" s="3" t="n"/>
+      <c r="L103" s="2" t="n"/>
+      <c r="M103" s="2" t="inlineStr">
+        <is>
+          <t>Configure the audit system to generate an audit event for any successful/unsuccessful use of the "rmdir" command by adding or updating the following rules in the "/etc/audit/rules.d/audit.rules" file:
+-a always,exit -F arch=b32 -S rmdir -F auid&gt;=1000 -F auid!=unset -k delete
+-a always,exit -F arch=b64 -S rmdir -F auid&gt;=1000 -F auid!=unset -k delete
+It's allowed to group this system call within the same line as "rename", "unlink", "rmdir", "renameat", and "unlinkat".
+The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
+      <c r="N103" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O103" s="2" t="n"/>
+      <c r="P103" s="2" t="n"/>
+      <c r="Q103" s="2" t="n"/>
     </row>
     <row r="104" ht="130" customHeight="1">
-      <c r="A104" s="3" t="inlineStr">
-        <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
-        </is>
-      </c>
-      <c r="B104" s="3" t="inlineStr">
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="inlineStr">
         <is>
           <t>CCI-000169,CCI-000172,CCI-000366,CCI-002884</t>
         </is>
       </c>
-      <c r="C104" s="3" t="inlineStr">
+      <c r="C104" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000466-GPOS-00210,SRG-OS-000467-GPOS-00211,SRG-OS-000468-GPOS-00212</t>
         </is>
       </c>
-      <c r="D104" s="3" t="inlineStr">
+      <c r="D104" s="2" t="inlineStr">
         <is>
           <t>CCE-83757-5</t>
         </is>
       </c>
-      <c r="E104" s="3" t="inlineStr">
+      <c r="E104" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
-      <c r="F104" s="3" t="inlineStr">
+      <c r="F104" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
-      <c r="G104" s="3" t="inlineStr">
+      <c r="G104" s="2" t="inlineStr">
         <is>
           <t>Without generating audit records that are specific to the security and mission needs of the organization, it would be difficult to establish, correlate, and investigate the events relating to an incident or identify those responsible for one.
 Audit records can be generated from various components within the information system (e.g., module or policy filter).</t>
         </is>
       </c>
-      <c r="H104" s="3" t="inlineStr">
+      <c r="H104" s="2" t="inlineStr">
         <is>
           <t>Auditing file deletions will create an audit trail for files that are removed
 from the system. The audit trail could aid in system troubleshooting, as well as, detecting
 malicious processes that attempt to delete log files to conceal their presence.</t>
         </is>
       </c>
-      <c r="I104" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J104" s="3" t="inlineStr">
+      <c r="I104" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J104" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system generates audit records when successful/unsuccessful attempts to delete privileges occur. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K104" s="3" t="inlineStr">
+      <c r="K104" s="2" t="inlineStr">
         <is>
           <t>To determine if the system is configured to audit calls to the
  unlink  system call, run the following command:
@@ -8565,72 +8589,80 @@
 If no line is returned, then this is a finding.</t>
         </is>
       </c>
-      <c r="L104" s="3" t="n"/>
-      <c r="M104" s="3" t="inlineStr"/>
-      <c r="N104" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O104" s="3" t="n"/>
-      <c r="P104" s="3" t="n"/>
-      <c r="Q104" s="3" t="n"/>
+      <c r="L104" s="2" t="n"/>
+      <c r="M104" s="2" t="inlineStr">
+        <is>
+          <t>Configure the audit system to generate an audit event for any successful/unsuccessful use of the "unlink" command by adding or updating the following rules in the "/etc/audit/rules.d/audit.rules" file:
+-a always,exit -F arch=b32 -S unlink -F auid&gt;=1000 -F auid!=unset -k delete
+-a always,exit -F arch=b64 -S unlink -F auid&gt;=1000 -F auid!=unset -k delete
+It's allowed to group this system call within the same line as "rename", "unlink", "rmdir", "renameat", and "unlinkat".
+The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
+      <c r="N104" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O104" s="2" t="n"/>
+      <c r="P104" s="2" t="n"/>
+      <c r="Q104" s="2" t="n"/>
     </row>
     <row r="105" ht="130" customHeight="1">
-      <c r="A105" s="3" t="inlineStr">
-        <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
-        </is>
-      </c>
-      <c r="B105" s="3" t="inlineStr">
+      <c r="A105" s="2" t="inlineStr">
+        <is>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+        </is>
+      </c>
+      <c r="B105" s="2" t="inlineStr">
         <is>
           <t>CCI-000169,CCI-000172,CCI-000366,CCI-002884</t>
         </is>
       </c>
-      <c r="C105" s="3" t="inlineStr">
+      <c r="C105" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000466-GPOS-00210,SRG-OS-000467-GPOS-00211,SRG-OS-000468-GPOS-00212</t>
         </is>
       </c>
-      <c r="D105" s="3" t="inlineStr">
+      <c r="D105" s="2" t="inlineStr">
         <is>
           <t>CCE-83755-9</t>
         </is>
       </c>
-      <c r="E105" s="3" t="inlineStr">
+      <c r="E105" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
-      <c r="F105" s="3" t="inlineStr">
+      <c r="F105" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
-      <c r="G105" s="3" t="inlineStr">
+      <c r="G105" s="2" t="inlineStr">
         <is>
           <t>Without generating audit records that are specific to the security and mission needs of the organization, it would be difficult to establish, correlate, and investigate the events relating to an incident or identify those responsible for one.
 Audit records can be generated from various components within the information system (e.g., module or policy filter).</t>
         </is>
       </c>
-      <c r="H105" s="3" t="inlineStr">
+      <c r="H105" s="2" t="inlineStr">
         <is>
           <t>Auditing file deletions will create an audit trail for files that are removed
 from the system. The audit trail could aid in system troubleshooting, as well as, detecting
 malicious processes that attempt to delete log files to conceal their presence.</t>
         </is>
       </c>
-      <c r="I105" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J105" s="3" t="inlineStr">
+      <c r="I105" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J105" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system generates audit records when successful/unsuccessful attempts to delete privileges occur. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K105" s="3" t="inlineStr">
+      <c r="K105" s="2" t="inlineStr">
         <is>
           <t>To determine if the system is configured to audit calls to the
  unlinkat  system call, run the following command:
@@ -8639,21 +8671,29 @@
 If no line is returned, then this is a finding.</t>
         </is>
       </c>
-      <c r="L105" s="3" t="n"/>
-      <c r="M105" s="3" t="inlineStr"/>
-      <c r="N105" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O105" s="3" t="n"/>
-      <c r="P105" s="3" t="n"/>
-      <c r="Q105" s="3" t="n"/>
+      <c r="L105" s="2" t="n"/>
+      <c r="M105" s="2" t="inlineStr">
+        <is>
+          <t>Configure the audit system to generate an audit event for any successful/unsuccessful use of the "unlinkat" command by adding or updating the following rules in the "/etc/audit/rules.d/audit.rules" file:
+-a always,exit -F arch=b32 -S unlinkat -F auid&gt;=1000 -F auid!=unset -k delete
+-a always,exit -F arch=b64 -S unlinkat -F auid&gt;=1000 -F auid!=unset -k delete
+It's allowed to group this system call within the same line as "rename", "unlink", "rmdir", "renameat", and "unlinkat".
+The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
+      <c r="N105" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O105" s="2" t="n"/>
+      <c r="P105" s="2" t="n"/>
+      <c r="Q105" s="2" t="n"/>
     </row>
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -8733,7 +8773,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -8813,7 +8853,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -9562,7 +9602,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>SC-8,MA-4 c,AC-17 (2),SC-13</t>
+          <t>AC-17 (2),SC-13,SC-8,MA-4 c</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9722,7 +9762,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9878,7 +9918,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10234,7 +10274,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -10314,7 +10354,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11081,7 +11121,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11162,7 +11202,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11248,7 +11288,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11694,7 +11734,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
@@ -11774,7 +11814,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B145" s="3" t="inlineStr">
@@ -11854,7 +11894,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
@@ -12950,7 +12990,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13027,7 +13067,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13100,7 +13140,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13173,7 +13213,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13258,7 +13298,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13333,7 +13373,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13408,7 +13448,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13483,7 +13523,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13986,7 +14026,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14275,7 +14315,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14350,7 +14390,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14432,7 +14472,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14514,7 +14554,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14596,7 +14636,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14678,7 +14718,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14760,7 +14800,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14842,7 +14882,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -14924,7 +14964,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15006,7 +15046,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15166,7 +15206,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15245,7 +15285,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15327,7 +15367,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15409,7 +15449,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15491,7 +15531,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15573,7 +15613,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15655,7 +15695,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15737,7 +15777,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
@@ -15812,7 +15852,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
@@ -15885,7 +15925,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
@@ -15962,7 +16002,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (1)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (1),IA-2 (2)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16049,7 +16089,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2,IA-2 (4),IA-2 (5)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (5),IA-2,IA-2 (2)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16138,7 +16178,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2,IA-2 (4),IA-2 (5)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (5),IA-2,IA-2 (2)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16382,7 +16422,7 @@
     <row r="204" ht="130" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
@@ -16824,7 +16864,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16901,7 +16941,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16987,7 +17027,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17147,7 +17187,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
@@ -17755,7 +17795,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17915,7 +17955,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
@@ -18001,7 +18041,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18371,7 +18411,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>IA-2,IA-8,AU-3 (1)</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19667,7 +19707,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="3" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B245" s="3" t="inlineStr">
@@ -20222,7 +20262,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -21460,7 +21500,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -21542,7 +21582,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (8),AC-6 (9)</t>
+          <t>AC-6 (9),AC-6 (8)</t>
         </is>
       </c>
       <c r="B268" s="3" t="inlineStr">
@@ -22136,7 +22176,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B276" s="3" t="inlineStr">
@@ -22209,7 +22249,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22894,7 +22934,7 @@
     <row r="285" ht="130" customHeight="1">
       <c r="A285" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B285" s="3" t="inlineStr">
@@ -24179,7 +24219,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
+          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B302" s="3" t="inlineStr">
@@ -24396,7 +24436,7 @@
     <row r="304" ht="130" customHeight="1">
       <c r="A304" s="3" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B304" s="3" t="inlineStr">
@@ -27758,7 +27798,7 @@
     <row r="349" ht="130" customHeight="1">
       <c r="A349" s="3" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B349" s="3" t="inlineStr">
@@ -30613,7 +30653,7 @@
     <row r="387" ht="130" customHeight="1">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
@@ -31007,7 +31047,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -33584,7 +33624,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="3" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B422" s="3" t="inlineStr">
@@ -33659,7 +33699,7 @@
     <row r="423" ht="130" customHeight="1">
       <c r="A423" s="3" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B423" s="3" t="inlineStr">
@@ -34346,7 +34386,7 @@
     <row r="432" ht="130" customHeight="1">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
@@ -34949,7 +34989,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35701,7 +35741,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="3" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B449" s="3" t="inlineStr">
@@ -35778,7 +35818,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="3" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B450" s="3" t="inlineStr">
@@ -37328,7 +37368,7 @@
     <row r="471" ht="130" customHeight="1">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-17 (2)</t>
+          <t>AC-17 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
@@ -38630,7 +38670,7 @@
     <row r="488" ht="130" customHeight="1">
       <c r="A488" s="3" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B488" s="3" t="inlineStr">
@@ -41215,7 +41255,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">
@@ -42405,7 +42445,7 @@
     <row r="535" ht="130" customHeight="1">
       <c r="A535" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B535" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@10f80dd42baf76106d7323f753daef9720667ce9 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3,AU-7 (1),AU-14 (1),AU-6 (4),AU-3 (1),AU-12 a,CM-5 (1),MA-4 (1) (a),AU-7 a</t>
+          <t>CM-5 (1),AU-3,AU-6 (4),AU-3 (1),CM-6 b,AU-7 (1),AU-12 a,MA-4 (1) (a),AU-7 a,AU-14 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1770,7 +1770,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2214,7 +2214,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-14 (1),AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a),AU-14 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -4170,7 +4170,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -4240,7 +4240,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -4320,7 +4320,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4645,7 +4645,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4737,7 +4737,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4821,7 +4821,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4896,7 +4896,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -4971,7 +4971,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5046,7 +5046,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5121,7 +5121,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -5196,7 +5196,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -5271,7 +5271,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -5346,7 +5346,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -5421,7 +5421,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -5496,7 +5496,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 c,AU-7 b,AU-12 (3),AU-12 a,CM-5 (1),AU-8 b,AU-7 a</t>
+          <t>CM-5 (1),AU-12 (3),AU-12 c,AU-8 b,AU-12 a,AU-7 a,CM-6 b,AU-7 b</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5570,7 +5570,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5732,7 +5732,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5814,7 +5814,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5978,7 +5978,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6060,7 +6060,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6142,7 +6142,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -7180,7 +7180,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7254,7 +7254,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7328,7 +7328,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -7402,7 +7402,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7482,7 +7482,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -7643,7 +7643,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7826,7 +7826,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -7978,7 +7978,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -8053,7 +8053,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -8128,7 +8128,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -8203,7 +8203,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -8283,7 +8283,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8365,7 +8365,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8447,7 +8447,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8529,7 +8529,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8611,7 +8611,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8693,7 +8693,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -8773,7 +8773,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -8853,7 +8853,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -9104,7 +9104,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9602,7 +9602,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-13,SC-8,MA-4 c</t>
+          <t>SC-13,AC-17 (2),SC-8,MA-4 c</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9684,7 +9684,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
@@ -9762,7 +9762,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9840,7 +9840,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9918,7 +9918,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10274,7 +10274,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -11654,7 +11654,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="3" t="inlineStr">
@@ -11734,7 +11734,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
@@ -11814,7 +11814,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B145" s="3" t="inlineStr">
@@ -11894,7 +11894,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
@@ -12206,7 +12206,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12593,7 +12593,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -12669,7 +12669,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12754,7 +12754,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12990,7 +12990,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13067,7 +13067,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13140,7 +13140,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13213,7 +13213,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13298,7 +13298,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13373,7 +13373,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13448,7 +13448,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13523,7 +13523,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -14026,7 +14026,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14315,7 +14315,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15046,7 +15046,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15128,7 +15128,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15206,7 +15206,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15695,7 +15695,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15777,7 +15777,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
@@ -15852,7 +15852,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B197" s="3" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
@@ -16002,7 +16002,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (1),IA-2 (2)</t>
+          <t>IA-2 (4),IA-2 (3),IA-2 (1),IA-2 (2)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16089,7 +16089,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (5),IA-2,IA-2 (2)</t>
+          <t>IA-2 (4),IA-2 (5),IA-2 (3),IA-2,IA-2 (2)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16178,7 +16178,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (5),IA-2,IA-2 (2)</t>
+          <t>IA-2 (4),IA-2 (5),IA-2 (3),IA-2,IA-2 (2)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16422,7 +16422,7 @@
     <row r="204" ht="130" customHeight="1">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
@@ -16864,7 +16864,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16941,7 +16941,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -17027,7 +17027,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>SC-8,AC-18 (1),SC-8 (1)</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17955,7 +17955,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
@@ -18221,7 +18221,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18313,7 +18313,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18411,7 +18411,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-8,AU-3 (1)</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19385,7 +19385,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B241" s="3" t="inlineStr">
@@ -19545,7 +19545,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20911,7 +20911,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
@@ -20999,7 +20999,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="3" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B261" s="3" t="inlineStr">
@@ -21500,7 +21500,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -21662,7 +21662,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B269" s="3" t="inlineStr">
@@ -22934,7 +22934,7 @@
     <row r="285" ht="130" customHeight="1">
       <c r="A285" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B285" s="3" t="inlineStr">
@@ -24219,7 +24219,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="3" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B302" s="3" t="inlineStr">
@@ -28681,7 +28681,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B361" s="3" t="inlineStr">
@@ -30409,7 +30409,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B384" s="3" t="inlineStr">
@@ -30653,7 +30653,7 @@
     <row r="387" ht="130" customHeight="1">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
@@ -31047,7 +31047,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -31125,7 +31125,7 @@
     <row r="393" ht="130" customHeight="1">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
@@ -33624,7 +33624,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="3" t="inlineStr">
@@ -33699,7 +33699,7 @@
     <row r="423" ht="130" customHeight="1">
       <c r="A423" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B423" s="3" t="inlineStr">
@@ -34386,7 +34386,7 @@
     <row r="432" ht="130" customHeight="1">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
@@ -34567,7 +34567,7 @@
     <row r="434" ht="130" customHeight="1">
       <c r="A434" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B434" s="3" t="inlineStr">
@@ -34654,7 +34654,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B435" s="3" t="inlineStr">
@@ -34989,7 +34989,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35741,7 +35741,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B449" s="3" t="inlineStr">
@@ -35818,7 +35818,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="3" t="inlineStr">
@@ -37138,7 +37138,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (7),MA-4 e,SC-10,AC-12</t>
+          <t>MA-4 (7),SC-10,AC-12,MA-4 e</t>
         </is>
       </c>
       <c r="B468" s="3" t="inlineStr">
@@ -37213,7 +37213,7 @@
     <row r="469" ht="130" customHeight="1">
       <c r="A469" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B469" s="3" t="inlineStr">
@@ -37292,7 +37292,7 @@
     <row r="470" ht="130" customHeight="1">
       <c r="A470" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B470" s="3" t="inlineStr">
@@ -37368,7 +37368,7 @@
     <row r="471" ht="130" customHeight="1">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8 (1),SC-8</t>
+          <t>AC-17 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
@@ -38670,7 +38670,7 @@
     <row r="488" ht="130" customHeight="1">
       <c r="A488" s="3" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B488" s="3" t="inlineStr">
@@ -38960,7 +38960,7 @@
     <row r="492" ht="130" customHeight="1">
       <c r="A492" s="3" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B492" s="3" t="inlineStr">
@@ -39977,7 +39977,7 @@
     <row r="505" ht="130" customHeight="1">
       <c r="A505" s="3" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B505" s="3" t="inlineStr">
@@ -40222,7 +40222,7 @@
     <row r="508" ht="130" customHeight="1">
       <c r="A508" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B508" s="2" t="inlineStr">
@@ -40324,7 +40324,7 @@
     <row r="509" ht="130" customHeight="1">
       <c r="A509" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B509" s="2" t="inlineStr">
@@ -40434,7 +40434,7 @@
     <row r="510" ht="130" customHeight="1">
       <c r="A510" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B510" s="2" t="inlineStr">
@@ -40545,7 +40545,7 @@
     <row r="511" ht="130" customHeight="1">
       <c r="A511" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B511" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@0fdf0ae68f37812c5bd9de42f5d51b2d85e86c75 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,CM-6 b,AU-6 (4),AU-7 a,AU-14 (1),CM-5 (1),AU-7 (1),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-6 (4),CM-6 b,AU-7 a,AU-7 (1),AU-3,AU-14 (1),CM-5 (1),MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1770,7 +1770,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2214,7 +2214,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-14 (1),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,AU-14 (1),MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3438,7 +3438,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-12 a,CM-6 b,AU-7 a,CM-5 (1),AU-12 c,AU-8 b,AU-7 b</t>
+          <t>AU-12 (3),CM-6 b,CM-5 (1),AU-12 c,AU-8 b,AU-7 b,AU-7 a,AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8606,7 +8606,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8777,7 +8777,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8856,7 +8856,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8935,7 +8935,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9022,7 +9022,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9109,7 +9109,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8,MA-4 c,SC-13</t>
+          <t>MA-4 c,SC-8,AC-17 (2),SC-13</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10106,7 +10106,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10873,7 +10873,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10954,7 +10954,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11040,7 +11040,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12268,7 +12268,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (4),IA-2 (3),IA-2 (1),IA-2 (2)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2,IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (3),IA-2 (2),IA-2,IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2,IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (3),IA-2 (2),IA-2,IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16258,7 +16258,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16887,7 +16887,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16976,7 +16976,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17389,7 +17389,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
@@ -17475,7 +17475,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17655,7 +17655,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -17747,7 +17747,7 @@
     <row r="219" ht="130" customHeight="1">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B219" s="2" t="inlineStr">
@@ -20300,7 +20300,7 @@
     <row r="250" ht="130" customHeight="1">
       <c r="A250" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B250" s="2" t="inlineStr">
@@ -20970,7 +20970,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -21132,7 +21132,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
@@ -21646,7 +21646,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B267" s="3" t="inlineStr">
@@ -23701,7 +23701,7 @@
     <row r="293" ht="130" customHeight="1">
       <c r="A293" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B293" s="3" t="inlineStr">
@@ -23918,7 +23918,7 @@
     <row r="295" ht="130" customHeight="1">
       <c r="A295" s="3" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B295" s="3" t="inlineStr">
@@ -29899,7 +29899,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="3" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B375" s="3" t="inlineStr">
@@ -30537,7 +30537,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (9),CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -35733,7 +35733,7 @@
     <row r="446" ht="130" customHeight="1">
       <c r="A446" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B446" s="3" t="inlineStr">
@@ -36380,7 +36380,7 @@
     <row r="455" ht="130" customHeight="1">
       <c r="A455" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B455" s="3" t="inlineStr">
@@ -36671,7 +36671,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
+          <t>AC-12,MA-4 e,SC-10,MA-4 (7)</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36978,7 +36978,7 @@
     <row r="463" ht="130" customHeight="1">
       <c r="A463" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8 (1),SC-8</t>
+          <t>SC-8,SC-8 (1),AC-17 (2)</t>
         </is>
       </c>
       <c r="B463" s="2" t="inlineStr">
@@ -39722,7 +39722,7 @@
     <row r="498" ht="130" customHeight="1">
       <c r="A498" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B498" s="2" t="inlineStr">
@@ -41367,7 +41367,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">
@@ -42557,7 +42557,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@2c4c03eb40c43ef361248d732c303f7e51147fca 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-12 a,CM-6 b,AU-3 (1),AU-7 (1),AU-3,AU-7 a,AU-14 (1),MA-4 (1) (a),CM-5 (1)</t>
+          <t>AU-7 (1),AU-14 (1),AU-3 (1),CM-5 (1),CM-6 b,AU-3,AU-6 (4),MA-4 (1) (a),AU-12 a,AU-7 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1770,7 +1770,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2214,7 +2214,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,AU-14 (1),MA-4 (1) (a)</t>
+          <t>AU-14 (1),AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3438,7 +3438,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-7 b,CM-6 b,AU-12 (3),AU-8 b,AU-12 c,AU-7 a,CM-5 (1)</t>
+          <t>AU-8 b,AU-12 (3),CM-5 (1),AU-7 b,CM-6 b,AU-12 a,AU-7 a,AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7155,7 +7155,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -7240,7 +7240,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7316,7 +7316,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8606,7 +8606,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8856,7 +8856,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8935,7 +8935,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9022,7 +9022,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9109,7 +9109,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-13,MA-4 c,AC-17 (2)</t>
+          <t>SC-13,AC-17 (2),SC-8,MA-4 c</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9436,7 +9436,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9592,7 +9592,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -9750,7 +9750,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -9819,7 +9819,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -9888,7 +9888,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -9957,7 +9957,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10106,7 +10106,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -11133,7 +11133,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),AC-6 (10)</t>
+          <t>AC-6 (10),AC-3 (4)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11230,7 +11230,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),AC-6 (10)</t>
+          <t>AC-6 (10),AC-3 (4)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11406,7 +11406,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -11958,7 +11958,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12268,7 +12268,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12429,7 +12429,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12505,7 +12505,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12590,7 +12590,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12747,7 +12747,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13434,7 +13434,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13505,7 +13505,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13576,7 +13576,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13648,7 +13648,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
@@ -13719,7 +13719,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
@@ -13790,7 +13790,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -13937,7 +13937,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
@@ -14008,7 +14008,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
@@ -14079,7 +14079,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2,IA-2 (5),IA-2 (4)</t>
+          <t>IA-2 (5),IA-2 (2),IA-2,IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2,IA-2 (5),IA-2 (4)</t>
+          <t>IA-2 (5),IA-2 (2),IA-2,IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16258,7 +16258,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16887,7 +16887,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16976,7 +16976,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17229,7 +17229,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17389,7 +17389,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
@@ -17475,7 +17475,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17655,7 +17655,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -17747,7 +17747,7 @@
     <row r="219" ht="130" customHeight="1">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B219" s="2" t="inlineStr">
@@ -17845,7 +17845,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18824,7 +18824,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b,SC-2</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19170,7 +19170,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -19732,7 +19732,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20300,7 +20300,7 @@
     <row r="250" ht="130" customHeight="1">
       <c r="A250" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B250" s="2" t="inlineStr">
@@ -20556,7 +20556,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -21052,7 +21052,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (8),AC-6 (9)</t>
+          <t>AC-6 (9),AC-6 (8)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -21132,7 +21132,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
@@ -21681,7 +21681,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -22286,45 +22286,45 @@
       <c r="Q273" s="2" t="n"/>
     </row>
     <row r="274" ht="130" customHeight="1">
-      <c r="A274" s="3" t="inlineStr">
+      <c r="A274" s="2" t="inlineStr">
         <is>
           <t>IA-5 (1) (a)</t>
         </is>
       </c>
-      <c r="B274" s="3" t="inlineStr">
+      <c r="B274" s="2" t="inlineStr">
         <is>
           <t>CCI-000192</t>
         </is>
       </c>
-      <c r="C274" s="3" t="inlineStr">
+      <c r="C274" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000069-GPOS-00037</t>
         </is>
       </c>
-      <c r="D274" s="3" t="inlineStr">
+      <c r="D274" s="2" t="inlineStr">
         <is>
           <t>CCE-83568-6</t>
         </is>
       </c>
-      <c r="E274" s="3" t="inlineStr">
+      <c r="E274" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce password complexity by requiring that at least one upper-case character be used.</t>
         </is>
       </c>
-      <c r="F274" s="3" t="inlineStr">
+      <c r="F274" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must enforce password complexity by requiring that at least one upper-case character be used.</t>
         </is>
       </c>
-      <c r="G274" s="3" t="inlineStr">
+      <c r="G274" s="2" t="inlineStr">
         <is>
           <t>Use of a complex password helps to increase the time and resources required to compromise the password. Password complexity, or strength, is a measure of the effectiveness of a password in resisting attempts at guessing and brute-force attacks.
 Password complexity is one factor of several that determines how long it takes to crack a password. The more complex the password, the greater the number of possible combinations that need to be tested before the password is compromised.</t>
         </is>
       </c>
-      <c r="H274" s="3" t="inlineStr">
-        <is>
-          <t>Use of a complex password helps to increase the time and resources reuiqred to compromise the password.
+      <c r="H274" s="2" t="inlineStr">
+        <is>
+          <t>Use of a complex password helps to increase the time and resources required to compromise the password.
 Password complexity, or strength, is a measure of the effectiveness of a password in resisting attempts
 at guessing and brute-force attacks.
 Password complexity is one factor of several that determines how long it takes to crack a password. The more
@@ -22332,41 +22332,46 @@
 the password is compromised.</t>
         </is>
       </c>
-      <c r="I274" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J274" s="3" t="inlineStr">
+      <c r="I274" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J274" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system enforces password complexity by requiring that at least one upper-case character be used. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K274" s="3" t="inlineStr">
+      <c r="K274" s="2" t="inlineStr">
         <is>
           <t>To check how many uppercase characters are required in a password, run the following command:
  $ grep ucredit /etc/security/pwquality.conf 
 The "ucredit" parameter (as a negative number) will indicate how many uppercase characters are required.
-The DoD and FISMA require at least one uppercase character in a password.
 This would appear as "ucredit = -1".
-If ucredit is not found or not set less than or equal to the required value, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L274" s="3" t="n"/>
-      <c r="M274" s="3" t="inlineStr"/>
-      <c r="N274" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O274" s="3" t="n"/>
-      <c r="P274" s="3" t="n"/>
-      <c r="Q274" s="3" t="n"/>
+If ucredit is not found or not set to the required value, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L274" s="2" t="n"/>
+      <c r="M274" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to enforce password complexity by requiring that at least one upper-case character be used by setting the "ucredit" option.
+Add the following line to /etc/security/pwquality.conf (or modify the line to have the required value):
+ucredit = -1</t>
+        </is>
+      </c>
+      <c r="N274" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O274" s="2" t="n"/>
+      <c r="P274" s="2" t="n"/>
+      <c r="Q274" s="2" t="n"/>
     </row>
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -23362,7 +23367,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
@@ -23433,7 +23438,7 @@
     <row r="289" ht="130" customHeight="1">
       <c r="A289" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B289" s="3" t="inlineStr">
@@ -23505,7 +23510,7 @@
     <row r="290" ht="130" customHeight="1">
       <c r="A290" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B290" s="3" t="inlineStr">
@@ -23663,7 +23668,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -23880,7 +23885,7 @@
     <row r="294" ht="130" customHeight="1">
       <c r="A294" s="3" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B294" s="3" t="inlineStr">
@@ -27242,7 +27247,7 @@
     <row r="339" ht="130" customHeight="1">
       <c r="A339" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B339" s="3" t="inlineStr">
@@ -30507,7 +30512,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b,AC-17 (9)</t>
+          <t>CM-6 b,AC-17 (1),AC-17 (9),CM-7 b</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30585,7 +30590,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -34914,7 +34919,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
@@ -35703,7 +35708,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B445" s="3" t="inlineStr">
@@ -36350,7 +36355,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B454" s="3" t="inlineStr">
@@ -36641,7 +36646,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 e,SC-10,MA-4 (7)</t>
+          <t>SC-10,MA-4 (7),AC-12,MA-4 e</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36716,7 +36721,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36795,7 +36800,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -36871,7 +36876,7 @@
     <row r="461" ht="130" customHeight="1">
       <c r="A461" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B461" s="3" t="inlineStr">
@@ -36948,7 +36953,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-17 (2)</t>
+          <t>SC-8,AC-17 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -37746,7 +37751,7 @@
       </c>
       <c r="F472" s="3" t="inlineStr">
         <is>
-          <t>Red Hat Enterprise Linux 9 must display the Standard Mandatory DoD Notice and Consent Banner until users acknowledge the usage conditions and take explicit actions to log on for further access.</t>
+          <t>Red Hat Enterprise Linux 9 must display the Standard Mandatory DoD Notice and Consent Banner until users acknowledge the usage conditions and take explicit actions to log on for further access via CLI and Graphical access.</t>
         </is>
       </c>
       <c r="G472" s="3" t="inlineStr">
@@ -37783,7 +37788,7 @@
       <c r="P472" s="3" t="n"/>
       <c r="Q472" s="3" t="inlineStr">
         <is>
-          <t>Red Hat Enterprise Linux 9 does not have configuration options to meet this requirement.</t>
+          <t>Red Hat Enterprise Linux 9 does not natively support a method of presenting an interactive acknowledgement of the login banner.</t>
         </is>
       </c>
     </row>
@@ -39949,7 +39954,7 @@
     <row r="500" ht="130" customHeight="1">
       <c r="A500" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B500" s="2" t="inlineStr">
@@ -40051,7 +40056,7 @@
     <row r="501" ht="130" customHeight="1">
       <c r="A501" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B501" s="2" t="inlineStr">
@@ -40161,7 +40166,7 @@
     <row r="502" ht="130" customHeight="1">
       <c r="A502" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B502" s="2" t="inlineStr">
@@ -40272,7 +40277,7 @@
     <row r="503" ht="130" customHeight="1">
       <c r="A503" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B503" s="2" t="inlineStr">
@@ -41418,7 +41423,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@b77bb44f19b2f79987727ad201de6ba526ba5d66 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-7 (1),AU-14 (1),AU-3 (1),CM-5 (1),CM-6 b,AU-3,AU-6 (4),MA-4 (1) (a),AU-12 a,AU-7 a</t>
+          <t>AU-7 a,CM-6 b,AU-12 a,MA-4 (1) (a),AU-3,AU-14 (1),CM-5 (1),AU-3 (1),AU-7 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1770,7 +1770,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2214,7 +2214,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-14 (1),AU-3 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
+          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-12 (3),CM-5 (1),AU-7 b,CM-6 b,AU-12 a,AU-7 a,AU-12 c</t>
+          <t>AU-7 b,AU-7 a,AU-12 c,CM-6 b,AU-12 a,CM-5 (1),AU-8 b,AU-12 (3)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5815,7 +5815,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5889,7 +5889,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5972,7 +5972,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -6050,7 +6050,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6141,7 +6141,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6223,7 +6223,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7240,7 +7240,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8777,7 +8777,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-13,AC-17 (2),SC-8,MA-4 c</t>
+          <t>SC-13,MA-4 c,AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9436,7 +9436,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9592,7 +9592,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -9750,7 +9750,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -9819,7 +9819,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -9888,7 +9888,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -9957,7 +9957,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10873,7 +10873,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10954,7 +10954,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11040,7 +11040,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11406,7 +11406,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -11958,7 +11958,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12268,7 +12268,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13434,7 +13434,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13505,7 +13505,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13576,7 +13576,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13648,7 +13648,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
@@ -13719,7 +13719,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
@@ -13790,7 +13790,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -13937,7 +13937,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
@@ -14008,7 +14008,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
@@ -14079,7 +14079,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2,IA-2 (4),IA-2 (3)</t>
+          <t>IA-2,IA-2 (4),IA-2 (5),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2,IA-2 (4),IA-2 (3)</t>
+          <t>IA-2,IA-2 (4),IA-2 (5),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16258,7 +16258,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>SC-8,AC-18 (1),SC-8 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16887,7 +16887,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16976,7 +16976,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17229,7 +17229,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17475,7 +17475,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),CM-6 b,SC-5</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17845,7 +17845,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -19170,7 +19170,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -19732,7 +19732,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20556,7 +20556,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -20643,37 +20643,37 @@
       <c r="Q253" s="2" t="n"/>
     </row>
     <row r="254" ht="130" customHeight="1">
-      <c r="A254" s="3" t="inlineStr">
-        <is>
-          <t>IA-2 (12),IA-2 (11)</t>
-        </is>
-      </c>
-      <c r="B254" s="3" t="inlineStr">
+      <c r="A254" s="2" t="inlineStr">
+        <is>
+          <t>IA-2 (11),IA-2 (12)</t>
+        </is>
+      </c>
+      <c r="B254" s="2" t="inlineStr">
         <is>
           <t>CCI-001954,CCI-001953</t>
         </is>
       </c>
-      <c r="C254" s="3" t="inlineStr">
+      <c r="C254" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000375-GPOS-00160,SRG-OS-000376-GPOS-00161</t>
         </is>
       </c>
-      <c r="D254" s="3" t="inlineStr">
+      <c r="D254" s="2" t="inlineStr">
         <is>
           <t>CCE-83595-9</t>
         </is>
       </c>
-      <c r="E254" s="3" t="inlineStr">
+      <c r="E254" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
         </is>
       </c>
-      <c r="F254" s="3" t="inlineStr">
+      <c r="F254" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
         </is>
       </c>
-      <c r="G254" s="3" t="inlineStr">
+      <c r="G254" s="2" t="inlineStr">
         <is>
           <t>Using an authentication device, such as a CAC or token that is separate from the information system, ensures that even if the information system is compromised, that compromise will not affect credentials stored on the authentication device.
 Multifactor solutions that require devices separate from information systems gaining access include, for example, hardware tokens providing time-based or challenge-response authenticators and smart cards such as the U.S. Government Personal Identity Verification card and the DoD Common Access Card.
@@ -20683,7 +20683,7 @@
 Requires further clarification from NIST.</t>
         </is>
       </c>
-      <c r="H254" s="3" t="inlineStr">
+      <c r="H254" s="2" t="inlineStr">
         <is>
           <t>Using an authentication device, such as a CAC or token that is separate from
 the information system, ensures that even if the information system is
@@ -20696,32 +20696,38 @@
 Access Card.</t>
         </is>
       </c>
-      <c r="I254" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J254" s="3" t="inlineStr">
+      <c r="I254" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J254" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system implements multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K254" s="3" t="inlineStr">
+      <c r="K254" s="2" t="inlineStr">
         <is>
           <t>Run the following command to determine if the  opensc  package is installed:  $ rpm -q opensc 
 If the package is not installed, then this is a finding.</t>
         </is>
       </c>
-      <c r="L254" s="3" t="n"/>
-      <c r="M254" s="3" t="inlineStr"/>
-      <c r="N254" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O254" s="3" t="n"/>
-      <c r="P254" s="3" t="n"/>
-      <c r="Q254" s="3" t="n"/>
+      <c r="L254" s="2" t="n"/>
+      <c r="M254" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+The  opensc  package can be installed with the following command:
+$ sudo dnf install opensc </t>
+        </is>
+      </c>
+      <c r="N254" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O254" s="2" t="n"/>
+      <c r="P254" s="2" t="n"/>
+      <c r="Q254" s="2" t="n"/>
     </row>
     <row r="255" ht="130" customHeight="1">
       <c r="A255" s="3" t="inlineStr">
@@ -20970,7 +20976,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -21052,7 +21058,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-6 (8)</t>
+          <t>AC-6 (8),AC-6 (9)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -21598,7 +21604,7 @@
     <row r="266" ht="130" customHeight="1">
       <c r="A266" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B266" s="2" t="inlineStr">
@@ -22371,7 +22377,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -22519,7 +22525,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22599,7 +22605,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -23367,7 +23373,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
@@ -23438,7 +23444,7 @@
     <row r="289" ht="130" customHeight="1">
       <c r="A289" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B289" s="3" t="inlineStr">
@@ -23510,7 +23516,7 @@
     <row r="290" ht="130" customHeight="1">
       <c r="A290" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B290" s="3" t="inlineStr">
@@ -27247,7 +27253,7 @@
     <row r="339" ht="130" customHeight="1">
       <c r="A339" s="3" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B339" s="3" t="inlineStr">
@@ -27478,7 +27484,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B342" s="3" t="inlineStr">
@@ -27552,7 +27558,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B343" s="3" t="inlineStr">
@@ -30512,7 +30518,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),AC-17 (9),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30590,7 +30596,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -33089,7 +33095,7 @@
     <row r="412" ht="130" customHeight="1">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
@@ -33171,7 +33177,7 @@
     <row r="413" ht="130" customHeight="1">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
@@ -35223,7 +35229,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35313,7 +35319,7 @@
     <row r="440" ht="130" customHeight="1">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
@@ -36646,7 +36652,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>SC-10,MA-4 (7),AC-12,MA-4 e</t>
+          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36721,7 +36727,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36800,7 +36806,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -36876,7 +36882,7 @@
     <row r="461" ht="130" customHeight="1">
       <c r="A461" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B461" s="3" t="inlineStr">
@@ -36953,7 +36959,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),AC-17 (2)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -38261,7 +38267,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -38580,7 +38586,7 @@
     <row r="483" ht="130" customHeight="1">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
@@ -41423,7 +41429,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@4b009c21cbfbdfbec66fbb92c15a4dfab376966f 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-6 b,AU-12 a,MA-4 (1) (a),AU-3,AU-14 (1),CM-5 (1),AU-3 (1),AU-7 (1),AU-6 (4)</t>
+          <t>AU-12 a,AU-6 (4),AU-7 a,AU-14 (1),MA-4 (1) (a),AU-3,AU-3 (1),CM-6 b,AU-7 (1),CM-5 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-14 (1),AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-14 (1),AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3438,7 +3438,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3503,7 +3503,7 @@
       <c r="M39" s="2" t="inlineStr">
         <is>
           <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
-name_format=hostname</t>
+name_format = hostname</t>
         </is>
       </c>
       <c r="N39" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 b,SI-6 d</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4410,7 +4410,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-7 a,AU-12 c,CM-6 b,AU-12 a,CM-5 (1),AU-8 b,AU-12 (3)</t>
+          <t>AU-12 c,AU-12 a,AU-7 a,AU-7 b,AU-8 b,CM-6 b,CM-5 (1),AU-12 (3)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5889,7 +5889,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5972,7 +5972,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -6050,7 +6050,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6141,7 +6141,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6223,7 +6223,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7155,7 +7155,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -7240,7 +7240,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7316,7 +7316,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8606,7 +8606,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8856,7 +8856,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8935,7 +8935,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9022,7 +9022,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9109,7 +9109,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 c,AC-17 (2),SC-8</t>
+          <t>AC-17 (2),MA-4 c,SC-13,SC-8</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10873,7 +10873,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10954,7 +10954,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11040,7 +11040,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11133,7 +11133,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-3 (4)</t>
+          <t>AC-3 (4),AC-6 (10)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11230,7 +11230,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-3 (4)</t>
+          <t>AC-3 (4),AC-6 (10)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12268,7 +12268,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12747,7 +12747,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-12 c,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (4),IA-2 (1),IA-2 (2),IA-2 (3)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (4),IA-2 (5),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (3),IA-2,IA-2 (5),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (4),IA-2 (5),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (3),IA-2,IA-2 (5),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16258,7 +16258,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16887,7 +16887,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16976,7 +16976,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17229,7 +17229,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17387,37 +17387,37 @@
       <c r="Q214" s="3" t="n"/>
     </row>
     <row r="215" ht="130" customHeight="1">
-      <c r="A215" s="3" t="inlineStr">
-        <is>
-          <t>AU-12 a,CM-6 b</t>
-        </is>
-      </c>
-      <c r="B215" s="3" t="inlineStr">
+      <c r="A215" s="2" t="inlineStr">
+        <is>
+          <t>CM-6 b,AU-12 a</t>
+        </is>
+      </c>
+      <c r="B215" s="2" t="inlineStr">
         <is>
           <t>CCI-000366</t>
         </is>
       </c>
-      <c r="C215" s="3" t="inlineStr">
+      <c r="C215" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000062-GPOS-00031,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D215" s="3" t="inlineStr">
+      <c r="D215" s="2" t="inlineStr">
         <is>
           <t>CCE-83682-5</t>
         </is>
       </c>
-      <c r="E215" s="3" t="inlineStr">
+      <c r="E215" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
         </is>
       </c>
-      <c r="F215" s="3" t="inlineStr">
+      <c r="F215" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
         </is>
       </c>
-      <c r="G215" s="3" t="inlineStr">
+      <c r="G215" s="2" t="inlineStr">
         <is>
           <t>Without the capability to generate audit records, it would be difficult to establish, correlate, and investigate the events relating to an incident or identify those responsible for one.
 Audit records can be generated from various components within the information system (e.g., module or policy filter).
@@ -17429,18 +17429,18 @@
 4) All kernel module load, unload, and restart actions.</t>
         </is>
       </c>
-      <c r="H215" s="3" t="inlineStr">
+      <c r="H215" s="2" t="inlineStr">
         <is>
           <t>If option "local_events" isn't set to "yes" only events from
 network will be aggregated.</t>
         </is>
       </c>
-      <c r="I215" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J215" s="3" t="inlineStr">
+      <c r="I215" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J215" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system provides audit record generation capability for DoD-defined auditable events for all operating system components. 
 DoD has defined the list of events for which the operating system will provide an audit record generation capability as the following: 
@@ -17451,7 +17451,7 @@
 If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K215" s="3" t="inlineStr">
+      <c r="K215" s="2" t="inlineStr">
         <is>
           <t>To verify that Audit Daemon is configured to include local events, run the
 following command:
@@ -17461,21 +17461,26 @@
 If local_events isn't set to yes, then this is a finding.</t>
         </is>
       </c>
-      <c r="L215" s="3" t="n"/>
-      <c r="M215" s="3" t="inlineStr"/>
-      <c r="N215" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O215" s="3" t="n"/>
-      <c r="P215" s="3" t="n"/>
-      <c r="Q215" s="3" t="n"/>
+      <c r="L215" s="2" t="n"/>
+      <c r="M215" s="2" t="inlineStr">
+        <is>
+          <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
+local_events = yes</t>
+        </is>
+      </c>
+      <c r="N215" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O215" s="2" t="n"/>
+      <c r="P215" s="2" t="n"/>
+      <c r="Q215" s="2" t="n"/>
     </row>
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17655,7 +17660,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -17747,7 +17752,7 @@
     <row r="219" ht="130" customHeight="1">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B219" s="2" t="inlineStr">
@@ -17845,7 +17850,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18824,7 +18829,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>SI-16,SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19170,7 +19175,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -19252,61 +19257,61 @@
       <c r="Q236" s="2" t="n"/>
     </row>
     <row r="237" ht="130" customHeight="1">
-      <c r="A237" s="3" t="inlineStr">
+      <c r="A237" s="2" t="inlineStr">
         <is>
           <t>AU-6 (4)</t>
         </is>
       </c>
-      <c r="B237" s="3" t="inlineStr">
+      <c r="B237" s="2" t="inlineStr">
         <is>
           <t>CCI-000154</t>
         </is>
       </c>
-      <c r="C237" s="3" t="inlineStr">
+      <c r="C237" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000051-GPOS-00024</t>
         </is>
       </c>
-      <c r="D237" s="3" t="inlineStr">
+      <c r="D237" s="2" t="inlineStr">
         <is>
           <t>CCE-83704-7</t>
         </is>
       </c>
-      <c r="E237" s="3" t="inlineStr">
+      <c r="E237" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
         </is>
       </c>
-      <c r="F237" s="3" t="inlineStr">
+      <c r="F237" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
         </is>
       </c>
-      <c r="G237" s="3" t="inlineStr">
+      <c r="G237" s="2" t="inlineStr">
         <is>
           <t>Successful incident response and auditing relies on timely, accurate system information and analysis in order to allow the organization to identify and respond to potential incidents in a proficient manner. If the operating system does not provide the ability to centrally review the operating system logs, forensic analysis is negatively impacted.
 Segregation of logging data to multiple disparate computer systems is counterproductive and makes log analysis and log event alarming difficult to implement and manage, particularly when the system has multiple logging components writing to different locations or systems.
 To support the centralized capability, the operating system must be able to provide the information in a format that can be extracted and used, allowing the application performing the centralization of the log records to meet this requirement.</t>
         </is>
       </c>
-      <c r="H237" s="3" t="inlineStr">
+      <c r="H237" s="2" t="inlineStr">
         <is>
           <t>If option "freq" isn't set to "50", the flush to disk
 may happen after higher number of records, increasing the danger
 of audit loss.</t>
         </is>
       </c>
-      <c r="I237" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J237" s="3" t="inlineStr">
+      <c r="I237" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J237" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system provides the capability to centrally review and analyze audit records from multiple components within the system. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K237" s="3" t="inlineStr">
+      <c r="K237" s="2" t="inlineStr">
         <is>
           <t>To verify that Audit Daemon is configured to flush to disk after
 every 50 records, run the following command:
@@ -19316,16 +19321,21 @@
 If freq isn't set to 50, then this is a finding.</t>
         </is>
       </c>
-      <c r="L237" s="3" t="n"/>
-      <c r="M237" s="3" t="inlineStr"/>
-      <c r="N237" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O237" s="3" t="n"/>
-      <c r="P237" s="3" t="n"/>
-      <c r="Q237" s="3" t="n"/>
+      <c r="L237" s="2" t="n"/>
+      <c r="M237" s="2" t="inlineStr">
+        <is>
+          <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
+freq = 50</t>
+        </is>
+      </c>
+      <c r="N237" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O237" s="2" t="n"/>
+      <c r="P237" s="2" t="n"/>
+      <c r="Q237" s="2" t="n"/>
     </row>
     <row r="238" ht="130" customHeight="1">
       <c r="A238" s="2" t="inlineStr">
@@ -20556,7 +20566,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -21604,7 +21614,7 @@
     <row r="266" ht="130" customHeight="1">
       <c r="A266" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B266" s="2" t="inlineStr">
@@ -21687,7 +21697,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -22377,7 +22387,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -22525,7 +22535,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22605,7 +22615,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -23373,7 +23383,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
@@ -23444,7 +23454,7 @@
     <row r="289" ht="130" customHeight="1">
       <c r="A289" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B289" s="3" t="inlineStr">
@@ -23516,7 +23526,7 @@
     <row r="290" ht="130" customHeight="1">
       <c r="A290" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B290" s="3" t="inlineStr">
@@ -23674,7 +23684,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -23891,7 +23901,7 @@
     <row r="294" ht="130" customHeight="1">
       <c r="A294" s="3" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B294" s="3" t="inlineStr">
@@ -27484,7 +27494,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B342" s="3" t="inlineStr">
@@ -27558,7 +27568,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B343" s="3" t="inlineStr">
@@ -28143,7 +28153,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -29878,59 +29888,59 @@
       <c r="Q373" s="3" t="n"/>
     </row>
     <row r="374" ht="130" customHeight="1">
-      <c r="A374" s="3" t="inlineStr">
+      <c r="A374" s="2" t="inlineStr">
         <is>
           <t>CM-6 b,AU-3</t>
         </is>
       </c>
-      <c r="B374" s="3" t="inlineStr">
+      <c r="B374" s="2" t="inlineStr">
         <is>
           <t>CCI-000366</t>
         </is>
       </c>
-      <c r="C374" s="3" t="inlineStr">
+      <c r="C374" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000255-GPOS-00096,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D374" s="3" t="inlineStr">
+      <c r="D374" s="2" t="inlineStr">
         <is>
           <t>CCE-83696-5</t>
         </is>
       </c>
-      <c r="E374" s="3" t="inlineStr">
+      <c r="E374" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
-      <c r="F374" s="3" t="inlineStr">
+      <c r="F374" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
-      <c r="G374" s="3" t="inlineStr">
+      <c r="G374" s="2" t="inlineStr">
         <is>
           <t>Configuring the operating system to implement organization-wide security implementation guides and security checklists ensures compliance with federal standards and establishes a common security baseline across DoD that reflects the most restrictive security posture consistent with operational requirements.
 Configuration settings are the set of parameters that can be changed in hardware, software, or firmware components of the system that affect the security posture and/or functionality of the system. Security-related parameters are those parameters impacting the security state of the system, including the parameters required to satisfy other security control requirements. Security-related parameters include, for example: registry settings; account, file, directory permission settings; and settings for functions, ports, protocols, services, and remote connections.</t>
         </is>
       </c>
-      <c r="H374" s="3" t="inlineStr">
+      <c r="H374" s="2" t="inlineStr">
         <is>
           <t>If option "log_format" isn't set to "ENRICHED", the
 audit records will be stored in a format exactly as the kernel sends them.</t>
         </is>
       </c>
-      <c r="I374" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J374" s="3" t="inlineStr">
+      <c r="I374" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J374" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system is configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs. If it is not, this is a finding.</t>
         </is>
       </c>
-      <c r="K374" s="3" t="inlineStr">
+      <c r="K374" s="2" t="inlineStr">
         <is>
           <t>To verify that Audit Daemon is configured to resolve all uid, gid, syscall,
 architecture, and socket address information before writing the event to disk,
@@ -29941,71 +29951,76 @@
 If log_format isn't set to ENRICHED, then this is a finding.</t>
         </is>
       </c>
-      <c r="L374" s="3" t="n"/>
-      <c r="M374" s="3" t="inlineStr"/>
-      <c r="N374" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O374" s="3" t="n"/>
-      <c r="P374" s="3" t="n"/>
-      <c r="Q374" s="3" t="n"/>
+      <c r="L374" s="2" t="n"/>
+      <c r="M374" s="2" t="inlineStr">
+        <is>
+          <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
+log_format = ENRICHED</t>
+        </is>
+      </c>
+      <c r="N374" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O374" s="2" t="n"/>
+      <c r="P374" s="2" t="n"/>
+      <c r="Q374" s="2" t="n"/>
     </row>
     <row r="375" ht="130" customHeight="1">
-      <c r="A375" s="3" t="inlineStr">
+      <c r="A375" s="2" t="inlineStr">
         <is>
           <t>CM-6 b</t>
         </is>
       </c>
-      <c r="B375" s="3" t="inlineStr">
+      <c r="B375" s="2" t="inlineStr">
         <is>
           <t>CCI-000366</t>
         </is>
       </c>
-      <c r="C375" s="3" t="inlineStr">
+      <c r="C375" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D375" s="3" t="inlineStr">
+      <c r="D375" s="2" t="inlineStr">
         <is>
           <t>CCE-83705-4</t>
         </is>
       </c>
-      <c r="E375" s="3" t="inlineStr">
+      <c r="E375" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
-      <c r="F375" s="3" t="inlineStr">
+      <c r="F375" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
-      <c r="G375" s="3" t="inlineStr">
+      <c r="G375" s="2" t="inlineStr">
         <is>
           <t>Configuring the operating system to implement organization-wide security implementation guides and security checklists ensures compliance with federal standards and establishes a common security baseline across DoD that reflects the most restrictive security posture consistent with operational requirements.
 Configuration settings are the set of parameters that can be changed in hardware, software, or firmware components of the system that affect the security posture and/or functionality of the system. Security-related parameters are those parameters impacting the security state of the system, including the parameters required to satisfy other security control requirements. Security-related parameters include, for example: registry settings; account, file, directory permission settings; and settings for functions, ports, protocols, services, and remote connections.</t>
         </is>
       </c>
-      <c r="H375" s="3" t="inlineStr">
+      <c r="H375" s="2" t="inlineStr">
         <is>
           <t>If "write_logs" isn't set to "yes", the Audit logs will
 not be written to the disk.</t>
         </is>
       </c>
-      <c r="I375" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J375" s="3" t="inlineStr">
+      <c r="I375" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J375" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system is configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs. If it is not, this is a finding.</t>
         </is>
       </c>
-      <c r="K375" s="3" t="inlineStr">
+      <c r="K375" s="2" t="inlineStr">
         <is>
           <t>To verify that Audit Daemon is configured to write logs to the disk, run the
 following command:
@@ -30015,16 +30030,21 @@
 If write_logs isn't set to yes, then this is a finding.</t>
         </is>
       </c>
-      <c r="L375" s="3" t="n"/>
-      <c r="M375" s="3" t="inlineStr"/>
-      <c r="N375" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O375" s="3" t="n"/>
-      <c r="P375" s="3" t="n"/>
-      <c r="Q375" s="3" t="n"/>
+      <c r="L375" s="2" t="n"/>
+      <c r="M375" s="2" t="inlineStr">
+        <is>
+          <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
+write_logs = yes</t>
+        </is>
+      </c>
+      <c r="N375" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O375" s="2" t="n"/>
+      <c r="P375" s="2" t="n"/>
+      <c r="Q375" s="2" t="n"/>
     </row>
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="3" t="inlineStr">
@@ -30518,7 +30538,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
+          <t>CM-6 b,AC-17 (9),AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30596,7 +30616,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -34925,7 +34945,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
@@ -35714,7 +35734,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B445" s="3" t="inlineStr">
@@ -36361,7 +36381,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B454" s="3" t="inlineStr">
@@ -36652,7 +36672,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
+          <t>MA-4 e,MA-4 (7),SC-10,AC-12</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36727,7 +36747,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36806,7 +36826,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -36959,7 +36979,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-17 (2)</t>
+          <t>AC-17 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -38267,7 +38287,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -38586,7 +38606,7 @@
     <row r="483" ht="130" customHeight="1">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
@@ -42619,7 +42639,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@36b4f501a63d0d344733b36a91e7d63839ce31f4 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -971,37 +971,37 @@
       <c r="Q6" s="2" t="n"/>
     </row>
     <row r="7" ht="130" customHeight="1">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>AU-5 b,AU-5 a</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>AU-5 a,AU-5 b</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>CCI-000139,CCI-000140</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000046-GPOS-00022,SRG-OS-000047-GPOS-00023</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>CCE-83709-6</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>The operating system must shut down by default upon audit failure (unless availability is an overriding concern).</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must shut down by default upon audit failure (unless availability is an overriding concern).</t>
         </is>
       </c>
-      <c r="G7" s="3" t="inlineStr">
+      <c r="G7" s="2" t="inlineStr">
         <is>
           <t>It is critical that when the operating system is at risk of failing to process audit logs as required, it takes action to mitigate the failure. Audit processing failures include: software/hardware errors; failures in the audit capturing mechanisms; and audit storage capacity being reached or exceeded. Responses to audit failure depend upon the nature of the failure mode.
 When availability is an overriding concern, other approved actions in response to an audit failure are as follows: 
@@ -1009,7 +1009,7 @@
 2) If audit records are sent to a centralized collection server and communication with this server is lost or the server fails, the operating system must queue audit records locally until communication is restored or until the audit records are retrieved manually. Upon restoration of the connection to the centralized collection server, action should be taken to synchronize the local audit data with the collection server.</t>
         </is>
       </c>
-      <c r="H7" s="3" t="inlineStr">
+      <c r="H7" s="2" t="inlineStr">
         <is>
           <t>It is critical for the appropriate personnel to be aware if a system
 is at risk of failing to process audit logs as required. Without this
@@ -1020,17 +1020,17 @@
 exceeded.</t>
         </is>
       </c>
-      <c r="I7" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J7" s="3" t="inlineStr">
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system shuts down by default upon audit failure (unless availability is an overriding concern). If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K7" s="3" t="inlineStr">
+      <c r="K7" s="2" t="inlineStr">
         <is>
           <t>To verify that the system will shutdown when "auditd" fails,
 run the following command:
@@ -1040,16 +1040,28 @@
 If the system is not configured to shutdown on auditd failures, then this is a finding.</t>
         </is>
       </c>
-      <c r="L7" s="3" t="n"/>
-      <c r="M7" s="3" t="inlineStr"/>
-      <c r="N7" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O7" s="3" t="n"/>
-      <c r="P7" s="3" t="n"/>
-      <c r="Q7" s="3" t="n"/>
+      <c r="L7" s="2" t="n"/>
+      <c r="M7" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to shutdown when auditing failures occur.
+If the auditd daemon is configured to use the augenrules program to read
+audit rules during daemon startup (the default), add the following line to
+the bottom of "/etc/audit/rules.d/immutable.rules":
+-f 2
+If the auditd daemon is configured to use the auditctl utility to read
+audit rules during daemon startup, add the following line to the
+bottom of the /etc/audit/audit.rules file:
+-f 2</t>
+        </is>
+      </c>
+      <c r="N7" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O7" s="2" t="n"/>
+      <c r="P7" s="2" t="n"/>
+      <c r="Q7" s="2" t="n"/>
     </row>
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="3" t="inlineStr">
@@ -1427,11 +1439,11 @@
       </c>
       <c r="K12" s="2" t="inlineStr">
         <is>
-          <t>For every temporary and emergency account, run the following command
+          <t>For every temporary account, run the following command
 to obtain its account aging and expiration information:
  $ sudo chage -l  USER  
 Verify each of these accounts has an expiration date set as documented.
-If any temporary or emergency accounts have no expiration date set or do not expire within a documented time frame, then this is a finding.</t>
+If any temporary accounts have no expiration date set or do not expire within a documented time frame, then this is a finding.</t>
         </is>
       </c>
       <c r="L12" s="2" t="n"/>
@@ -1455,7 +1467,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-6 (4),AU-7 a,AU-14 (1),MA-4 (1) (a),AU-3,AU-3 (1),CM-6 b,AU-7 (1),CM-5 (1)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-7 a,CM-6 b,AU-7 (1),AU-6 (4),AU-3,AU-3 (1),AU-14 (1),CM-5 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3258,7 +3270,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-14 (1),AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-14 (1),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3361,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3832,7 +3844,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4148,7 +4160,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4234,7 +4246,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4330,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 b,SI-6 d</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4410,7 +4422,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4494,7 +4506,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4581,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4656,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4731,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4806,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4881,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4956,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5031,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5106,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5181,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-7 a,AU-7 b,AU-8 b,CM-6 b,CM-5 (1),AU-12 (3)</t>
+          <t>AU-7 a,AU-12 c,AU-12 (3),AU-8 b,CM-6 b,AU-7 b,AU-12 a,CM-5 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5255,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5336,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5417,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5499,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5581,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5663,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5745,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5815,7 +5827,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -6853,7 +6865,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6939,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7013,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7087,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7651,7 +7663,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7738,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7813,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7888,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7968,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8050,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8132,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8214,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8296,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8378,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8458,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8538,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8606,7 +8618,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8777,7 +8789,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8856,7 +8868,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8935,7 +8947,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9022,7 +9034,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9109,7 +9121,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -9354,7 +9366,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 c,SC-13,SC-8</t>
+          <t>AC-17 (2),SC-13,MA-4 c,SC-8</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9436,7 +9448,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9514,7 +9526,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9592,7 +9604,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9670,7 +9682,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -9750,7 +9762,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -9819,7 +9831,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -9888,7 +9900,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -9957,7 +9969,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10026,7 +10038,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10106,7 +10118,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10223,7 +10235,14 @@
 Techniques used to address this include protocols using nonces (e.g., numbers generated for a specific one-time use) or challenges (e.g., TLS, WS_Security). Additional techniques include time-synchronous or challenge-response one-time authenticators.</t>
         </is>
       </c>
-      <c r="H124" s="2" t="inlineStr"/>
+      <c r="H124" s="2" t="inlineStr">
+        <is>
+          <t>A replay attack may enable an unauthorized user to gain access to Red Hat Enterprise Linux 9. Authentication sessions between the authenticator and Red Hat Enterprise Linux 9 validating the user credentials must not be vulnerable to a replay attack.
+An authentication process resists replay attacks if it is impractical to achieve a successful authentication by recording and replaying a previous authentication message.
+A privileged account is any information system account with authorizations of a privileged user.
+Techniques used to address this include protocols using nonces (e.g., numbers generated for a specific one-time use) or challenges (e.g., TLS, WS_Security). Additional techniques include time-synchronous or challenge-response one-time authenticators.</t>
+        </is>
+      </c>
       <c r="I124" s="2" t="inlineStr">
         <is>
           <t>Applicable - Inherently Met</t>
@@ -10873,7 +10892,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10954,7 +10973,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11040,7 +11059,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11133,7 +11152,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),AC-6 (10)</t>
+          <t>AC-6 (10),AC-3 (4)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11230,7 +11249,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),AC-6 (10)</t>
+          <t>AC-6 (10),AC-3 (4)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11406,7 +11425,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -11486,7 +11505,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11585,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11665,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -11958,7 +11977,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12268,7 +12287,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12429,7 +12448,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12505,7 +12524,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12590,7 +12609,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12826,7 +12845,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12922,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12995,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13068,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13153,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13228,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13303,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13378,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13434,7 +13453,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13505,7 +13524,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13576,7 +13595,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13648,7 +13667,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
@@ -13719,7 +13738,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
@@ -13790,7 +13809,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
@@ -13862,7 +13881,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -13937,7 +13956,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
@@ -14008,7 +14027,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
@@ -14079,7 +14098,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14151,7 +14170,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14245,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14327,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14409,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14491,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14573,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14655,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14737,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14819,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14901,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14983,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15061,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15140,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15222,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15304,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15386,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15468,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15550,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15632,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15707,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15780,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15857,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (1),IA-2 (2),IA-2 (3)</t>
+          <t>IA-2 (4),IA-2 (3),IA-2 (1),IA-2 (2)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15944,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2,IA-2 (5),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (5),IA-2 (2),IA-2 (3),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16033,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2,IA-2 (5),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (5),IA-2 (2),IA-2 (3),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16258,7 +16277,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16638,7 +16657,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16734,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16820,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16887,7 +16906,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16976,7 +16995,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17229,7 +17248,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17389,7 +17408,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17480,7 +17499,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17850,7 +17869,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>IA-8,AU-3 (1),IA-2</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18829,7 +18848,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-2,CM-6 b</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19742,7 +19761,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20310,7 +20329,7 @@
     <row r="250" ht="130" customHeight="1">
       <c r="A250" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B250" s="2" t="inlineStr">
@@ -20655,7 +20674,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B254" s="2" t="inlineStr">
@@ -21148,7 +21167,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
@@ -21697,7 +21716,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -22387,7 +22406,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -22535,7 +22554,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22615,7 +22634,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -23684,7 +23703,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -23823,136 +23842,144 @@
       <c r="Q292" s="3" t="n"/>
     </row>
     <row r="293" ht="130" customHeight="1">
-      <c r="A293" s="3" t="inlineStr">
+      <c r="A293" s="2" t="inlineStr">
         <is>
           <t>AU-5 a</t>
         </is>
       </c>
-      <c r="B293" s="3" t="inlineStr">
+      <c r="B293" s="2" t="inlineStr">
         <is>
           <t>CCI-000139,CCI-000366</t>
         </is>
       </c>
-      <c r="C293" s="3" t="inlineStr">
+      <c r="C293" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000046-GPOS-00022</t>
         </is>
       </c>
-      <c r="D293" s="3" t="inlineStr">
+      <c r="D293" s="2" t="inlineStr">
         <is>
           <t>CCE-90826-9</t>
         </is>
       </c>
-      <c r="E293" s="3" t="inlineStr">
+      <c r="E293" s="2" t="inlineStr">
         <is>
           <t>The operating system must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
-      <c r="F293" s="3" t="inlineStr">
+      <c r="F293" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
-      <c r="G293" s="3" t="inlineStr">
+      <c r="G293" s="2" t="inlineStr">
         <is>
           <t>It is critical for the appropriate personnel to be aware if a system is at risk of failing to process audit logs as required. Without this notification, the security personnel may be unaware of an impending failure of the audit capability, and system operation may be adversely affected.
 Audit processing failures include software/hardware errors, failures in the audit capturing mechanisms, and audit storage capacity being reached or exceeded.
 This requirement applies to each audit data storage repository (i.e., distinct information system component where audit records are stored), the centralized audit storage capacity of organizations (i.e., all audit data storage repositories combined), or both.</t>
         </is>
       </c>
-      <c r="H293" s="3" t="inlineStr">
+      <c r="H293" s="2" t="inlineStr">
         <is>
           <t>A number of system services utilize email messages sent to the root user to
 notify system administrators of active or impending issues.  These messages must
 be forwarded to at least one monitored email address.</t>
         </is>
       </c>
-      <c r="I293" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J293" s="3" t="inlineStr">
+      <c r="I293" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J293" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system alerts the ISSO and SA (at a minimum) in the event of an audit processing failure. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K293" s="3" t="inlineStr">
+      <c r="K293" s="2" t="inlineStr">
         <is>
           <t>Find the list of alias maps used by the Postfix mail server:
  $ sudo postconf alias_maps 
 Query the Postfix alias maps for an alias for the  root  user:
  $ sudo postmap -q root hash:/etc/aliases 
 The output should return an alias.
-If it is not, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L293" s="3" t="n"/>
-      <c r="M293" s="3" t="inlineStr"/>
-      <c r="N293" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O293" s="3" t="n"/>
-      <c r="P293" s="3" t="n"/>
-      <c r="Q293" s="3" t="n"/>
+If the alias is not set, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L293" s="2" t="n"/>
+      <c r="M293" s="2" t="inlineStr">
+        <is>
+          <t>Configure a valid email address as an alias for the root account.
+Append the following line to "/etc/aliases":
+root: system.administrator@mail.mil
+Then, run the following command:
+$ sudo newaliases</t>
+        </is>
+      </c>
+      <c r="N293" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O293" s="2" t="n"/>
+      <c r="P293" s="2" t="n"/>
+      <c r="Q293" s="2" t="n"/>
     </row>
     <row r="294" ht="130" customHeight="1">
-      <c r="A294" s="3" t="inlineStr">
-        <is>
-          <t>AU-5 (1),AU-5 a</t>
-        </is>
-      </c>
-      <c r="B294" s="3" t="inlineStr">
+      <c r="A294" s="2" t="inlineStr">
+        <is>
+          <t>AU-5 a,AU-5 (1)</t>
+        </is>
+      </c>
+      <c r="B294" s="2" t="inlineStr">
         <is>
           <t>CCI-000139,CCI-001855</t>
         </is>
       </c>
-      <c r="C294" s="3" t="inlineStr">
+      <c r="C294" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000046-GPOS-00022,SRG-OS-000343-GPOS-00134</t>
         </is>
       </c>
-      <c r="D294" s="3" t="inlineStr">
+      <c r="D294" s="2" t="inlineStr">
         <is>
           <t>CCE-83698-1</t>
         </is>
       </c>
-      <c r="E294" s="3" t="inlineStr">
+      <c r="E294" s="2" t="inlineStr">
         <is>
           <t>The operating system must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
-      <c r="F294" s="3" t="inlineStr">
+      <c r="F294" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
-      <c r="G294" s="3" t="inlineStr">
+      <c r="G294" s="2" t="inlineStr">
         <is>
           <t>It is critical for the appropriate personnel to be aware if a system is at risk of failing to process audit logs as required. Without this notification, the security personnel may be unaware of an impending failure of the audit capability, and system operation may be adversely affected.
 Audit processing failures include software/hardware errors, failures in the audit capturing mechanisms, and audit storage capacity being reached or exceeded.
 This requirement applies to each audit data storage repository (i.e., distinct information system component where audit records are stored), the centralized audit storage capacity of organizations (i.e., all audit data storage repositories combined), or both.</t>
         </is>
       </c>
-      <c r="H294" s="3" t="inlineStr">
+      <c r="H294" s="2" t="inlineStr">
         <is>
           <t>Email sent to the root account is typically aliased to the
 administrators of the system, who can take appropriate action.</t>
         </is>
       </c>
-      <c r="I294" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J294" s="3" t="inlineStr">
+      <c r="I294" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J294" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system alerts the ISSO and SA (at a minimum) in the event of an audit processing failure. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K294" s="3" t="inlineStr">
+      <c r="K294" s="2" t="inlineStr">
         <is>
           <t>Inspect "/etc/audit/auditd.conf" and locate the following line to
 determine if the system is configured to send email to an
@@ -23961,16 +23988,22 @@
 If auditd is not configured to send emails per identified actions, then this is a finding.</t>
         </is>
       </c>
-      <c r="L294" s="3" t="n"/>
-      <c r="M294" s="3" t="inlineStr"/>
-      <c r="N294" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O294" s="3" t="n"/>
-      <c r="P294" s="3" t="n"/>
-      <c r="Q294" s="3" t="n"/>
+      <c r="L294" s="2" t="n"/>
+      <c r="M294" s="2" t="inlineStr">
+        <is>
+          <t>Configure "auditd" service to notify the SA and ISSO in the event of an audit processing failure.
+Edit the following line in "/etc/audit/auditd.conf" to ensure that administrators are notified via email for those situations:
+action_mail_acct = root</t>
+        </is>
+      </c>
+      <c r="N294" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O294" s="2" t="n"/>
+      <c r="P294" s="2" t="n"/>
+      <c r="Q294" s="2" t="n"/>
     </row>
     <row r="295" ht="130" customHeight="1">
       <c r="A295" s="3" t="inlineStr">
@@ -27263,7 +27296,7 @@
     <row r="339" ht="130" customHeight="1">
       <c r="A339" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B339" s="3" t="inlineStr">
@@ -29890,7 +29923,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -30144,7 +30177,7 @@
     <row r="377" ht="130" customHeight="1">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
@@ -30538,7 +30571,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (9),AC-17 (1),CM-7 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1),AC-17 (9)</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30616,7 +30649,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -33115,7 +33148,7 @@
     <row r="412" ht="130" customHeight="1">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
@@ -33197,7 +33230,7 @@
     <row r="413" ht="130" customHeight="1">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
@@ -33890,7 +33923,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -34071,7 +34104,7 @@
     <row r="424" ht="130" customHeight="1">
       <c r="A424" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B424" s="3" t="inlineStr">
@@ -34158,7 +34191,7 @@
     <row r="425" ht="130" customHeight="1">
       <c r="A425" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B425" s="3" t="inlineStr">
@@ -34493,7 +34526,7 @@
     <row r="429" ht="130" customHeight="1">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
@@ -35249,7 +35282,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35339,7 +35372,7 @@
     <row r="440" ht="130" customHeight="1">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
@@ -36672,7 +36705,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>MA-4 e,MA-4 (7),SC-10,AC-12</t>
+          <t>MA-4 e,MA-4 (7),AC-12,SC-10</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36747,7 +36780,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36826,7 +36859,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -36979,7 +37012,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8,SC-8 (1)</t>
+          <t>AC-17 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -38606,7 +38639,7 @@
     <row r="483" ht="130" customHeight="1">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
@@ -39729,7 +39762,7 @@
     <row r="497" ht="130" customHeight="1">
       <c r="A497" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B497" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@a5157e3dff29d2114cf8ac6d2725bf0bd4321833 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -1467,7 +1467,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-7 a,AU-7 (1),AU-6 (4),AU-14 (1),AU-8 b,CM-5 (1),MA-4 (1) (a),AU-12 (3),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),AU-14 (1),AU-6 (4),MA-4 (1) (a),AU-7 (1),AU-3,AU-12 a,AU-7 b,AU-12 c,CM-5 (1),AU-8 b,AU-7 a,AU-12 (3)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1782,7 +1782,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2152,7 +2152,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2226,7 +2226,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3270,7 +3270,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),AU-14 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3361,7 +3361,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3449,7 +3449,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-7 a,AU-7 (1),AU-6 (4),AU-14 (1),AU-8 b,CM-5 (1),MA-4 (1) (a),AU-12 (3),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),AU-14 (1),AU-6 (4),MA-4 (1) (a),AU-7 (1),AU-3,AU-12 a,AU-7 b,AU-12 c,CM-5 (1),AU-8 b,AU-7 a,AU-12 (3)</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3916,7 +3916,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4077,7 +4077,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4232,7 +4232,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4402,7 +4402,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4578,7 +4578,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4653,7 +4653,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4728,7 +4728,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4803,7 +4803,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4878,7 +4878,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4953,7 +4953,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5028,7 +5028,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5103,7 +5103,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5178,7 +5178,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -5253,7 +5253,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5334,7 +5334,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5415,7 +5415,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5497,7 +5497,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5579,7 +5579,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5661,7 +5661,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5743,7 +5743,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5825,7 +5825,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5899,7 +5899,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5982,7 +5982,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -6060,7 +6060,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6151,7 +6151,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6233,7 +6233,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6863,7 +6863,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6937,7 +6937,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7011,7 +7011,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7085,7 +7085,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7509,7 +7509,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7585,7 +7585,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -7661,7 +7661,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7736,7 +7736,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7811,7 +7811,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7886,7 +7886,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7966,7 +7966,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8048,7 +8048,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8130,7 +8130,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8212,7 +8212,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8294,7 +8294,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8456,7 +8456,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8536,7 +8536,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8866,7 +8866,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -9364,7 +9364,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-13,MA-4 c,SC-8</t>
+          <t>MA-4 c,SC-8,AC-17 (2),SC-13</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9524,7 +9524,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9680,7 +9680,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10036,7 +10036,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10116,7 +10116,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10890,7 +10890,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10971,7 +10971,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11057,7 +11057,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11503,7 +11503,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11583,7 +11583,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11663,7 +11663,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12285,7 +12285,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12446,7 +12446,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12522,7 +12522,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12607,7 +12607,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12843,7 +12843,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12920,7 +12920,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12993,7 +12993,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13066,7 +13066,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13151,7 +13151,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13226,7 +13226,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13301,7 +13301,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13376,7 +13376,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13879,7 +13879,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14168,7 +14168,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14243,7 +14243,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14325,7 +14325,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14407,7 +14407,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14571,7 +14571,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14653,7 +14653,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14735,7 +14735,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14817,7 +14817,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14899,7 +14899,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -15059,7 +15059,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15138,7 +15138,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15220,7 +15220,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15302,7 +15302,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15384,7 +15384,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15466,7 +15466,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15548,7 +15548,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15630,7 +15630,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15705,7 +15705,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c,AC-2 (4)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 a,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15778,7 +15778,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15855,7 +15855,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (3),IA-2 (2),IA-2 (1)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (1),IA-2 (4)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15942,7 +15942,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (5),IA-2 (4),IA-2 (3),IA-2</t>
+          <t>IA-2 (3),IA-2,IA-2 (4),IA-2 (5),IA-2 (2)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16031,7 +16031,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (5),IA-2 (4),IA-2 (3),IA-2</t>
+          <t>IA-2 (3),IA-2,IA-2 (4),IA-2 (5),IA-2 (2)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16275,7 +16275,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16655,7 +16655,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16732,7 +16732,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16818,7 +16818,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16904,7 +16904,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16993,7 +16993,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17246,7 +17246,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17677,7 +17677,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -17867,7 +17867,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18838,7 +18838,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b,SI-16</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19022,7 +19022,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19751,7 +19751,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20575,7 +20575,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -20664,7 +20664,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B254" s="2" t="inlineStr">
@@ -21623,7 +21623,7 @@
     <row r="266" ht="130" customHeight="1">
       <c r="A266" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B266" s="2" t="inlineStr">
@@ -21706,7 +21706,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -22396,7 +22396,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -23392,7 +23392,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
@@ -23463,7 +23463,7 @@
     <row r="289" ht="130" customHeight="1">
       <c r="A289" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B289" s="3" t="inlineStr">
@@ -23535,7 +23535,7 @@
     <row r="290" ht="130" customHeight="1">
       <c r="A290" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B290" s="3" t="inlineStr">
@@ -23693,7 +23693,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -27436,7 +27436,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -29913,7 +29913,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -30167,7 +30167,7 @@
     <row r="377" ht="130" customHeight="1">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
@@ -30561,7 +30561,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b,AC-17 (9)</t>
+          <t>AC-17 (9),AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30639,7 +30639,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -33138,7 +33138,7 @@
     <row r="412" ht="130" customHeight="1">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
@@ -33220,7 +33220,7 @@
     <row r="413" ht="130" customHeight="1">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
@@ -33913,7 +33913,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -34516,7 +34516,7 @@
     <row r="429" ht="130" customHeight="1">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
@@ -35272,7 +35272,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35362,7 +35362,7 @@
     <row r="440" ht="130" customHeight="1">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
@@ -35757,7 +35757,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B445" s="3" t="inlineStr">
@@ -36404,7 +36404,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B454" s="3" t="inlineStr">
@@ -36695,7 +36695,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
+          <t>MA-4 (7),MA-4 e,AC-12,SC-10</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36770,7 +36770,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36849,7 +36849,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -37002,7 +37002,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -39752,7 +39752,7 @@
     <row r="497" ht="130" customHeight="1">
       <c r="A497" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B497" s="2" t="inlineStr">
@@ -40003,7 +40003,7 @@
     <row r="500" ht="130" customHeight="1">
       <c r="A500" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B500" s="2" t="inlineStr">
@@ -40105,7 +40105,7 @@
     <row r="501" ht="130" customHeight="1">
       <c r="A501" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B501" s="2" t="inlineStr">
@@ -40215,7 +40215,7 @@
     <row r="502" ht="130" customHeight="1">
       <c r="A502" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B502" s="2" t="inlineStr">
@@ -40326,7 +40326,7 @@
     <row r="503" ht="130" customHeight="1">
       <c r="A503" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B503" s="2" t="inlineStr">
@@ -42662,7 +42662,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ konstruktoid/scap-security-guide@130668613ebed741d9b1cfdd0f343ddf6a7843d5 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1467,7 +1467,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-14 (1),AU-7 b,AU-3,AU-7 a,MA-4 (1) (a),AU-6 (4),AU-12 c,AU-12 a,AU-3 (1),AU-8 b,CM-5 (1),AU-7 (1)</t>
+          <t>AU-3,AU-12 a,AU-7 (1),AU-7 a,AU-12 (3),MA-4 (1) (a),AU-6 (4),AU-12 c,AU-8 b,AU-7 b,AU-3 (1),CM-5 (1),AU-14 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-14 (1),AU-7 b,AU-3,AU-7 a,MA-4 (1) (a),AU-6 (4),AU-12 c,AU-12 a,AU-3 (1),AU-8 b,CM-5 (1),AU-7 (1)</t>
+          <t>AU-3,AU-12 a,AU-7 (1),AU-7 a,AU-12 (3),MA-4 (1) (a),AU-6 (4),AU-12 c,AU-8 b,AU-7 b,AU-3 (1),CM-5 (1),AU-14 (1)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1627,7 +1627,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1703,7 +1703,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -3345,7 +3345,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1),AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3918,7 +3918,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4079,7 +4079,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4320,7 +4320,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4404,7 +4404,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d,SI-6 b</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4496,7 +4496,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4580,7 +4580,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4655,7 +4655,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4730,7 +4730,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4805,7 +4805,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4880,7 +4880,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4955,7 +4955,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5030,7 +5030,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5105,7 +5105,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5180,7 +5180,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -5255,7 +5255,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5336,7 +5336,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5417,7 +5417,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5499,7 +5499,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5581,7 +5581,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5663,7 +5663,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5745,7 +5745,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5827,7 +5827,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -6865,7 +6865,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6939,7 +6939,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7013,7 +7013,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7087,7 +7087,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7511,7 +7511,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7587,7 +7587,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -7663,7 +7663,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7738,7 +7738,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7813,7 +7813,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7888,7 +7888,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7968,7 +7968,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8050,7 +8050,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8132,7 +8132,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8214,7 +8214,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8296,7 +8296,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8378,7 +8378,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8458,7 +8458,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8538,7 +8538,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8789,7 +8789,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8868,7 +8868,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8947,7 +8947,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9034,7 +9034,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9121,7 +9121,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -9366,7 +9366,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-13,AC-17 (2),SC-8,MA-4 c</t>
+          <t>SC-13,AC-17 (2),MA-4 c,SC-8</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9448,7 +9448,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9526,7 +9526,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9604,7 +9604,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9682,7 +9682,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -9762,7 +9762,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -9831,7 +9831,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -9900,7 +9900,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -9969,7 +9969,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10038,7 +10038,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10118,7 +10118,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10892,7 +10892,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10973,7 +10973,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11059,7 +11059,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11425,7 +11425,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -11505,7 +11505,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11585,7 +11585,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11665,7 +11665,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -11977,7 +11977,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12287,7 +12287,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12766,7 +12766,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12845,7 +12845,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12922,7 +12922,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12995,7 +12995,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13068,7 +13068,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13153,7 +13153,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13228,7 +13228,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13303,7 +13303,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13378,7 +13378,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13453,7 +13453,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13524,7 +13524,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13595,7 +13595,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13667,7 +13667,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
@@ -13738,7 +13738,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
@@ -13809,7 +13809,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
@@ -13881,7 +13881,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -13956,7 +13956,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
@@ -14027,7 +14027,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
@@ -14098,7 +14098,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14170,7 +14170,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14245,7 +14245,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14327,7 +14327,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14409,7 +14409,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14491,7 +14491,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14573,7 +14573,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14655,7 +14655,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14737,7 +14737,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14819,7 +14819,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14901,7 +14901,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14983,7 +14983,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15061,7 +15061,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15140,7 +15140,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15222,7 +15222,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15304,7 +15304,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15386,7 +15386,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15468,7 +15468,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15550,7 +15550,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15632,7 +15632,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15707,7 +15707,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (1),IA-2 (4),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15794,7 +15794,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (3),IA-2 (2),IA-2 (5),IA-2</t>
+          <t>IA-2 (5),IA-2,IA-2 (4),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15883,7 +15883,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (3),IA-2 (2),IA-2 (5),IA-2</t>
+          <t>IA-2 (5),IA-2,IA-2 (4),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -16507,7 +16507,7 @@
     <row r="204" ht="130" customHeight="1">
       <c r="A204" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B204" s="2" t="inlineStr">
@@ -16584,7 +16584,7 @@
     <row r="205" ht="130" customHeight="1">
       <c r="A205" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B205" s="2" t="inlineStr">
@@ -16670,7 +16670,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16756,7 +16756,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16845,7 +16845,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17098,7 +17098,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -17258,7 +17258,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17529,7 +17529,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17719,7 +17719,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -18690,7 +18690,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>CM-6 b,SC-2,SI-16</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18874,7 +18874,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19036,7 +19036,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19519,44 +19519,44 @@
       <c r="Q239" s="2" t="n"/>
     </row>
     <row r="240" ht="130" customHeight="1">
-      <c r="A240" s="3" t="inlineStr">
+      <c r="A240" s="2" t="inlineStr">
         <is>
           <t>IA-5 (1) (b)</t>
         </is>
       </c>
-      <c r="B240" s="3" t="inlineStr">
+      <c r="B240" s="2" t="inlineStr">
         <is>
           <t>CCI-000195</t>
         </is>
       </c>
-      <c r="C240" s="3" t="inlineStr">
+      <c r="C240" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000072-GPOS-00040</t>
         </is>
       </c>
-      <c r="D240" s="3" t="inlineStr">
+      <c r="D240" s="2" t="inlineStr">
         <is>
           <t>CCE-83564-5</t>
         </is>
       </c>
-      <c r="E240" s="3" t="inlineStr">
+      <c r="E240" s="2" t="inlineStr">
         <is>
           <t>The operating system must require the change of at least 50% of the total number of characters when passwords are changed.</t>
         </is>
       </c>
-      <c r="F240" s="3" t="inlineStr">
+      <c r="F240" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 Must Require The Change Of At Least 50% Of The Total Number Of Characters When Passwords Are Changed.</t>
         </is>
       </c>
-      <c r="G240" s="3" t="inlineStr">
+      <c r="G240" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system allows the user to consecutively reuse extensive portions of passwords, this increases the chances of password compromise by increasing the window of opportunity for attempts at guessing and brute-force attacks.
 The number of changed characters refers to the number of changes required with respect to the total number of positions in the current password. In other words, characters may be the same within the two passwords; however, the positions of the like characters must be different.
 If the password length is an odd number then number of changed characters must be rounded up.  For example, a password length of 15 characters must require the change of at least 8 characters.</t>
         </is>
       </c>
-      <c r="H240" s="3" t="inlineStr">
+      <c r="H240" s="2" t="inlineStr">
         <is>
           <t>Use of a complex password helps to increase the time and resources
 required to compromise the password. Password complexity, or strength,
@@ -19571,39 +19571,46 @@
 Note that passwords which are changed on compromised systems will still be compromised, however.</t>
         </is>
       </c>
-      <c r="I240" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J240" s="3" t="inlineStr">
+      <c r="I240" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J240" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system requires the change of at least eight of the total number of characters when passwords are changed. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K240" s="3" t="inlineStr">
+      <c r="K240" s="2" t="inlineStr">
         <is>
           <t>To check how many characters must differ during a password change, run the following command:
- $ grep difok /etc/security/pwquality.conf 
+ $ sudo grep difok /etc/security/pwquality.conf
+difok = 8
 The "difok" parameter will indicate how many characters must differ.
-If difok is not found or not equal to or greater than the required value, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L240" s="3" t="n"/>
-      <c r="M240" s="3" t="inlineStr"/>
-      <c r="N240" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O240" s="3" t="n"/>
-      <c r="P240" s="3" t="n"/>
-      <c r="Q240" s="3" t="n"/>
+If difok is not found or set to less than the required value, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L240" s="2" t="n"/>
+      <c r="M240" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to require the change of at least 8 of the total number of characters when passwords are changed by setting the "difok" option.
+Add the following line to "/etc/security/pwquality.conf" (or modify the line to have the required value):
+difok = 8</t>
+        </is>
+      </c>
+      <c r="N240" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O240" s="2" t="n"/>
+      <c r="P240" s="2" t="n"/>
+      <c r="Q240" s="2" t="n"/>
     </row>
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19684,46 +19691,46 @@
       <c r="Q241" s="2" t="n"/>
     </row>
     <row r="242" ht="130" customHeight="1">
-      <c r="A242" s="3" t="inlineStr">
+      <c r="A242" s="2" t="inlineStr">
         <is>
           <t>IA-5 (1) (b)</t>
         </is>
       </c>
-      <c r="B242" s="3" t="inlineStr">
+      <c r="B242" s="2" t="inlineStr">
         <is>
           <t>CCI-000195</t>
         </is>
       </c>
-      <c r="C242" s="3" t="inlineStr">
+      <c r="C242" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000072-GPOS-00040</t>
         </is>
       </c>
-      <c r="D242" s="3" t="inlineStr">
+      <c r="D242" s="2" t="inlineStr">
         <is>
           <t>CCE-83575-1</t>
         </is>
       </c>
-      <c r="E242" s="3" t="inlineStr">
+      <c r="E242" s="2" t="inlineStr">
         <is>
           <t>The operating system must require the change of at least 50% of the total number of characters when passwords are changed.</t>
         </is>
       </c>
-      <c r="F242" s="3" t="inlineStr">
+      <c r="F242" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 Must Require The Change Of At Least 50% Of The Total Number Of Characters When Passwords Are Changed.</t>
         </is>
       </c>
-      <c r="G242" s="3" t="inlineStr">
+      <c r="G242" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system allows the user to consecutively reuse extensive portions of passwords, this increases the chances of password compromise by increasing the window of opportunity for attempts at guessing and brute-force attacks.
 The number of changed characters refers to the number of changes required with respect to the total number of positions in the current password. In other words, characters may be the same within the two passwords; however, the positions of the like characters must be different.
 If the password length is an odd number then number of changed characters must be rounded up.  For example, a password length of 15 characters must require the change of at least 8 characters.</t>
         </is>
       </c>
-      <c r="H242" s="3" t="inlineStr">
-        <is>
-          <t>Use of a complex password helps to increase the time and resources required to comrpomise the password.
+      <c r="H242" s="2" t="inlineStr">
+        <is>
+          <t>Use of a complex password helps to increase the time and resources required to compromise the password.
 Password complexity, or strength, is a measure of the effectiveness of a password in resisting
 attempts at guessing and brute-force attacks.
 Password complexity is one factor of several that determines how long it takes to crack a password. The
@@ -19731,74 +19738,79 @@
 password is compromised.</t>
         </is>
       </c>
-      <c r="I242" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J242" s="3" t="inlineStr">
+      <c r="I242" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J242" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system requires the change of at least eight of the total number of characters when passwords are changed. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K242" s="3" t="inlineStr">
+      <c r="K242" s="2" t="inlineStr">
         <is>
           <t>To check the value for maximum consecutive repeating characters, run the following command:
- $ grep maxclassrepeat /etc/security/pwquality.conf 
-For DoD systems, the output should show "maxclassrepeat"=4 or less but greater than zero.
-If that is not the case, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L242" s="3" t="n"/>
-      <c r="M242" s="3" t="inlineStr"/>
-      <c r="N242" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O242" s="3" t="n"/>
-      <c r="P242" s="3" t="n"/>
-      <c r="Q242" s="3" t="n"/>
+ $ sudo grep maxclassrepeat /etc/security/pwquality.conf 
+If the value of "maxclassrepeat" is set to "0", more than "4" or is commented out, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L242" s="2" t="n"/>
+      <c r="M242" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to require the change of the number of repeating characters of the same character class when passwords are changed by setting the "maxclassrepeat" option.
+Add the following line to "/etc/security/pwquality.conf" conf (or modify the line to have the required value):
+maxclassrepeat = 4</t>
+        </is>
+      </c>
+      <c r="N242" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O242" s="2" t="n"/>
+      <c r="P242" s="2" t="n"/>
+      <c r="Q242" s="2" t="n"/>
     </row>
     <row r="243" ht="130" customHeight="1">
-      <c r="A243" s="3" t="inlineStr">
+      <c r="A243" s="2" t="inlineStr">
         <is>
           <t>IA-5 (1) (b)</t>
         </is>
       </c>
-      <c r="B243" s="3" t="inlineStr">
+      <c r="B243" s="2" t="inlineStr">
         <is>
           <t>CCI-000195</t>
         </is>
       </c>
-      <c r="C243" s="3" t="inlineStr">
+      <c r="C243" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000072-GPOS-00040</t>
         </is>
       </c>
-      <c r="D243" s="3" t="inlineStr">
+      <c r="D243" s="2" t="inlineStr">
         <is>
           <t>CCE-83567-8</t>
         </is>
       </c>
-      <c r="E243" s="3" t="inlineStr">
+      <c r="E243" s="2" t="inlineStr">
         <is>
           <t>The operating system must require the change of at least 50% of the total number of characters when passwords are changed.</t>
         </is>
       </c>
-      <c r="F243" s="3" t="inlineStr">
+      <c r="F243" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 Must Require The Change Of At Least 50% Of The Total Number Of Characters When Passwords Are Changed.</t>
         </is>
       </c>
-      <c r="G243" s="3" t="inlineStr">
+      <c r="G243" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system allows the user to consecutively reuse extensive portions of passwords, this increases the chances of password compromise by increasing the window of opportunity for attempts at guessing and brute-force attacks.
 The number of changed characters refers to the number of changes required with respect to the total number of positions in the current password. In other words, characters may be the same within the two passwords; however, the positions of the like characters must be different.
 If the password length is an odd number then number of changed characters must be rounded up.  For example, a password length of 15 characters must require the change of at least 8 characters.</t>
         </is>
       </c>
-      <c r="H243" s="3" t="inlineStr">
+      <c r="H243" s="2" t="inlineStr">
         <is>
           <t>Use of a complex password helps to increase the time and resources required to compromise the password.
 Password complexity, or strength, is a measure of the effectiveness of a password in resisting attempts at
@@ -19809,75 +19821,79 @@
 Passwords with excessive repeating characters may be more vulnerable to password-guessing attacks.</t>
         </is>
       </c>
-      <c r="I243" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J243" s="3" t="inlineStr">
+      <c r="I243" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J243" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system requires the change of at least eight of the total number of characters when passwords are changed. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K243" s="3" t="inlineStr">
+      <c r="K243" s="2" t="inlineStr">
         <is>
           <t>To check the maximum value for consecutive repeating characters, run the following command:
- $ grep maxrepeat /etc/security/pwquality.conf 
-Look for the value of the "maxrepeat" parameter. The DoD requirement is 3, which would appear as
-"maxrepeat=3".
-If maxrepeat is not found or not greater than or equal to the required value, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L243" s="3" t="n"/>
-      <c r="M243" s="3" t="inlineStr"/>
-      <c r="N243" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O243" s="3" t="n"/>
-      <c r="P243" s="3" t="n"/>
-      <c r="Q243" s="3" t="n"/>
+ $ sudo grep maxrepeat /etc/security/pwquality.conf 
+If the value of "maxrepeat" is set to more than "3" or is commented out, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L243" s="2" t="n"/>
+      <c r="M243" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to require the change of the number of repeating consecutive characters when passwords are changed by setting the "maxrepeat" option.
+Add the following line to "/etc/security/pwquality.conf" (or modify the line to have the required value):
+maxrepeat = 3</t>
+        </is>
+      </c>
+      <c r="N243" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O243" s="2" t="n"/>
+      <c r="P243" s="2" t="n"/>
+      <c r="Q243" s="2" t="n"/>
     </row>
     <row r="244" ht="130" customHeight="1">
-      <c r="A244" s="3" t="inlineStr">
+      <c r="A244" s="2" t="inlineStr">
         <is>
           <t>IA-5 (1) (b)</t>
         </is>
       </c>
-      <c r="B244" s="3" t="inlineStr">
+      <c r="B244" s="2" t="inlineStr">
         <is>
           <t>CCI-000195</t>
         </is>
       </c>
-      <c r="C244" s="3" t="inlineStr">
+      <c r="C244" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000072-GPOS-00040</t>
         </is>
       </c>
-      <c r="D244" s="3" t="inlineStr">
+      <c r="D244" s="2" t="inlineStr">
         <is>
           <t>CCE-83563-7</t>
         </is>
       </c>
-      <c r="E244" s="3" t="inlineStr">
+      <c r="E244" s="2" t="inlineStr">
         <is>
           <t>The operating system must require the change of at least 50% of the total number of characters when passwords are changed.</t>
         </is>
       </c>
-      <c r="F244" s="3" t="inlineStr">
+      <c r="F244" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 Must Require The Change Of At Least 50% Of The Total Number Of Characters When Passwords Are Changed.</t>
         </is>
       </c>
-      <c r="G244" s="3" t="inlineStr">
+      <c r="G244" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system allows the user to consecutively reuse extensive portions of passwords, this increases the chances of password compromise by increasing the window of opportunity for attempts at guessing and brute-force attacks.
 The number of changed characters refers to the number of changes required with respect to the total number of positions in the current password. In other words, characters may be the same within the two passwords; however, the positions of the like characters must be different.
 If the password length is an odd number then number of changed characters must be rounded up.  For example, a password length of 15 characters must require the change of at least 8 characters.</t>
         </is>
       </c>
-      <c r="H244" s="3" t="inlineStr">
+      <c r="H244" s="2" t="inlineStr">
         <is>
           <t>Use of a complex password helps to increase the time and resources required to compromise the password.
 Password complexity, or strength, is a measure of the effectiveness of a password in resisting attempts
@@ -19889,37 +19905,43 @@
 by ensuring a larger search space.</t>
         </is>
       </c>
-      <c r="I244" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J244" s="3" t="inlineStr">
+      <c r="I244" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J244" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system requires the change of at least eight of the total number of characters when passwords are changed. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K244" s="3" t="inlineStr">
+      <c r="K244" s="2" t="inlineStr">
         <is>
           <t>To check how many categories of characters must be used in password during a password change,
 run the following command:
- $ grep minclass /etc/security/pwquality.conf 
+ $ sudo grep minclass /etc/security/pwquality.conf 
 The "minclass" parameter will indicate how many character classes must be used. If
-the requirement was for the password to contain characters from three different categories,
-then this would appear as "minclass = 3".
-If minclass is not found or not set equal to or greater than the required value, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L244" s="3" t="n"/>
-      <c r="M244" s="3" t="inlineStr"/>
-      <c r="N244" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O244" s="3" t="n"/>
-      <c r="P244" s="3" t="n"/>
-      <c r="Q244" s="3" t="n"/>
+the requirement was for the password to contain characters from 4 different categories,
+then this would appear as "minclass = 4".
+If the value of "minclass" is set to less than "4" or is commented out, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L244" s="2" t="n"/>
+      <c r="M244" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to require the change of at least 4 character classes when passwords are changed by setting the "minclass" option.
+Add the following line to "/etc/security/pwquality.conf" (or modify the line to have the required value):
+minclass = 4</t>
+        </is>
+      </c>
+      <c r="N244" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O244" s="2" t="n"/>
+      <c r="P244" s="2" t="n"/>
+      <c r="Q244" s="2" t="n"/>
     </row>
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
@@ -20252,7 +20274,7 @@
     <row r="249" ht="130" customHeight="1">
       <c r="A249" s="3" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B249" s="3" t="inlineStr">
@@ -20340,7 +20362,7 @@
     <row r="250" ht="130" customHeight="1">
       <c r="A250" s="3" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B250" s="3" t="inlineStr">
@@ -20847,7 +20869,7 @@
     <row r="256" ht="130" customHeight="1">
       <c r="A256" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B256" s="2" t="inlineStr">
@@ -23240,7 +23262,7 @@
     <row r="286" ht="130" customHeight="1">
       <c r="A286" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B286" s="3" t="inlineStr">
@@ -23311,7 +23333,7 @@
     <row r="287" ht="130" customHeight="1">
       <c r="A287" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B287" s="3" t="inlineStr">
@@ -23383,7 +23405,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
@@ -30268,7 +30290,7 @@
     <row r="379" ht="130" customHeight="1">
       <c r="A379" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,CM-6 b,AC-17 (9),AC-17 (1)</t>
         </is>
       </c>
       <c r="B379" s="2" t="inlineStr">
@@ -30346,7 +30368,7 @@
     <row r="380" ht="130" customHeight="1">
       <c r="A380" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B380" s="2" t="inlineStr">
@@ -32845,7 +32867,7 @@
     <row r="409" ht="130" customHeight="1">
       <c r="A409" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B409" s="2" t="inlineStr">
@@ -32927,7 +32949,7 @@
     <row r="410" ht="130" customHeight="1">
       <c r="A410" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B410" s="2" t="inlineStr">
@@ -33801,7 +33823,7 @@
     <row r="421" ht="130" customHeight="1">
       <c r="A421" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B421" s="3" t="inlineStr">
@@ -33888,7 +33910,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B422" s="3" t="inlineStr">
@@ -34979,7 +35001,7 @@
     <row r="436" ht="130" customHeight="1">
       <c r="A436" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B436" s="2" t="inlineStr">
@@ -35069,7 +35091,7 @@
     <row r="437" ht="130" customHeight="1">
       <c r="A437" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B437" s="2" t="inlineStr">
@@ -35464,7 +35486,7 @@
     <row r="442" ht="130" customHeight="1">
       <c r="A442" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B442" s="3" t="inlineStr">
@@ -36402,7 +36424,7 @@
     <row r="455" ht="130" customHeight="1">
       <c r="A455" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (7),AC-12,SC-10,MA-4 e</t>
+          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
         </is>
       </c>
       <c r="B455" s="3" t="inlineStr">
@@ -36632,7 +36654,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36709,7 +36731,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B459" s="2" t="inlineStr">
@@ -38016,7 +38038,7 @@
     <row r="476" ht="130" customHeight="1">
       <c r="A476" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B476" s="2" t="inlineStr">
@@ -38335,7 +38357,7 @@
     <row r="480" ht="130" customHeight="1">
       <c r="A480" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B480" s="2" t="inlineStr">

</xml_diff>